<commit_message>
Benchmarking: update XLS summaries
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="44">
   <si>
     <t>N</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Int32?</t>
+  </si>
+  <si>
+    <t>NXP K66</t>
+  </si>
+  <si>
+    <t>180 MHz</t>
   </si>
 </sst>
 </file>
@@ -1232,11 +1238,11 @@
         <v>cfft</v>
       </c>
       <c r="I31" s="8" t="str">
-        <f>I6</f>
+        <f t="shared" ref="I31:J33" si="4">I6</f>
         <v>rfft</v>
       </c>
       <c r="J31" s="8" t="str">
-        <f>J6</f>
+        <f t="shared" si="4"/>
         <v>cfft</v>
       </c>
       <c r="K31" s="8" t="str">
@@ -1247,7 +1253,7 @@
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="str">
-        <f t="shared" ref="C32:K32" si="4">C7</f>
+        <f t="shared" ref="C32:K32" si="5">C7</f>
         <v>radix4</v>
       </c>
       <c r="D32" s="8" t="str">
@@ -1255,11 +1261,11 @@
         <v>radix4</v>
       </c>
       <c r="E32" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>radix2</v>
       </c>
       <c r="F32" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>radix4</v>
       </c>
       <c r="G32" s="8" t="str">
@@ -1267,26 +1273,26 @@
         <v>radix4</v>
       </c>
       <c r="H32" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>radix2</v>
+      </c>
+      <c r="I32" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>radix2</v>
-      </c>
-      <c r="I32" s="8" t="str">
-        <f>I7</f>
         <v>radix4</v>
       </c>
       <c r="J32" s="8" t="str">
-        <f>J7</f>
+        <f t="shared" si="4"/>
         <v>radix4</v>
       </c>
       <c r="K32" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>radix2</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="8" t="str">
-        <f t="shared" ref="C33:K33" si="5">C8</f>
+        <f t="shared" ref="C33:K33" si="6">C8</f>
         <v>int16</v>
       </c>
       <c r="D33" s="8" t="str">
@@ -1294,11 +1300,11 @@
         <v>int16</v>
       </c>
       <c r="E33" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>int16</v>
       </c>
       <c r="F33" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>int32</v>
       </c>
       <c r="G33" s="8" t="str">
@@ -1306,19 +1312,19 @@
         <v>int32</v>
       </c>
       <c r="H33" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>int32</v>
       </c>
       <c r="I33" s="8" t="str">
-        <f>I8</f>
+        <f t="shared" si="4"/>
         <v>float32</v>
       </c>
       <c r="J33" s="8" t="str">
-        <f>J8</f>
+        <f t="shared" si="4"/>
         <v>float32</v>
       </c>
       <c r="K33" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>float32</v>
       </c>
     </row>
@@ -1379,7 +1385,7 @@
         <v>4</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:K35" si="6">1/(1-H34)</f>
+        <f t="shared" ref="H35:K35" si="7">1/(1-H34)</f>
         <v>4</v>
       </c>
       <c r="I35">
@@ -1391,7 +1397,7 @@
         <v>4</v>
       </c>
       <c r="K35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
@@ -1430,31 +1436,31 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37">
-        <f t="shared" ref="B37:B44" si="7">B10</f>
+        <f t="shared" ref="B37:B44" si="8">B10</f>
         <v>32</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3">
-        <f>$B10/E$35/(E10/1000000)/1000/2</f>
+        <f t="shared" ref="E37:E44" si="9">$B10/E$35/(E10/1000000)/1000/2</f>
         <v>126.54223347042075</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3">
-        <f>$B10/H$35/(H10/1000000)/1000/2</f>
+        <f t="shared" ref="H37:H44" si="10">$B10/H$35/(H10/1000000)/1000/2</f>
         <v>73.909830007390994</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3">
-        <f>$B10/K$35/(K10/1000000)/1000/2</f>
+        <f t="shared" ref="K37:K44" si="11">$B10/K$35/(K10/1000000)/1000/2</f>
         <v>13.481176906743958</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="C38" s="3">
@@ -1466,7 +1472,7 @@
         <v>152.75921329005155</v>
       </c>
       <c r="E38" s="3">
-        <f>$B11/E$35/(E11/1000000)/1000/2</f>
+        <f t="shared" si="9"/>
         <v>119.1362620997766</v>
       </c>
       <c r="F38" s="3">
@@ -1478,7 +1484,7 @@
         <v>71.774627669118971</v>
       </c>
       <c r="H38" s="3">
-        <f>$B11/H$35/(H11/1000000)/1000/2</f>
+        <f t="shared" si="10"/>
         <v>65.584522052795535</v>
       </c>
       <c r="I38" s="3">
@@ -1490,37 +1496,37 @@
         <v>14.978468451600824</v>
       </c>
       <c r="K38" s="3">
-        <f>$B11/K$35/(K11/1000000)/1000/2</f>
+        <f t="shared" si="11"/>
         <v>11.233903922036708</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>128</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3">
-        <f>$B12/E$35/(E12/1000000)/1000/2</f>
+        <f t="shared" si="9"/>
         <v>110.83402604599611</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3">
-        <f>$B12/H$35/(H12/1000000)/1000/2</f>
+        <f t="shared" si="10"/>
         <v>58.372856621670913</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3">
-        <f>$B12/K$35/(K12/1000000)/1000/2</f>
+        <f t="shared" si="11"/>
         <v>9.6097827588485067</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>256</v>
       </c>
       <c r="C40" s="3">
@@ -1532,7 +1538,7 @@
         <v>133.94165166799212</v>
       </c>
       <c r="E40" s="3">
-        <f>$B13/E$35/(E13/1000000)/1000/2</f>
+        <f t="shared" si="9"/>
         <v>102.15482841181166</v>
       </c>
       <c r="F40" s="3">
@@ -1544,7 +1550,7 @@
         <v>55.473693334489028</v>
       </c>
       <c r="H40" s="3">
-        <f>$B13/H$35/(H13/1000000)/1000/2</f>
+        <f t="shared" si="10"/>
         <v>52.081637967514084</v>
       </c>
       <c r="I40" s="3">
@@ -1556,37 +1562,37 @@
         <v>10.794400404790014</v>
       </c>
       <c r="K40" s="3">
-        <f>$B13/K$35/(K13/1000000)/1000/2</f>
+        <f t="shared" si="11"/>
         <v>8.3787180561374122</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>512</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3">
-        <f>$B14/E$35/(E14/1000000)/1000/2</f>
+        <f t="shared" si="9"/>
         <v>95.926136874606556</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3">
-        <f>$B14/H$35/(H14/1000000)/1000/2</f>
+        <f t="shared" si="10"/>
         <v>46.993171304794771</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3">
-        <f>$B14/K$35/(K14/1000000)/1000/2</f>
+        <f t="shared" si="11"/>
         <v>7.4249901966926313</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
       <c r="C42" s="3">
@@ -1598,7 +1604,7 @@
         <v>116.60532740589586</v>
       </c>
       <c r="E42" s="3">
-        <f>$B15/E$35/(E15/1000000)/1000/2</f>
+        <f t="shared" si="9"/>
         <v>88.728684319977816</v>
       </c>
       <c r="F42" s="3">
@@ -1610,7 +1616,7 @@
         <v>45.141950273320404</v>
       </c>
       <c r="H42" s="3">
-        <f>$B15/H$35/(H15/1000000)/1000/2</f>
+        <f t="shared" si="10"/>
         <v>42.525482066206862</v>
       </c>
       <c r="I42" s="3">
@@ -1622,37 +1628,37 @@
         <v>8.419473980207659</v>
       </c>
       <c r="K42" s="3">
-        <f>$B15/K$35/(K15/1000000)/1000/2</f>
+        <f t="shared" si="11"/>
         <v>6.6625372815806871</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2048</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3">
-        <f>$B16/E$35/(E16/1000000)/1000/2</f>
+        <f t="shared" si="9"/>
         <v>82.89860140992387</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3">
-        <f>$B16/H$35/(H16/1000000)/1000/2</f>
+        <f t="shared" si="10"/>
         <v>38.914232120354427</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3">
-        <f>$B16/K$35/(K16/1000000)/1000/2</f>
+        <f t="shared" si="11"/>
         <v>6.0441363613826908</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4096</v>
       </c>
       <c r="C44" s="3">
@@ -1664,7 +1670,7 @@
         <v>102.69596978492015</v>
       </c>
       <c r="E44" s="3">
-        <f>$B17/E$35/(E17/1000000)/1000/2</f>
+        <f t="shared" si="9"/>
         <v>77.967010208805391</v>
       </c>
       <c r="F44" s="3"/>
@@ -1673,7 +1679,7 @@
         <v>38.14800382374132</v>
       </c>
       <c r="H44" s="3">
-        <f>$B17/H$35/(H17/1000000)/1000/2</f>
+        <f t="shared" si="10"/>
         <v>35.882736338979726</v>
       </c>
       <c r="I44" s="3"/>
@@ -1682,7 +1688,7 @@
         <v>6.9025859082090886</v>
       </c>
       <c r="K44" s="3">
-        <f>$B17/K$35/(K17/1000000)/1000/2</f>
+        <f t="shared" si="11"/>
         <v>5.5284901887655469</v>
       </c>
     </row>
@@ -1729,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W24"/>
+  <dimension ref="B2:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,15 +1750,15 @@
     <col min="11" max="12" width="11.140625" customWidth="1"/>
     <col min="13" max="14" width="10.85546875" customWidth="1"/>
     <col min="15" max="15" width="2" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="2.5703125" customWidth="1"/>
-    <col min="18" max="19" width="11.42578125" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" style="9" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" style="9" customWidth="1"/>
+    <col min="16" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="2.5703125" customWidth="1"/>
+    <col min="19" max="21" width="11.42578125" customWidth="1"/>
+    <col min="22" max="22" width="3.5703125" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" style="9" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -1786,23 +1792,29 @@
       <c r="P2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" t="s">
-        <v>22</v>
+      <c r="Q2" t="s">
+        <v>42</v>
       </c>
       <c r="S2" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="T2" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1836,20 +1848,26 @@
       <c r="P3" t="s">
         <v>10</v>
       </c>
-      <c r="R3" t="s">
-        <v>10</v>
+      <c r="Q3" t="s">
+        <v>43</v>
       </c>
       <c r="S3" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="T3" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="U3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>33</v>
       </c>
@@ -1883,20 +1901,26 @@
       <c r="P4" t="s">
         <v>34</v>
       </c>
-      <c r="R4" t="s">
+      <c r="Q4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" t="s">
         <v>23</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="U4" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="W4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>26</v>
       </c>
@@ -1930,20 +1954,26 @@
       <c r="P5" t="s">
         <v>32</v>
       </c>
-      <c r="R5" t="s">
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" t="s">
         <v>26</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>32</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="U5" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="V5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>27</v>
       </c>
@@ -1977,20 +2007,26 @@
       <c r="P6" t="s">
         <v>25</v>
       </c>
-      <c r="R6" t="s">
+      <c r="Q6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s">
         <v>27</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>25</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="U6" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="W6" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -2027,20 +2063,26 @@
       <c r="P7" t="s">
         <v>4</v>
       </c>
-      <c r="R7" t="s">
+      <c r="Q7" t="s">
         <v>4</v>
       </c>
       <c r="S7" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="V7" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>32</v>
       </c>
@@ -2071,21 +2113,27 @@
       <c r="P8">
         <v>410.03</v>
       </c>
-      <c r="R8">
+      <c r="Q8">
+        <v>125</v>
+      </c>
+      <c r="S8">
         <f>'ARM-Specific Functions'!K10</f>
         <v>296.70999999999998</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>338.42</v>
       </c>
-      <c r="U8" s="9">
+      <c r="U8">
+        <v>62</v>
+      </c>
+      <c r="W8" s="9">
         <v>654.98</v>
       </c>
-      <c r="V8" s="9">
+      <c r="X8" s="9">
         <v>846.76</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>64</v>
       </c>
@@ -2116,21 +2164,27 @@
       <c r="P9">
         <v>854.36</v>
       </c>
-      <c r="R9">
+      <c r="Q9">
+        <v>235</v>
+      </c>
+      <c r="S9">
         <f>'ARM-Specific Functions'!K11</f>
         <v>712.13</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>724.79</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U9">
+        <v>103</v>
+      </c>
+      <c r="W9" s="9">
         <v>1122.1300000000001</v>
       </c>
-      <c r="V9" s="9">
+      <c r="X9" s="9">
         <v>1662.88</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>128</v>
       </c>
@@ -2161,21 +2215,21 @@
       <c r="P10">
         <v>1982.42</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <f>'ARM-Specific Functions'!K12</f>
         <v>1664.97</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>1759.28</v>
       </c>
-      <c r="U10" s="9">
+      <c r="W10" s="9">
         <v>2080.58</v>
       </c>
-      <c r="V10" s="9">
+      <c r="X10" s="9">
         <v>3368.27</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>256</v>
       </c>
@@ -2206,21 +2260,21 @@
       <c r="P11">
         <v>4197.54</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f>'ARM-Specific Functions'!K13</f>
         <v>3819.2</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>3756.42</v>
       </c>
-      <c r="U11" s="9">
+      <c r="W11" s="9">
         <v>4087.76</v>
       </c>
-      <c r="V11" s="9">
+      <c r="X11" s="9">
         <v>6991.74</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>512</v>
       </c>
@@ -2251,21 +2305,21 @@
       <c r="P12">
         <v>9582.68</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f>'ARM-Specific Functions'!K14</f>
         <v>8619.5400000000009</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>8768.08</v>
       </c>
-      <c r="U12" s="9">
+      <c r="W12" s="9">
         <v>8299.17</v>
       </c>
-      <c r="V12" s="9">
+      <c r="X12" s="9">
         <v>14675.67</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1024</v>
       </c>
@@ -2305,21 +2359,21 @@
       <c r="P13">
         <v>20189.66</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <f>'ARM-Specific Functions'!K15</f>
         <v>19211.900000000001</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>18485.53</v>
       </c>
-      <c r="U13" s="9">
+      <c r="W13" s="9">
         <v>17191.080000000002</v>
       </c>
-      <c r="V13" s="9">
+      <c r="X13" s="9">
         <v>30967.26</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2048</v>
       </c>
@@ -2347,195 +2401,224 @@
       <c r="P14">
         <v>45220.12</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <f>'ARM-Specific Functions'!K16</f>
         <v>42355.1</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>42107.63</v>
       </c>
-      <c r="U14" s="9">
+      <c r="W14" s="9">
         <v>35957.269999999997</v>
       </c>
-      <c r="V14" s="9">
+      <c r="X14" s="9">
         <v>65450.37</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B8</f>
         <v>32</v>
       </c>
-      <c r="R17" s="2">
-        <f>R8/$B8</f>
-        <v>9.2721874999999994</v>
-      </c>
       <c r="S17" s="2">
         <f>S8/$B8</f>
+        <v>9.2721874999999994</v>
+      </c>
+      <c r="T17" s="2">
+        <f>T8/$B8</f>
         <v>10.575625</v>
       </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="10">
-        <f t="shared" ref="U17:V17" si="0">U8/$B8</f>
+      <c r="U17" s="2">
+        <f>U8/$B8</f>
+        <v>1.9375</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="W17" s="10">
+        <f t="shared" ref="W17:X17" si="0">W8/$B8</f>
         <v>20.468125000000001</v>
       </c>
-      <c r="V17" s="10">
+      <c r="X17" s="10">
         <f t="shared" si="0"/>
         <v>26.46125</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" ref="B18:B23" si="1">B9</f>
         <v>64</v>
       </c>
-      <c r="R18" s="2">
-        <f t="shared" ref="R18:V18" si="2">R9/$B9</f>
+      <c r="S18" s="2">
+        <f t="shared" ref="S18:X18" si="2">S9/$B9</f>
         <v>11.12703125</v>
       </c>
-      <c r="S18" s="2">
-        <f t="shared" ref="S18" si="3">S9/$B9</f>
+      <c r="T18" s="2">
+        <f t="shared" ref="T18:U18" si="3">T9/$B9</f>
         <v>11.324843749999999</v>
       </c>
-      <c r="T18" s="2"/>
-      <c r="U18" s="10">
+      <c r="U18" s="2">
+        <f t="shared" si="3"/>
+        <v>1.609375</v>
+      </c>
+      <c r="V18" s="2"/>
+      <c r="W18" s="10">
         <f t="shared" si="2"/>
         <v>17.533281250000002</v>
       </c>
-      <c r="V18" s="10">
+      <c r="X18" s="10">
         <f t="shared" si="2"/>
         <v>25.982500000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="R19" s="2">
-        <f t="shared" ref="R19:V19" si="4">R10/$B10</f>
+      <c r="S19" s="2">
+        <f t="shared" ref="S19:X19" si="4">S10/$B10</f>
         <v>13.007578125</v>
       </c>
-      <c r="S19" s="2">
-        <f t="shared" ref="S19" si="5">S10/$B10</f>
+      <c r="T19" s="2">
+        <f t="shared" ref="T19:U19" si="5">T10/$B10</f>
         <v>13.744375</v>
       </c>
-      <c r="T19" s="2"/>
-      <c r="U19" s="10">
+      <c r="U19" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="2"/>
+      <c r="W19" s="10">
         <f t="shared" si="4"/>
         <v>16.254531249999999</v>
       </c>
-      <c r="V19" s="10">
+      <c r="X19" s="10">
         <f t="shared" si="4"/>
         <v>26.314609375</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="R20" s="2">
-        <f t="shared" ref="R20:V20" si="6">R11/$B11</f>
+      <c r="S20" s="2">
+        <f t="shared" ref="S20:X20" si="6">S11/$B11</f>
         <v>14.918749999999999</v>
       </c>
-      <c r="S20" s="2">
-        <f t="shared" ref="S20" si="7">S11/$B11</f>
+      <c r="T20" s="2">
+        <f t="shared" ref="T20:U20" si="7">T11/$B11</f>
         <v>14.673515625</v>
       </c>
-      <c r="T20" s="2"/>
-      <c r="U20" s="10">
+      <c r="U20" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="2"/>
+      <c r="W20" s="10">
         <f t="shared" si="6"/>
         <v>15.967812500000001</v>
       </c>
-      <c r="V20" s="10">
+      <c r="X20" s="10">
         <f t="shared" si="6"/>
         <v>27.311484374999999</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
-      <c r="R21" s="2">
-        <f t="shared" ref="R21:V21" si="8">R12/$B12</f>
+      <c r="S21" s="2">
+        <f t="shared" ref="S21:X21" si="8">S12/$B12</f>
         <v>16.835039062500002</v>
       </c>
-      <c r="S21" s="2">
-        <f t="shared" ref="S21" si="9">S12/$B12</f>
+      <c r="T21" s="2">
+        <f t="shared" ref="T21:U21" si="9">T12/$B12</f>
         <v>17.12515625</v>
       </c>
-      <c r="T21" s="2"/>
-      <c r="U21" s="10">
+      <c r="U21" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V21" s="2"/>
+      <c r="W21" s="10">
         <f t="shared" si="8"/>
         <v>16.20931640625</v>
       </c>
-      <c r="V21" s="10">
+      <c r="X21" s="10">
         <f t="shared" si="8"/>
         <v>28.66341796875</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-      <c r="R22" s="2">
-        <f t="shared" ref="R22:V22" si="10">R13/$B13</f>
+      <c r="S22" s="2">
+        <f t="shared" ref="S22:X22" si="10">S13/$B13</f>
         <v>18.761621093750001</v>
       </c>
-      <c r="S22" s="2">
-        <f t="shared" ref="S22" si="11">S13/$B13</f>
+      <c r="T22" s="2">
+        <f t="shared" ref="T22:U22" si="11">T13/$B13</f>
         <v>18.052275390624999</v>
       </c>
-      <c r="T22" s="2"/>
-      <c r="U22" s="10">
+      <c r="U22" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="2"/>
+      <c r="W22" s="10">
         <f t="shared" si="10"/>
         <v>16.788164062500002</v>
       </c>
-      <c r="V22" s="10">
+      <c r="X22" s="10">
         <f t="shared" si="10"/>
         <v>30.241464843749998</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
-      <c r="R23" s="2">
-        <f t="shared" ref="R23:V23" si="12">R14/$B14</f>
+      <c r="S23" s="2">
+        <f t="shared" ref="S23:X23" si="12">S14/$B14</f>
         <v>20.681201171874999</v>
       </c>
-      <c r="S23" s="2">
-        <f t="shared" ref="S23" si="13">S14/$B14</f>
+      <c r="T23" s="2">
+        <f t="shared" ref="T23:U23" si="13">T14/$B14</f>
         <v>20.560366210937499</v>
       </c>
-      <c r="T23" s="2"/>
-      <c r="U23" s="10">
+      <c r="U23" s="2">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="2"/>
+      <c r="W23" s="10">
         <f t="shared" si="12"/>
         <v>17.557260742187498</v>
       </c>
-      <c r="V23" s="10">
+      <c r="X23" s="10">
         <f t="shared" si="12"/>
         <v>31.958188476562501</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="R24" s="2"/>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Benchmark: got kiss_fft and arm_fft working.
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="44">
   <si>
     <t>N</t>
   </si>
@@ -111,9 +111,6 @@
     <t>usec/N</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>KissFFT</t>
   </si>
   <si>
@@ -147,18 +144,22 @@
     <t>NXP K66</t>
   </si>
   <si>
-    <t>180 MHz</t>
+    <t>vs RealTime @ 44100</t>
+  </si>
+  <si>
+    <t>180 MHz (120?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +182,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +200,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,10 +225,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -220,9 +241,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1735,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y24"/>
+  <dimension ref="B2:AJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,18 +1772,20 @@
     <col min="5" max="5" width="2.42578125" customWidth="1"/>
     <col min="6" max="9" width="10.85546875" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="11" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="2" customWidth="1"/>
-    <col min="16" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="2.5703125" customWidth="1"/>
-    <col min="19" max="21" width="11.42578125" customWidth="1"/>
-    <col min="22" max="22" width="3.5703125" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" style="9" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="15" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="2" customWidth="1"/>
+    <col min="17" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="19" width="2.5703125" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="3.5703125" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" style="9" customWidth="1"/>
+    <col min="26" max="26" width="10.42578125" style="9" customWidth="1"/>
+    <col min="32" max="32" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -1772,49 +1799,84 @@
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
       <c r="N2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="R2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="U2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W2" s="9" t="s">
+      <c r="V2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB2" t="str">
+        <f>K2</f>
+        <v>Teensy 3.0</v>
+      </c>
+      <c r="AC2" t="str">
+        <f>Q2</f>
+        <v>Teensy 3.0</v>
+      </c>
+      <c r="AD2" t="str">
+        <f>T2</f>
+        <v>Teensy 3.0</v>
+      </c>
+      <c r="AE2" t="str">
+        <f>U2</f>
+        <v>Teensy 3.0</v>
+      </c>
+      <c r="AG2" t="str">
+        <f>L2</f>
+        <v>NXP K66</v>
+      </c>
+      <c r="AH2" t="str">
+        <f>R2</f>
+        <v>NXP K66</v>
+      </c>
+      <c r="AI2" t="str">
+        <f>V2</f>
+        <v>NXP K66</v>
+      </c>
+      <c r="AJ2" t="str">
+        <f>W2</f>
+        <v>NXP K66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1828,152 +1890,266 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" t="s">
-        <v>37</v>
-      </c>
       <c r="N3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="Z3" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB3" t="str">
+        <f t="shared" ref="AB3:AB6" si="0">K3</f>
+        <v>96 MHz</v>
+      </c>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC6" si="1">Q3</f>
+        <v>96 MHz</v>
+      </c>
+      <c r="AD3" t="str">
+        <f>T3</f>
+        <v>96 MHz</v>
+      </c>
+      <c r="AE3" t="str">
+        <f>U3</f>
+        <v>96 MHz</v>
+      </c>
+      <c r="AG3" t="str">
+        <f t="shared" ref="AG3:AG6" si="2">L3</f>
+        <v>180 MHz (120?)</v>
+      </c>
+      <c r="AH3" t="str">
+        <f t="shared" ref="AG3:AH6" si="3">R3</f>
+        <v>180 MHz (120?)</v>
+      </c>
+      <c r="AI3" t="str">
+        <f>V3</f>
+        <v>180 MHz (120?)</v>
+      </c>
+      <c r="AJ3" t="str">
+        <f>W3</f>
+        <v>180 MHz (120?)</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" t="s">
-        <v>41</v>
+      <c r="L4" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="W4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="Y4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB4" t="str">
+        <f t="shared" si="0"/>
+        <v>Int32</v>
+      </c>
+      <c r="AC4" t="str">
+        <f t="shared" si="1"/>
+        <v>Int32</v>
+      </c>
+      <c r="AD4" t="str">
+        <f>T4</f>
+        <v>Float</v>
+      </c>
+      <c r="AE4" t="str">
+        <f>U4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AG4" t="str">
+        <f t="shared" si="2"/>
+        <v>Int32</v>
+      </c>
+      <c r="AH4" t="str">
+        <f t="shared" si="3"/>
+        <v>Int32</v>
+      </c>
+      <c r="AI4" t="str">
+        <f>V4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AJ4" t="str">
+        <f>W4</f>
+        <v>All Float</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L5" t="s">
-        <v>40</v>
+      <c r="L5" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="T5" t="s">
-        <v>32</v>
-      </c>
-      <c r="U5" t="s">
-        <v>32</v>
-      </c>
-      <c r="W5" s="9" t="s">
+      <c r="U5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB5" t="str">
+        <f t="shared" si="0"/>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AC5" t="str">
+        <f t="shared" si="1"/>
+        <v>KissFFT</v>
+      </c>
+      <c r="AD5" t="str">
+        <f>T5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AE5" t="str">
+        <f>U5</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="AG5" t="str">
+        <f t="shared" si="2"/>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AH5" t="str">
+        <f t="shared" si="3"/>
+        <v>KissFFT</v>
+      </c>
+      <c r="AI5" t="str">
+        <f>V5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AJ5" t="str">
+        <f>W5</f>
+        <v>KissFFT</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>27</v>
       </c>
@@ -1992,11 +2168,11 @@
       <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L6" t="s">
-        <v>25</v>
+      <c r="L6" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="M6" t="s">
         <v>25</v>
@@ -2004,29 +2180,67 @@
       <c r="N6" t="s">
         <v>25</v>
       </c>
-      <c r="P6" t="s">
+      <c r="O6" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="S6" t="s">
+      <c r="R6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Z6" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB6" t="str">
+        <f t="shared" si="0"/>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AC6" t="str">
+        <f t="shared" si="1"/>
+        <v>Generic C</v>
+      </c>
+      <c r="AD6" t="str">
+        <f>T6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AE6" t="str">
+        <f>U6</f>
+        <v>Generic C</v>
+      </c>
+      <c r="AG6" t="str">
+        <f t="shared" si="2"/>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AH6" t="str">
+        <f t="shared" si="3"/>
+        <v>Generic C</v>
+      </c>
+      <c r="AI6" t="str">
+        <f>V6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AJ6" t="str">
+        <f>W6</f>
+        <v>Generic C</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -2048,10 +2262,10 @@
       <c r="I7" t="s">
         <v>4</v>
       </c>
-      <c r="K7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="K7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="M7" t="s">
@@ -2060,29 +2274,59 @@
       <c r="N7" t="s">
         <v>4</v>
       </c>
-      <c r="P7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>4</v>
-      </c>
-      <c r="S7" t="s">
-        <v>4</v>
-      </c>
-      <c r="T7" t="s">
-        <v>4</v>
-      </c>
-      <c r="U7" t="s">
-        <v>4</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X7" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>32</v>
       </c>
@@ -2097,43 +2341,82 @@
         <f>'ARM-Specific Functions'!H10</f>
         <v>54.12</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="13">
         <f>'ARM-Specific Functions'!H10</f>
         <v>54.12</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="12">
+        <v>52</v>
+      </c>
+      <c r="M8">
         <v>74.41</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>144.16</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>262.33999999999997</v>
       </c>
-      <c r="P8">
+      <c r="Q8" s="13">
         <v>410.03</v>
       </c>
-      <c r="Q8">
-        <v>125</v>
-      </c>
-      <c r="S8">
+      <c r="R8" s="12">
+        <v>127</v>
+      </c>
+      <c r="T8" s="13">
         <f>'ARM-Specific Functions'!K10</f>
         <v>296.70999999999998</v>
       </c>
-      <c r="T8">
+      <c r="U8" s="13">
         <v>338.42</v>
       </c>
-      <c r="U8">
+      <c r="V8" s="12">
+        <v>37</v>
+      </c>
+      <c r="W8" s="12">
         <v>62</v>
       </c>
-      <c r="W8" s="9">
+      <c r="Y8" s="9">
         <v>654.98</v>
       </c>
-      <c r="X8" s="9">
+      <c r="Z8" s="9">
         <v>846.76</v>
       </c>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB8" s="11">
+        <f>K8*0.000001/($B8/44100)</f>
+        <v>7.4584124999999987E-2</v>
+      </c>
+      <c r="AC8" s="11">
+        <f>Q8*0.000001/($B8/44100)</f>
+        <v>0.56507259374999996</v>
+      </c>
+      <c r="AD8" s="11">
+        <f>T8*0.000001/($B8/44100)</f>
+        <v>0.40890346874999989</v>
+      </c>
+      <c r="AE8" s="11">
+        <f>U8*0.000001/($B8/44100)</f>
+        <v>0.46638506249999995</v>
+      </c>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11">
+        <f>L8*0.000001/($B8/44100)</f>
+        <v>7.166249999999999E-2</v>
+      </c>
+      <c r="AH8" s="11">
+        <f>R8*0.000001/($B8/44100)</f>
+        <v>0.17502187499999999</v>
+      </c>
+      <c r="AI8" s="11">
+        <f>V8*0.000001/($B8/44100)</f>
+        <v>5.0990624999999998E-2</v>
+      </c>
+      <c r="AJ8" s="11">
+        <f>W8*0.000001/($B8/44100)</f>
+        <v>8.5443749999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>64</v>
       </c>
@@ -2148,43 +2431,82 @@
         <f>'ARM-Specific Functions'!H11</f>
         <v>121.98</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="13">
         <f>'ARM-Specific Functions'!H11</f>
         <v>121.98</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="12">
+        <v>114</v>
+      </c>
+      <c r="M9">
         <v>162.52000000000001</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>323.75</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>592.08000000000004</v>
       </c>
-      <c r="P9">
+      <c r="Q9" s="13">
         <v>854.36</v>
       </c>
-      <c r="Q9">
-        <v>235</v>
-      </c>
-      <c r="S9">
+      <c r="R9" s="12">
+        <v>238</v>
+      </c>
+      <c r="T9" s="13">
         <f>'ARM-Specific Functions'!K11</f>
         <v>712.13</v>
       </c>
-      <c r="T9">
+      <c r="U9" s="13">
         <v>724.79</v>
       </c>
-      <c r="U9">
-        <v>103</v>
-      </c>
-      <c r="W9" s="9">
+      <c r="V9" s="12">
+        <v>79</v>
+      </c>
+      <c r="W9" s="12">
+        <v>102</v>
+      </c>
+      <c r="Y9" s="9">
         <v>1122.1300000000001</v>
       </c>
-      <c r="X9" s="9">
+      <c r="Z9" s="9">
         <v>1662.88</v>
       </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB9" s="11">
+        <f t="shared" ref="AB9:AB14" si="4">K9*0.000001/($B9/44100)</f>
+        <v>8.4051843749999994E-2</v>
+      </c>
+      <c r="AC9" s="11">
+        <f t="shared" ref="AC9:AC14" si="5">Q9*0.000001/($B9/44100)</f>
+        <v>0.58870743749999999</v>
+      </c>
+      <c r="AD9" s="11">
+        <f>T9*0.000001/($B9/44100)</f>
+        <v>0.49070207812499994</v>
+      </c>
+      <c r="AE9" s="11">
+        <f>U9*0.000001/($B9/44100)</f>
+        <v>0.49942560937499991</v>
+      </c>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11">
+        <f t="shared" ref="AG9:AG14" si="6">L9*0.000001/($B9/44100)</f>
+        <v>7.8553124999999988E-2</v>
+      </c>
+      <c r="AH9" s="11">
+        <f t="shared" ref="AG9:AH14" si="7">R9*0.000001/($B9/44100)</f>
+        <v>0.16399687499999999</v>
+      </c>
+      <c r="AI9" s="11">
+        <f>V9*0.000001/(B9/44100)</f>
+        <v>5.4435937499999996E-2</v>
+      </c>
+      <c r="AJ9" s="11">
+        <f>W9*0.000001/(C9/44100)</f>
+        <v>6.698734177215189E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>128</v>
       </c>
@@ -2199,37 +2521,82 @@
         <f>'ARM-Specific Functions'!H12</f>
         <v>274.10000000000002</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="13">
         <f>'ARM-Specific Functions'!H12</f>
         <v>274.10000000000002</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="12">
+        <v>257</v>
+      </c>
+      <c r="M10">
         <v>355.3</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>721.27</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>1318.83</v>
       </c>
-      <c r="P10">
+      <c r="Q10" s="13">
         <v>1982.42</v>
       </c>
-      <c r="S10">
+      <c r="R10" s="12">
+        <v>632</v>
+      </c>
+      <c r="T10" s="13">
         <f>'ARM-Specific Functions'!K12</f>
         <v>1664.97</v>
       </c>
-      <c r="T10">
+      <c r="U10" s="13">
         <v>1759.28</v>
       </c>
-      <c r="W10" s="9">
+      <c r="V10" s="12">
+        <v>173</v>
+      </c>
+      <c r="W10" s="12">
+        <v>282</v>
+      </c>
+      <c r="Y10" s="9">
         <v>2080.58</v>
       </c>
-      <c r="X10" s="9">
+      <c r="Z10" s="9">
         <v>3368.27</v>
       </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB10" s="11">
+        <f t="shared" si="4"/>
+        <v>9.4436015624999994E-2</v>
+      </c>
+      <c r="AC10" s="11">
+        <f t="shared" si="5"/>
+        <v>0.68300564062499991</v>
+      </c>
+      <c r="AD10" s="11">
+        <f>T10*0.000001/($B10/44100)</f>
+        <v>0.57363419531250004</v>
+      </c>
+      <c r="AE10" s="11">
+        <f>U10*0.000001/($B10/44100)</f>
+        <v>0.60612693749999991</v>
+      </c>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11">
+        <f t="shared" si="6"/>
+        <v>8.8544531250000003E-2</v>
+      </c>
+      <c r="AH10" s="11">
+        <f t="shared" si="7"/>
+        <v>0.21774374999999999</v>
+      </c>
+      <c r="AI10" s="11">
+        <f>V10*0.000001/(B10/44100)</f>
+        <v>5.9603906249999998E-2</v>
+      </c>
+      <c r="AJ10" s="11">
+        <f>W10*0.000001/(C10/44100)</f>
+        <v>8.6147132169576035E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>256</v>
       </c>
@@ -2244,37 +2611,82 @@
         <f>'ARM-Specific Functions'!H13</f>
         <v>614.41999999999996</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="13">
         <f>'ARM-Specific Functions'!H13</f>
         <v>614.41999999999996</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="12">
+        <v>570</v>
+      </c>
+      <c r="M11">
         <v>776.61</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>1595.22</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>2917.8</v>
       </c>
-      <c r="P11">
+      <c r="Q11" s="13">
         <v>4197.54</v>
       </c>
-      <c r="S11">
+      <c r="R11" s="12">
+        <v>1199</v>
+      </c>
+      <c r="T11" s="13">
         <f>'ARM-Specific Functions'!K13</f>
         <v>3819.2</v>
       </c>
-      <c r="T11">
+      <c r="U11" s="13">
         <v>3756.42</v>
       </c>
-      <c r="W11" s="9">
+      <c r="V11" s="12">
+        <v>374</v>
+      </c>
+      <c r="W11" s="12">
+        <v>477</v>
+      </c>
+      <c r="Y11" s="9">
         <v>4087.76</v>
       </c>
-      <c r="X11" s="9">
+      <c r="Z11" s="9">
         <v>6991.74</v>
       </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB11" s="11">
+        <f t="shared" si="4"/>
+        <v>0.10584344531249999</v>
+      </c>
+      <c r="AC11" s="11">
+        <f t="shared" si="5"/>
+        <v>0.72309185156249989</v>
+      </c>
+      <c r="AD11" s="11">
+        <f>T11*0.000001/($B11/44100)</f>
+        <v>0.65791687499999996</v>
+      </c>
+      <c r="AE11" s="11">
+        <f>U11*0.000001/($B11/44100)</f>
+        <v>0.64710203906249997</v>
+      </c>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11">
+        <f t="shared" si="6"/>
+        <v>9.8191406249999988E-2</v>
+      </c>
+      <c r="AH11" s="11">
+        <f t="shared" si="7"/>
+        <v>0.20654648437500001</v>
+      </c>
+      <c r="AI11" s="11">
+        <f>V11*0.000001/(B11/44100)</f>
+        <v>6.4427343749999991E-2</v>
+      </c>
+      <c r="AJ11" s="11">
+        <f>W11*0.000001/(C11/44100)</f>
+        <v>6.7153072625698321E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>512</v>
       </c>
@@ -2289,37 +2701,82 @@
         <f>'ARM-Specific Functions'!H14</f>
         <v>1361.9</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="13">
         <f>'ARM-Specific Functions'!H14</f>
         <v>1361.9</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="12">
+        <v>1251</v>
+      </c>
+      <c r="M12">
         <v>1688.09</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>3498.65</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>6393.07</v>
       </c>
-      <c r="P12">
+      <c r="Q12" s="13">
         <v>9582.68</v>
       </c>
-      <c r="S12">
+      <c r="R12" s="12">
+        <v>3031</v>
+      </c>
+      <c r="T12" s="13">
         <f>'ARM-Specific Functions'!K14</f>
         <v>8619.5400000000009</v>
       </c>
-      <c r="T12">
+      <c r="U12" s="13">
         <v>8768.08</v>
       </c>
-      <c r="W12" s="9">
+      <c r="V12" s="12">
+        <v>799</v>
+      </c>
+      <c r="W12" s="12">
+        <v>1272</v>
+      </c>
+      <c r="Y12" s="9">
         <v>8299.17</v>
       </c>
-      <c r="X12" s="9">
+      <c r="Z12" s="9">
         <v>14675.67</v>
       </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB12" s="11">
+        <f t="shared" si="4"/>
+        <v>0.11730427734375</v>
+      </c>
+      <c r="AC12" s="11">
+        <f t="shared" si="5"/>
+        <v>0.82538317968749997</v>
+      </c>
+      <c r="AD12" s="11">
+        <f>T12*0.000001/($B12/44100)</f>
+        <v>0.74242522265624999</v>
+      </c>
+      <c r="AE12" s="11">
+        <f>U12*0.000001/($B12/44100)</f>
+        <v>0.75521939062499988</v>
+      </c>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11">
+        <f t="shared" si="6"/>
+        <v>0.10775214843749999</v>
+      </c>
+      <c r="AH12" s="11">
+        <f t="shared" si="7"/>
+        <v>0.26106855468749995</v>
+      </c>
+      <c r="AI12" s="11">
+        <f>V12*0.000001/(B12/44100)</f>
+        <v>6.8820117187500002E-2</v>
+      </c>
+      <c r="AJ12" s="11">
+        <f>W12*0.000001/(C12/44100)</f>
+        <v>8.4078059893881701E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1024</v>
       </c>
@@ -2343,37 +2800,82 @@
       <c r="I13">
         <v>13542.68</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="13">
         <f>'ARM-Specific Functions'!H15</f>
         <v>3009.96</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="12">
+        <v>2740</v>
+      </c>
+      <c r="M13">
         <v>3654.13</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>7621.21</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>13917.22</v>
       </c>
-      <c r="P13">
+      <c r="Q13" s="13">
         <v>20189.66</v>
       </c>
-      <c r="S13">
+      <c r="R13" s="12">
+        <v>5801</v>
+      </c>
+      <c r="T13" s="13">
         <f>'ARM-Specific Functions'!K15</f>
         <v>19211.900000000001</v>
       </c>
-      <c r="T13">
+      <c r="U13" s="13">
         <v>18485.53</v>
       </c>
-      <c r="W13" s="9">
+      <c r="V13" s="12">
+        <v>1725</v>
+      </c>
+      <c r="W13" s="12">
+        <v>2196</v>
+      </c>
+      <c r="Y13" s="9">
         <v>17191.080000000002</v>
       </c>
-      <c r="X13" s="9">
+      <c r="Z13" s="9">
         <v>30967.26</v>
       </c>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB13" s="11">
+        <f t="shared" si="4"/>
+        <v>0.12962816015625001</v>
+      </c>
+      <c r="AC13" s="11">
+        <f t="shared" si="5"/>
+        <v>0.86949609960937491</v>
+      </c>
+      <c r="AD13" s="11">
+        <f>T13*0.000001/($B13/44100)</f>
+        <v>0.82738749023437497</v>
+      </c>
+      <c r="AE13" s="11">
+        <f>U13*0.000001/($B13/44100)</f>
+        <v>0.79610534472656236</v>
+      </c>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11">
+        <f t="shared" si="6"/>
+        <v>0.11800195312499999</v>
+      </c>
+      <c r="AH13" s="11">
+        <f t="shared" si="7"/>
+        <v>0.24982822265624999</v>
+      </c>
+      <c r="AI13" s="11">
+        <f>V13*0.000001/(B13/44100)</f>
+        <v>7.4289550781249991E-2</v>
+      </c>
+      <c r="AJ13" s="11">
+        <f>W13*0.000001/(C13/44100)</f>
+        <v>6.7131290725079715E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2048</v>
       </c>
@@ -2385,240 +2887,293 @@
         <f>'ARM-Specific Functions'!H16</f>
         <v>6578.57</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="13">
         <f>'ARM-Specific Functions'!H16</f>
         <v>6578.57</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="12">
+        <v>5906</v>
+      </c>
+      <c r="M14">
         <v>7866.48</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>16942.04</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>30090.02</v>
       </c>
-      <c r="P14">
+      <c r="Q14" s="13">
         <v>45220.12</v>
       </c>
-      <c r="S14">
+      <c r="R14" s="12">
+        <v>14133</v>
+      </c>
+      <c r="T14" s="13">
         <f>'ARM-Specific Functions'!K16</f>
         <v>42355.1</v>
       </c>
-      <c r="T14">
+      <c r="U14" s="13">
         <v>42107.63</v>
       </c>
-      <c r="W14" s="9">
+      <c r="V14" s="12">
+        <v>3628</v>
+      </c>
+      <c r="W14" s="12">
+        <v>5658</v>
+      </c>
+      <c r="Y14" s="9">
         <v>35957.269999999997</v>
       </c>
-      <c r="X14" s="9">
+      <c r="Z14" s="9">
         <v>65450.37</v>
       </c>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AB14" s="11">
+        <f t="shared" si="4"/>
+        <v>0.14165768408203125</v>
+      </c>
+      <c r="AC14" s="11">
+        <f t="shared" si="5"/>
+        <v>0.97373402929687503</v>
+      </c>
+      <c r="AD14" s="11">
+        <f>T14*0.000001/($B14/44100)</f>
+        <v>0.91204097167968745</v>
+      </c>
+      <c r="AE14" s="11">
+        <f>U14*0.000001/($B14/44100)</f>
+        <v>0.90671214990234361</v>
+      </c>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11">
+        <f t="shared" si="6"/>
+        <v>0.12717509765624999</v>
+      </c>
+      <c r="AH14" s="11">
+        <f t="shared" si="7"/>
+        <v>0.30432875976562501</v>
+      </c>
+      <c r="AI14" s="11">
+        <f>V14*0.000001/(B14/44100)</f>
+        <v>7.8122460937499999E-2</v>
+      </c>
+      <c r="AJ14" s="11">
+        <f>W14*0.000001/(C14/44100)</f>
+        <v>8.0799518151879288E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B8</f>
         <v>32</v>
       </c>
-      <c r="S17" s="2">
-        <f>S8/$B8</f>
-        <v>9.2721874999999994</v>
-      </c>
       <c r="T17" s="2">
         <f>T8/$B8</f>
-        <v>10.575625</v>
+        <v>9.2721874999999994</v>
       </c>
       <c r="U17" s="2">
         <f>U8/$B8</f>
+        <v>10.575625</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2">
+        <f>W8/$B8</f>
         <v>1.9375</v>
       </c>
-      <c r="V17" s="2"/>
-      <c r="W17" s="10">
-        <f t="shared" ref="W17:X17" si="0">W8/$B8</f>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="10">
+        <f t="shared" ref="Y17:Z17" si="8">Y8/$B8</f>
         <v>20.468125000000001</v>
       </c>
-      <c r="X17" s="10">
-        <f t="shared" si="0"/>
+      <c r="Z17" s="10">
+        <f t="shared" si="8"/>
         <v>26.46125</v>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f t="shared" ref="B18:B23" si="1">B9</f>
+        <f t="shared" ref="B18:B23" si="9">B9</f>
         <v>64</v>
       </c>
-      <c r="S18" s="2">
-        <f t="shared" ref="S18:X18" si="2">S9/$B9</f>
+      <c r="T18" s="2">
+        <f t="shared" ref="T18:Z18" si="10">T9/$B9</f>
         <v>11.12703125</v>
       </c>
-      <c r="T18" s="2">
-        <f t="shared" ref="T18:U18" si="3">T9/$B9</f>
+      <c r="U18" s="2">
+        <f t="shared" ref="U18:W18" si="11">U9/$B9</f>
         <v>11.324843749999999</v>
       </c>
-      <c r="U18" s="2">
-        <f t="shared" si="3"/>
-        <v>1.609375</v>
-      </c>
       <c r="V18" s="2"/>
-      <c r="W18" s="10">
-        <f t="shared" si="2"/>
+      <c r="W18" s="2">
+        <f t="shared" si="11"/>
+        <v>1.59375</v>
+      </c>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="10">
+        <f t="shared" si="10"/>
         <v>17.533281250000002</v>
       </c>
-      <c r="X18" s="10">
-        <f t="shared" si="2"/>
+      <c r="Z18" s="10">
+        <f t="shared" si="10"/>
         <v>25.982500000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
-      <c r="S19" s="2">
-        <f t="shared" ref="S19:X19" si="4">S10/$B10</f>
+      <c r="T19" s="2">
+        <f t="shared" ref="T19:Z19" si="12">T10/$B10</f>
         <v>13.007578125</v>
       </c>
-      <c r="T19" s="2">
-        <f t="shared" ref="T19:U19" si="5">T10/$B10</f>
+      <c r="U19" s="2">
+        <f t="shared" ref="U19:W19" si="13">U10/$B10</f>
         <v>13.744375</v>
       </c>
-      <c r="U19" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="V19" s="2"/>
-      <c r="W19" s="10">
-        <f t="shared" si="4"/>
+      <c r="W19" s="2">
+        <f t="shared" si="13"/>
+        <v>2.203125</v>
+      </c>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="10">
+        <f t="shared" si="12"/>
         <v>16.254531249999999</v>
       </c>
-      <c r="X19" s="10">
-        <f t="shared" si="4"/>
+      <c r="Z19" s="10">
+        <f t="shared" si="12"/>
         <v>26.314609375</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>256</v>
       </c>
-      <c r="S20" s="2">
-        <f t="shared" ref="S20:X20" si="6">S11/$B11</f>
+      <c r="T20" s="2">
+        <f t="shared" ref="T20:Z20" si="14">T11/$B11</f>
         <v>14.918749999999999</v>
       </c>
-      <c r="T20" s="2">
-        <f t="shared" ref="T20:U20" si="7">T11/$B11</f>
+      <c r="U20" s="2">
+        <f t="shared" ref="U20:W20" si="15">U11/$B11</f>
         <v>14.673515625</v>
       </c>
-      <c r="U20" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="V20" s="2"/>
-      <c r="W20" s="10">
-        <f t="shared" si="6"/>
+      <c r="W20" s="2">
+        <f t="shared" si="15"/>
+        <v>1.86328125</v>
+      </c>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="10">
+        <f t="shared" si="14"/>
         <v>15.967812500000001</v>
       </c>
-      <c r="X20" s="10">
-        <f t="shared" si="6"/>
+      <c r="Z20" s="10">
+        <f t="shared" si="14"/>
         <v>27.311484374999999</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>512</v>
       </c>
-      <c r="S21" s="2">
-        <f t="shared" ref="S21:X21" si="8">S12/$B12</f>
+      <c r="T21" s="2">
+        <f t="shared" ref="T21:Z21" si="16">T12/$B12</f>
         <v>16.835039062500002</v>
       </c>
-      <c r="T21" s="2">
-        <f t="shared" ref="T21:U21" si="9">T12/$B12</f>
+      <c r="U21" s="2">
+        <f t="shared" ref="U21:W21" si="17">U12/$B12</f>
         <v>17.12515625</v>
       </c>
-      <c r="U21" s="2">
+      <c r="V21" s="2"/>
+      <c r="W21" s="2">
+        <f t="shared" si="17"/>
+        <v>2.484375</v>
+      </c>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="10">
+        <f t="shared" si="16"/>
+        <v>16.20931640625</v>
+      </c>
+      <c r="Z21" s="10">
+        <f t="shared" si="16"/>
+        <v>28.66341796875</v>
+      </c>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B22">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="V21" s="2"/>
-      <c r="W21" s="10">
-        <f t="shared" si="8"/>
-        <v>16.20931640625</v>
-      </c>
-      <c r="X21" s="10">
-        <f t="shared" si="8"/>
-        <v>28.66341796875</v>
-      </c>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-      <c r="S22" s="2">
-        <f t="shared" ref="S22:X22" si="10">S13/$B13</f>
+      <c r="T22" s="2">
+        <f t="shared" ref="T22:Z22" si="18">T13/$B13</f>
         <v>18.761621093750001</v>
       </c>
-      <c r="T22" s="2">
-        <f t="shared" ref="T22:U22" si="11">T13/$B13</f>
+      <c r="U22" s="2">
+        <f t="shared" ref="U22:W22" si="19">U13/$B13</f>
         <v>18.052275390624999</v>
       </c>
-      <c r="U22" s="2">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
       <c r="V22" s="2"/>
-      <c r="W22" s="10">
-        <f t="shared" si="10"/>
+      <c r="W22" s="2">
+        <f t="shared" si="19"/>
+        <v>2.14453125</v>
+      </c>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="10">
+        <f t="shared" si="18"/>
         <v>16.788164062500002</v>
       </c>
-      <c r="X22" s="10">
-        <f t="shared" si="10"/>
+      <c r="Z22" s="10">
+        <f t="shared" si="18"/>
         <v>30.241464843749998</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>2048</v>
       </c>
-      <c r="S23" s="2">
-        <f t="shared" ref="S23:X23" si="12">S14/$B14</f>
+      <c r="T23" s="2">
+        <f t="shared" ref="T23:Z23" si="20">T14/$B14</f>
         <v>20.681201171874999</v>
       </c>
-      <c r="T23" s="2">
-        <f t="shared" ref="T23:U23" si="13">T14/$B14</f>
+      <c r="U23" s="2">
+        <f t="shared" ref="U23:W23" si="21">U14/$B14</f>
         <v>20.560366210937499</v>
       </c>
-      <c r="U23" s="2">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
       <c r="V23" s="2"/>
-      <c r="W23" s="10">
-        <f t="shared" si="12"/>
+      <c r="W23" s="2">
+        <f t="shared" si="21"/>
+        <v>2.7626953125</v>
+      </c>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="10">
+        <f t="shared" si="20"/>
         <v>17.557260742187498</v>
       </c>
-      <c r="X23" s="10">
-        <f t="shared" si="12"/>
+      <c r="Z23" s="10">
+        <f t="shared" si="20"/>
         <v>31.958188476562501</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="S24" s="2"/>
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Benchmark: Running K66 at 180MHz!
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="46">
   <si>
     <t>N</t>
   </si>
@@ -147,7 +147,13 @@
     <t>vs RealTime @ 44100</t>
   </si>
   <si>
-    <t>180 MHz (120?)</t>
+    <t>120 MHz</t>
+  </si>
+  <si>
+    <t>180 MHz</t>
+  </si>
+  <si>
+    <t>cfft, radix 4</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +221,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -229,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -244,6 +256,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1760,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AJ24"/>
+  <dimension ref="B2:AO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC21" sqref="AC21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,20 +1785,20 @@
     <col min="5" max="5" width="2.42578125" customWidth="1"/>
     <col min="6" max="9" width="10.85546875" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="11" max="13" width="11.140625" customWidth="1"/>
-    <col min="14" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="2" customWidth="1"/>
-    <col min="17" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="2.5703125" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.42578125" customWidth="1"/>
-    <col min="24" max="24" width="3.5703125" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" style="9" customWidth="1"/>
-    <col min="26" max="26" width="10.42578125" style="9" customWidth="1"/>
-    <col min="32" max="32" width="2.140625" customWidth="1"/>
+    <col min="11" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="16" width="10.85546875" customWidth="1"/>
+    <col min="17" max="17" width="2" customWidth="1"/>
+    <col min="18" max="19" width="10.85546875" customWidth="1"/>
+    <col min="20" max="20" width="2.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="11.42578125" customWidth="1"/>
+    <col min="27" max="27" width="3.5703125" customWidth="1"/>
+    <col min="28" max="28" width="11.28515625" style="9" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" style="9" customWidth="1"/>
+    <col min="35" max="35" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:41" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -1810,73 +1823,90 @@
       <c r="L2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>35</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>22</v>
       </c>
       <c r="U2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="12" t="s">
-        <v>41</v>
+      <c r="V2" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="X2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AE2" t="str">
         <f>K2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AC2" t="str">
-        <f>Q2</f>
+      <c r="AF2" t="str">
+        <f>R2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AD2" t="str">
-        <f>T2</f>
-        <v>Teensy 3.0</v>
-      </c>
-      <c r="AE2" t="str">
+      <c r="AG2" t="str">
         <f>U2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AG2" t="str">
-        <f>L2</f>
+      <c r="AH2" t="str">
+        <f>V2</f>
+        <v>Teensy 3.0</v>
+      </c>
+      <c r="AJ2" t="str">
+        <f>M2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AH2" t="str">
-        <f>R2</f>
+      <c r="AK2" t="str">
+        <f>S2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AI2" t="str">
-        <f>V2</f>
-        <v>NXP K66</v>
-      </c>
-      <c r="AJ2" t="str">
+      <c r="AL2" t="str">
         <f>W2</f>
         <v>NXP K66</v>
       </c>
-    </row>
-    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AM2" t="str">
+        <f>X2</f>
+        <v>NXP K66</v>
+      </c>
+      <c r="AN2" t="str">
+        <f>Y2</f>
+        <v>NXP K66</v>
+      </c>
+      <c r="AO2" t="str">
+        <f t="shared" ref="AO2:AO6" si="0">Z2</f>
+        <v>NXP K66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1898,76 +1928,93 @@
       <c r="K3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>10</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>36</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="U3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="Z3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="AB3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="AC3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB6" si="0">K3</f>
+      <c r="AE3" t="str">
+        <f>K3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AC3" t="str">
-        <f t="shared" ref="AC3:AC6" si="1">Q3</f>
+      <c r="AF3" t="str">
+        <f>R3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AD3" t="str">
-        <f>T3</f>
-        <v>96 MHz</v>
-      </c>
-      <c r="AE3" t="str">
+      <c r="AG3" t="str">
         <f>U3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG6" si="2">L3</f>
-        <v>180 MHz (120?)</v>
-      </c>
       <c r="AH3" t="str">
-        <f t="shared" ref="AG3:AH6" si="3">R3</f>
-        <v>180 MHz (120?)</v>
-      </c>
-      <c r="AI3" t="str">
         <f>V3</f>
-        <v>180 MHz (120?)</v>
+        <v>96 MHz</v>
       </c>
       <c r="AJ3" t="str">
+        <f>M3</f>
+        <v>120 MHz</v>
+      </c>
+      <c r="AK3" t="str">
+        <f>S3</f>
+        <v>120 MHz</v>
+      </c>
+      <c r="AL3" t="str">
         <f>W3</f>
-        <v>180 MHz (120?)</v>
-      </c>
-    </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
+        <v>180 MHz</v>
+      </c>
+      <c r="AM3" t="str">
+        <f>X3</f>
+        <v>180 MHz</v>
+      </c>
+      <c r="AN3" t="str">
+        <f>Y3</f>
+        <v>120 MHz</v>
+      </c>
+      <c r="AO3" t="str">
+        <f t="shared" si="0"/>
+        <v>120 MHz</v>
+      </c>
+    </row>
+    <row r="4" spans="2:41" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>32</v>
       </c>
@@ -1992,8 +2039,8 @@
       <c r="L4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="M4" t="s">
-        <v>40</v>
+      <c r="M4" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="N4" t="s">
         <v>40</v>
@@ -2001,64 +2048,81 @@
       <c r="O4" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="S4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="U4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="U4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="12" t="s">
+      <c r="V4" s="13" t="s">
         <v>29</v>
       </c>
       <c r="W4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y4" s="9" t="s">
+      <c r="X4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="Y4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AB4" t="str">
-        <f t="shared" si="0"/>
+      <c r="AE4" t="str">
+        <f>K4</f>
         <v>Int32</v>
       </c>
-      <c r="AC4" t="str">
-        <f t="shared" si="1"/>
+      <c r="AF4" t="str">
+        <f>R4</f>
         <v>Int32</v>
       </c>
-      <c r="AD4" t="str">
-        <f>T4</f>
+      <c r="AG4" t="str">
+        <f>U4</f>
         <v>Float</v>
       </c>
-      <c r="AE4" t="str">
-        <f>U4</f>
-        <v>All Float</v>
-      </c>
-      <c r="AG4" t="str">
-        <f t="shared" si="2"/>
-        <v>Int32</v>
-      </c>
       <c r="AH4" t="str">
-        <f t="shared" si="3"/>
-        <v>Int32</v>
-      </c>
-      <c r="AI4" t="str">
         <f>V4</f>
         <v>All Float</v>
       </c>
       <c r="AJ4" t="str">
+        <f>M4</f>
+        <v>Int32</v>
+      </c>
+      <c r="AK4" t="str">
+        <f>S4</f>
+        <v>Int32</v>
+      </c>
+      <c r="AL4" t="str">
         <f>W4</f>
         <v>All Float</v>
       </c>
-    </row>
-    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AM4" t="str">
+        <f>X4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AN4" t="str">
+        <f>Y4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AO4" t="str">
+        <f t="shared" si="0"/>
+        <v>All Float</v>
+      </c>
+    </row>
+    <row r="5" spans="2:41" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>26</v>
       </c>
@@ -2083,8 +2147,8 @@
       <c r="L5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M5" t="s">
-        <v>39</v>
+      <c r="M5" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="N5" t="s">
         <v>39</v>
@@ -2092,64 +2156,81 @@
       <c r="O5" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="13" t="s">
+      <c r="P5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="S5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="U5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="V5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="V5" s="12" t="s">
+      <c r="W5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="W5" s="12" t="s">
+      <c r="Y5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AB5" t="str">
+      <c r="AE5" t="str">
+        <f>K5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AF5" t="str">
+        <f>R5</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="AG5" t="str">
+        <f>U5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AH5" t="str">
+        <f>V5</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="AJ5" t="str">
+        <f>M5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AK5" t="str">
+        <f>S5</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="AL5" t="str">
+        <f>W5</f>
+        <v>cfft, radix 4</v>
+      </c>
+      <c r="AM5" t="str">
+        <f>X5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AN5" t="str">
+        <f>Y5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AO5" t="str">
         <f t="shared" si="0"/>
-        <v>cfft, radix 2</v>
-      </c>
-      <c r="AC5" t="str">
-        <f t="shared" si="1"/>
         <v>KissFFT</v>
       </c>
-      <c r="AD5" t="str">
-        <f>T5</f>
-        <v>cfft, radix 2</v>
-      </c>
-      <c r="AE5" t="str">
-        <f>U5</f>
-        <v>KissFFT</v>
-      </c>
-      <c r="AG5" t="str">
-        <f t="shared" si="2"/>
-        <v>cfft, radix 2</v>
-      </c>
-      <c r="AH5" t="str">
-        <f t="shared" si="3"/>
-        <v>KissFFT</v>
-      </c>
-      <c r="AI5" t="str">
-        <f>V5</f>
-        <v>cfft, radix 2</v>
-      </c>
-      <c r="AJ5" t="str">
-        <f>W5</f>
-        <v>KissFFT</v>
-      </c>
-    </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:41" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>27</v>
       </c>
@@ -2174,8 +2255,8 @@
       <c r="L6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M6" t="s">
-        <v>25</v>
+      <c r="M6" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="N6" t="s">
         <v>25</v>
@@ -2183,64 +2264,81 @@
       <c r="O6" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="P6" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="S6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="V6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="12" t="s">
+      <c r="W6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="12" t="s">
+      <c r="X6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="AB6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AB6" t="str">
+      <c r="AE6" t="str">
+        <f>K6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AF6" t="str">
+        <f>R6</f>
+        <v>Generic C</v>
+      </c>
+      <c r="AG6" t="str">
+        <f>U6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AH6" t="str">
+        <f>V6</f>
+        <v>Generic C</v>
+      </c>
+      <c r="AJ6" t="str">
+        <f>M6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AK6" t="str">
+        <f>S6</f>
+        <v>Generic C</v>
+      </c>
+      <c r="AL6" t="str">
+        <f>W6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AM6" t="str">
+        <f>X6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AN6" t="str">
+        <f>Y6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AO6" t="str">
         <f t="shared" si="0"/>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AC6" t="str">
-        <f t="shared" si="1"/>
         <v>Generic C</v>
       </c>
-      <c r="AD6" t="str">
-        <f>T6</f>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AE6" t="str">
-        <f>U6</f>
-        <v>Generic C</v>
-      </c>
-      <c r="AG6" t="str">
-        <f t="shared" si="2"/>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AH6" t="str">
-        <f t="shared" si="3"/>
-        <v>Generic C</v>
-      </c>
-      <c r="AI6" t="str">
-        <f>V6</f>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AJ6" t="str">
-        <f>W6</f>
-        <v>Generic C</v>
-      </c>
-    </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2366,7 @@
       <c r="L7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="N7" t="s">
@@ -2277,56 +2375,71 @@
       <c r="O7" t="s">
         <v>4</v>
       </c>
-      <c r="Q7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="T7" s="13" t="s">
+      <c r="P7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="U7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="12" t="s">
+      <c r="V7" s="13" t="s">
         <v>4</v>
       </c>
       <c r="W7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="Y7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>42</v>
+      <c r="X7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="AE7" t="s">
         <v>42</v>
       </c>
+      <c r="AF7" t="s">
+        <v>42</v>
+      </c>
       <c r="AG7" t="s">
         <v>42</v>
       </c>
       <c r="AH7" t="s">
         <v>42</v>
       </c>
-      <c r="AI7" t="s">
-        <v>42</v>
-      </c>
       <c r="AJ7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>32</v>
       </c>
@@ -2346,77 +2459,94 @@
         <v>54.12</v>
       </c>
       <c r="L8" s="12">
-        <v>52</v>
-      </c>
-      <c r="M8">
+        <v>35</v>
+      </c>
+      <c r="M8" s="12">
+        <v>51</v>
+      </c>
+      <c r="N8">
         <v>74.41</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>144.16</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>262.33999999999997</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="R8" s="13">
         <v>410.03</v>
       </c>
-      <c r="R8" s="12">
+      <c r="S8" s="12">
         <v>127</v>
       </c>
-      <c r="T8" s="13">
+      <c r="U8" s="13">
         <f>'ARM-Specific Functions'!K10</f>
         <v>296.70999999999998</v>
       </c>
-      <c r="U8" s="13">
+      <c r="V8" s="13">
         <v>338.42</v>
       </c>
-      <c r="V8" s="12">
+      <c r="W8" s="12">
+        <v>26</v>
+      </c>
+      <c r="X8" s="12">
+        <v>25</v>
+      </c>
+      <c r="Y8" s="12">
         <v>37</v>
       </c>
-      <c r="W8" s="12">
+      <c r="Z8" s="12">
         <v>62</v>
       </c>
-      <c r="Y8" s="9">
+      <c r="AB8" s="9">
         <v>654.98</v>
       </c>
-      <c r="Z8" s="9">
+      <c r="AC8" s="9">
         <v>846.76</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AE8" s="11">
         <f>K8*0.000001/($B8/44100)</f>
         <v>7.4584124999999987E-2</v>
       </c>
-      <c r="AC8" s="11">
-        <f>Q8*0.000001/($B8/44100)</f>
+      <c r="AF8" s="11">
+        <f>R8*0.000001/($B8/44100)</f>
         <v>0.56507259374999996</v>
       </c>
-      <c r="AD8" s="11">
-        <f>T8*0.000001/($B8/44100)</f>
+      <c r="AG8" s="11">
+        <f>U8*0.000001/($B8/44100)</f>
         <v>0.40890346874999989</v>
       </c>
-      <c r="AE8" s="11">
-        <f>U8*0.000001/($B8/44100)</f>
+      <c r="AH8" s="11">
+        <f>V8*0.000001/($B8/44100)</f>
         <v>0.46638506249999995</v>
       </c>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11">
-        <f>L8*0.000001/($B8/44100)</f>
-        <v>7.166249999999999E-2</v>
-      </c>
-      <c r="AH8" s="11">
-        <f>R8*0.000001/($B8/44100)</f>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11">
+        <f>M8*0.000001/($B8/44100)</f>
+        <v>7.0284374999999996E-2</v>
+      </c>
+      <c r="AK8" s="11">
+        <f>S8*0.000001/($B8/44100)</f>
         <v>0.17502187499999999</v>
       </c>
-      <c r="AI8" s="11">
-        <f>V8*0.000001/($B8/44100)</f>
+      <c r="AL8" s="11">
+        <f>W8*0.000001/($B8/44100)</f>
+        <v>3.5831249999999995E-2</v>
+      </c>
+      <c r="AM8" s="11">
+        <f>X8*0.000001/($B8/44100)</f>
+        <v>3.4453124999999994E-2</v>
+      </c>
+      <c r="AN8" s="11">
+        <f>Y8*0.000001/($B8/44100)</f>
         <v>5.0990624999999998E-2</v>
       </c>
-      <c r="AJ8" s="11">
-        <f>W8*0.000001/($B8/44100)</f>
+      <c r="AO8" s="11">
+        <f>Z8*0.000001/($B8/44100)</f>
         <v>8.5443749999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>64</v>
       </c>
@@ -2436,77 +2566,94 @@
         <v>121.98</v>
       </c>
       <c r="L9" s="12">
+        <v>77</v>
+      </c>
+      <c r="M9" s="12">
         <v>114</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>162.52000000000001</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>323.75</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>592.08000000000004</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="R9" s="13">
         <v>854.36</v>
       </c>
-      <c r="R9" s="12">
+      <c r="S9" s="12">
         <v>238</v>
       </c>
-      <c r="T9" s="13">
+      <c r="U9" s="13">
         <f>'ARM-Specific Functions'!K11</f>
         <v>712.13</v>
       </c>
-      <c r="U9" s="13">
+      <c r="V9" s="13">
         <v>724.79</v>
       </c>
-      <c r="V9" s="12">
+      <c r="W9" s="12">
+        <v>46</v>
+      </c>
+      <c r="X9" s="12">
+        <v>55</v>
+      </c>
+      <c r="Y9" s="12">
         <v>79</v>
       </c>
-      <c r="W9" s="12">
+      <c r="Z9" s="12">
         <v>102</v>
       </c>
-      <c r="Y9" s="9">
+      <c r="AB9" s="9">
         <v>1122.1300000000001</v>
       </c>
-      <c r="Z9" s="9">
+      <c r="AC9" s="9">
         <v>1662.88</v>
       </c>
-      <c r="AB9" s="11">
-        <f t="shared" ref="AB9:AB14" si="4">K9*0.000001/($B9/44100)</f>
+      <c r="AE9" s="11">
+        <f>K9*0.000001/($B9/44100)</f>
         <v>8.4051843749999994E-2</v>
       </c>
-      <c r="AC9" s="11">
-        <f t="shared" ref="AC9:AC14" si="5">Q9*0.000001/($B9/44100)</f>
+      <c r="AF9" s="11">
+        <f>R9*0.000001/($B9/44100)</f>
         <v>0.58870743749999999</v>
       </c>
-      <c r="AD9" s="11">
-        <f>T9*0.000001/($B9/44100)</f>
+      <c r="AG9" s="11">
+        <f>U9*0.000001/($B9/44100)</f>
         <v>0.49070207812499994</v>
       </c>
-      <c r="AE9" s="11">
-        <f>U9*0.000001/($B9/44100)</f>
+      <c r="AH9" s="11">
+        <f>V9*0.000001/($B9/44100)</f>
         <v>0.49942560937499991</v>
       </c>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11">
-        <f t="shared" ref="AG9:AG14" si="6">L9*0.000001/($B9/44100)</f>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="11">
+        <f>M9*0.000001/($B9/44100)</f>
         <v>7.8553124999999988E-2</v>
       </c>
-      <c r="AH9" s="11">
-        <f t="shared" ref="AG9:AH14" si="7">R9*0.000001/($B9/44100)</f>
+      <c r="AK9" s="11">
+        <f>S9*0.000001/($B9/44100)</f>
         <v>0.16399687499999999</v>
       </c>
-      <c r="AI9" s="11">
-        <f>V9*0.000001/(B9/44100)</f>
+      <c r="AL9" s="11">
+        <f t="shared" ref="AL9:AM14" si="1">W9*0.000001/($B9/44100)</f>
+        <v>3.1696874999999999E-2</v>
+      </c>
+      <c r="AM9" s="11">
+        <f t="shared" si="1"/>
+        <v>3.7898437499999993E-2</v>
+      </c>
+      <c r="AN9" s="11">
+        <f t="shared" ref="AN9:AN14" si="2">Y9*0.000001/($B9/44100)</f>
         <v>5.4435937499999996E-2</v>
       </c>
-      <c r="AJ9" s="11">
-        <f>W9*0.000001/(C9/44100)</f>
-        <v>6.698734177215189E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AO9" s="11">
+        <f t="shared" ref="AO9:AO14" si="3">Z9*0.000001/($B9/44100)</f>
+        <v>7.0284374999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>128</v>
       </c>
@@ -2526,77 +2673,94 @@
         <v>274.10000000000002</v>
       </c>
       <c r="L10" s="12">
-        <v>257</v>
-      </c>
-      <c r="M10">
+        <v>173</v>
+      </c>
+      <c r="M10" s="12">
+        <v>254</v>
+      </c>
+      <c r="N10">
         <v>355.3</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>721.27</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>1318.83</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="R10" s="13">
         <v>1982.42</v>
       </c>
-      <c r="R10" s="12">
+      <c r="S10" s="12">
         <v>632</v>
       </c>
-      <c r="T10" s="13">
+      <c r="U10" s="13">
         <f>'ARM-Specific Functions'!K12</f>
         <v>1664.97</v>
       </c>
-      <c r="U10" s="13">
+      <c r="V10" s="13">
         <v>1759.28</v>
       </c>
-      <c r="V10" s="12">
+      <c r="W10" s="12">
+        <v>107</v>
+      </c>
+      <c r="X10" s="12">
+        <v>118</v>
+      </c>
+      <c r="Y10" s="12">
         <v>173</v>
       </c>
-      <c r="W10" s="12">
+      <c r="Z10" s="12">
         <v>282</v>
       </c>
-      <c r="Y10" s="9">
+      <c r="AB10" s="9">
         <v>2080.58</v>
       </c>
-      <c r="Z10" s="9">
+      <c r="AC10" s="9">
         <v>3368.27</v>
       </c>
-      <c r="AB10" s="11">
-        <f t="shared" si="4"/>
+      <c r="AE10" s="11">
+        <f>K10*0.000001/($B10/44100)</f>
         <v>9.4436015624999994E-2</v>
       </c>
-      <c r="AC10" s="11">
-        <f t="shared" si="5"/>
+      <c r="AF10" s="11">
+        <f>R10*0.000001/($B10/44100)</f>
         <v>0.68300564062499991</v>
       </c>
-      <c r="AD10" s="11">
-        <f>T10*0.000001/($B10/44100)</f>
+      <c r="AG10" s="11">
+        <f>U10*0.000001/($B10/44100)</f>
         <v>0.57363419531250004</v>
       </c>
-      <c r="AE10" s="11">
-        <f>U10*0.000001/($B10/44100)</f>
+      <c r="AH10" s="11">
+        <f>V10*0.000001/($B10/44100)</f>
         <v>0.60612693749999991</v>
       </c>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11">
-        <f t="shared" si="6"/>
-        <v>8.8544531250000003E-2</v>
-      </c>
-      <c r="AH10" s="11">
-        <f t="shared" si="7"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11">
+        <f>M10*0.000001/($B10/44100)</f>
+        <v>8.7510937499999997E-2</v>
+      </c>
+      <c r="AK10" s="11">
+        <f>S10*0.000001/($B10/44100)</f>
         <v>0.21774374999999999</v>
       </c>
-      <c r="AI10" s="11">
-        <f>V10*0.000001/(B10/44100)</f>
+      <c r="AL10" s="11">
+        <f t="shared" si="1"/>
+        <v>3.6864843750000001E-2</v>
+      </c>
+      <c r="AM10" s="11">
+        <f t="shared" si="1"/>
+        <v>4.0654687499999995E-2</v>
+      </c>
+      <c r="AN10" s="11">
+        <f t="shared" si="2"/>
         <v>5.9603906249999998E-2</v>
       </c>
-      <c r="AJ10" s="11">
-        <f>W10*0.000001/(C10/44100)</f>
-        <v>8.6147132169576035E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AO10" s="11">
+        <f t="shared" si="3"/>
+        <v>9.7157812499999982E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>256</v>
       </c>
@@ -2616,77 +2780,94 @@
         <v>614.41999999999996</v>
       </c>
       <c r="L11" s="12">
-        <v>570</v>
-      </c>
-      <c r="M11">
+        <v>382</v>
+      </c>
+      <c r="M11" s="12">
+        <v>566</v>
+      </c>
+      <c r="N11">
         <v>776.61</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>1595.22</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>2917.8</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="R11" s="13">
         <v>4197.54</v>
       </c>
-      <c r="R11" s="12">
+      <c r="S11" s="12">
         <v>1199</v>
       </c>
-      <c r="T11" s="13">
+      <c r="U11" s="13">
         <f>'ARM-Specific Functions'!K13</f>
         <v>3819.2</v>
       </c>
-      <c r="U11" s="13">
+      <c r="V11" s="13">
         <v>3756.42</v>
       </c>
-      <c r="V11" s="12">
+      <c r="W11" s="12">
+        <v>207</v>
+      </c>
+      <c r="X11" s="12">
+        <v>255</v>
+      </c>
+      <c r="Y11" s="12">
         <v>374</v>
       </c>
-      <c r="W11" s="12">
+      <c r="Z11" s="12">
         <v>477</v>
       </c>
-      <c r="Y11" s="9">
+      <c r="AB11" s="9">
         <v>4087.76</v>
       </c>
-      <c r="Z11" s="9">
+      <c r="AC11" s="9">
         <v>6991.74</v>
       </c>
-      <c r="AB11" s="11">
-        <f t="shared" si="4"/>
+      <c r="AE11" s="11">
+        <f>K11*0.000001/($B11/44100)</f>
         <v>0.10584344531249999</v>
       </c>
-      <c r="AC11" s="11">
-        <f t="shared" si="5"/>
+      <c r="AF11" s="11">
+        <f>R11*0.000001/($B11/44100)</f>
         <v>0.72309185156249989</v>
       </c>
-      <c r="AD11" s="11">
-        <f>T11*0.000001/($B11/44100)</f>
+      <c r="AG11" s="11">
+        <f>U11*0.000001/($B11/44100)</f>
         <v>0.65791687499999996</v>
       </c>
-      <c r="AE11" s="11">
-        <f>U11*0.000001/($B11/44100)</f>
+      <c r="AH11" s="11">
+        <f>V11*0.000001/($B11/44100)</f>
         <v>0.64710203906249997</v>
       </c>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11">
-        <f t="shared" si="6"/>
-        <v>9.8191406249999988E-2</v>
-      </c>
-      <c r="AH11" s="11">
-        <f t="shared" si="7"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11">
+        <f>M11*0.000001/($B11/44100)</f>
+        <v>9.7502343749999998E-2</v>
+      </c>
+      <c r="AK11" s="11">
+        <f>S11*0.000001/($B11/44100)</f>
         <v>0.20654648437500001</v>
       </c>
-      <c r="AI11" s="11">
-        <f>V11*0.000001/(B11/44100)</f>
+      <c r="AL11" s="11">
+        <f t="shared" si="1"/>
+        <v>3.5658984375000001E-2</v>
+      </c>
+      <c r="AM11" s="11">
+        <f t="shared" si="1"/>
+        <v>4.3927734374999992E-2</v>
+      </c>
+      <c r="AN11" s="11">
+        <f t="shared" si="2"/>
         <v>6.4427343749999991E-2</v>
       </c>
-      <c r="AJ11" s="11">
-        <f>W11*0.000001/(C11/44100)</f>
-        <v>6.7153072625698321E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AO11" s="11">
+        <f t="shared" si="3"/>
+        <v>8.2170703124999994E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>512</v>
       </c>
@@ -2706,77 +2887,94 @@
         <v>1361.9</v>
       </c>
       <c r="L12" s="12">
-        <v>1251</v>
-      </c>
-      <c r="M12">
+        <v>835</v>
+      </c>
+      <c r="M12" s="12">
+        <v>1243</v>
+      </c>
+      <c r="N12">
         <v>1688.09</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>3498.65</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>6393.07</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="R12" s="13">
         <v>9582.68</v>
       </c>
-      <c r="R12" s="12">
+      <c r="S12" s="12">
         <v>3031</v>
       </c>
-      <c r="T12" s="13">
+      <c r="U12" s="13">
         <f>'ARM-Specific Functions'!K14</f>
         <v>8619.5400000000009</v>
       </c>
-      <c r="U12" s="13">
+      <c r="V12" s="13">
         <v>8768.08</v>
       </c>
-      <c r="V12" s="12">
+      <c r="W12" s="12">
+        <v>470</v>
+      </c>
+      <c r="X12" s="12">
+        <v>550</v>
+      </c>
+      <c r="Y12" s="12">
         <v>799</v>
       </c>
-      <c r="W12" s="12">
+      <c r="Z12" s="12">
         <v>1272</v>
       </c>
-      <c r="Y12" s="9">
+      <c r="AB12" s="9">
         <v>8299.17</v>
       </c>
-      <c r="Z12" s="9">
+      <c r="AC12" s="9">
         <v>14675.67</v>
       </c>
-      <c r="AB12" s="11">
-        <f t="shared" si="4"/>
+      <c r="AE12" s="11">
+        <f>K12*0.000001/($B12/44100)</f>
         <v>0.11730427734375</v>
       </c>
-      <c r="AC12" s="11">
-        <f t="shared" si="5"/>
+      <c r="AF12" s="11">
+        <f>R12*0.000001/($B12/44100)</f>
         <v>0.82538317968749997</v>
       </c>
-      <c r="AD12" s="11">
-        <f>T12*0.000001/($B12/44100)</f>
+      <c r="AG12" s="11">
+        <f>U12*0.000001/($B12/44100)</f>
         <v>0.74242522265624999</v>
       </c>
-      <c r="AE12" s="11">
-        <f>U12*0.000001/($B12/44100)</f>
+      <c r="AH12" s="11">
+        <f>V12*0.000001/($B12/44100)</f>
         <v>0.75521939062499988</v>
       </c>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11">
-        <f t="shared" si="6"/>
-        <v>0.10775214843749999</v>
-      </c>
-      <c r="AH12" s="11">
-        <f t="shared" si="7"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="11">
+        <f>M12*0.000001/($B12/44100)</f>
+        <v>0.1070630859375</v>
+      </c>
+      <c r="AK12" s="11">
+        <f>S12*0.000001/($B12/44100)</f>
         <v>0.26106855468749995</v>
       </c>
-      <c r="AI12" s="11">
-        <f>V12*0.000001/(B12/44100)</f>
+      <c r="AL12" s="11">
+        <f t="shared" si="1"/>
+        <v>4.0482421875000001E-2</v>
+      </c>
+      <c r="AM12" s="11">
+        <f t="shared" si="1"/>
+        <v>4.7373046874999991E-2</v>
+      </c>
+      <c r="AN12" s="11">
+        <f t="shared" si="2"/>
         <v>6.8820117187500002E-2</v>
       </c>
-      <c r="AJ12" s="11">
-        <f>W12*0.000001/(C12/44100)</f>
-        <v>8.4078059893881701E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AO12" s="11">
+        <f t="shared" si="3"/>
+        <v>0.1095609375</v>
+      </c>
+    </row>
+    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1024</v>
       </c>
@@ -2805,77 +3003,94 @@
         <v>3009.96</v>
       </c>
       <c r="L13" s="12">
-        <v>2740</v>
-      </c>
-      <c r="M13">
+        <v>1827</v>
+      </c>
+      <c r="M13" s="12">
+        <v>1243</v>
+      </c>
+      <c r="N13">
         <v>3654.13</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>7621.21</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>13917.22</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="R13" s="13">
         <v>20189.66</v>
       </c>
-      <c r="R13" s="12">
+      <c r="S13" s="12">
         <v>5801</v>
       </c>
-      <c r="T13" s="13">
+      <c r="U13" s="13">
         <f>'ARM-Specific Functions'!K15</f>
         <v>19211.900000000001</v>
       </c>
-      <c r="U13" s="13">
+      <c r="V13" s="13">
         <v>18485.53</v>
       </c>
-      <c r="V13" s="12">
+      <c r="W13" s="12">
+        <v>956</v>
+      </c>
+      <c r="X13" s="12">
+        <v>1183</v>
+      </c>
+      <c r="Y13" s="12">
         <v>1725</v>
       </c>
-      <c r="W13" s="12">
+      <c r="Z13" s="12">
         <v>2196</v>
       </c>
-      <c r="Y13" s="9">
+      <c r="AB13" s="9">
         <v>17191.080000000002</v>
       </c>
-      <c r="Z13" s="9">
+      <c r="AC13" s="9">
         <v>30967.26</v>
       </c>
-      <c r="AB13" s="11">
-        <f t="shared" si="4"/>
+      <c r="AE13" s="11">
+        <f>K13*0.000001/($B13/44100)</f>
         <v>0.12962816015625001</v>
       </c>
-      <c r="AC13" s="11">
-        <f t="shared" si="5"/>
+      <c r="AF13" s="11">
+        <f>R13*0.000001/($B13/44100)</f>
         <v>0.86949609960937491</v>
       </c>
-      <c r="AD13" s="11">
-        <f>T13*0.000001/($B13/44100)</f>
+      <c r="AG13" s="11">
+        <f>U13*0.000001/($B13/44100)</f>
         <v>0.82738749023437497</v>
       </c>
-      <c r="AE13" s="11">
-        <f>U13*0.000001/($B13/44100)</f>
+      <c r="AH13" s="11">
+        <f>V13*0.000001/($B13/44100)</f>
         <v>0.79610534472656236</v>
       </c>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11">
-        <f t="shared" si="6"/>
-        <v>0.11800195312499999</v>
-      </c>
-      <c r="AH13" s="11">
-        <f t="shared" si="7"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11">
+        <f>M13*0.000001/($B13/44100)</f>
+        <v>5.3531542968749998E-2</v>
+      </c>
+      <c r="AK13" s="11">
+        <f>S13*0.000001/($B13/44100)</f>
         <v>0.24982822265624999</v>
       </c>
-      <c r="AI13" s="11">
-        <f>V13*0.000001/(B13/44100)</f>
+      <c r="AL13" s="11">
+        <f t="shared" si="1"/>
+        <v>4.1171484374999998E-2</v>
+      </c>
+      <c r="AM13" s="11">
+        <f t="shared" si="1"/>
+        <v>5.0947558593749998E-2</v>
+      </c>
+      <c r="AN13" s="11">
+        <f t="shared" si="2"/>
         <v>7.4289550781249991E-2</v>
       </c>
-      <c r="AJ13" s="11">
-        <f>W13*0.000001/(C13/44100)</f>
-        <v>6.7131290725079715E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AO13" s="11">
+        <f t="shared" si="3"/>
+        <v>9.4573828124999995E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2048</v>
       </c>
@@ -2892,288 +3107,409 @@
         <v>6578.57</v>
       </c>
       <c r="L14" s="12">
-        <v>5906</v>
-      </c>
-      <c r="M14">
+        <v>3927</v>
+      </c>
+      <c r="M14" s="12">
+        <v>5874</v>
+      </c>
+      <c r="N14">
         <v>7866.48</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>16942.04</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>30090.02</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="R14" s="13">
         <v>45220.12</v>
       </c>
-      <c r="R14" s="12">
+      <c r="S14" s="12">
         <v>14133</v>
       </c>
-      <c r="T14" s="13">
+      <c r="U14" s="13">
         <f>'ARM-Specific Functions'!K16</f>
         <v>42355.1</v>
       </c>
-      <c r="U14" s="13">
+      <c r="V14" s="13">
         <v>42107.63</v>
       </c>
-      <c r="V14" s="12">
+      <c r="W14" s="12">
+        <v>2135</v>
+      </c>
+      <c r="X14" s="12">
+        <v>2464</v>
+      </c>
+      <c r="Y14" s="12">
         <v>3628</v>
       </c>
-      <c r="W14" s="12">
+      <c r="Z14" s="12">
         <v>5658</v>
       </c>
-      <c r="Y14" s="9">
+      <c r="AB14" s="9">
         <v>35957.269999999997</v>
       </c>
-      <c r="Z14" s="9">
+      <c r="AC14" s="9">
         <v>65450.37</v>
       </c>
-      <c r="AB14" s="11">
-        <f t="shared" si="4"/>
+      <c r="AE14" s="11">
+        <f>K14*0.000001/($B14/44100)</f>
         <v>0.14165768408203125</v>
       </c>
-      <c r="AC14" s="11">
-        <f t="shared" si="5"/>
+      <c r="AF14" s="11">
+        <f>R14*0.000001/($B14/44100)</f>
         <v>0.97373402929687503</v>
       </c>
-      <c r="AD14" s="11">
-        <f>T14*0.000001/($B14/44100)</f>
+      <c r="AG14" s="11">
+        <f>U14*0.000001/($B14/44100)</f>
         <v>0.91204097167968745</v>
       </c>
-      <c r="AE14" s="11">
-        <f>U14*0.000001/($B14/44100)</f>
+      <c r="AH14" s="11">
+        <f>V14*0.000001/($B14/44100)</f>
         <v>0.90671214990234361</v>
       </c>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11">
-        <f t="shared" si="6"/>
-        <v>0.12717509765624999</v>
-      </c>
-      <c r="AH14" s="11">
-        <f t="shared" si="7"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11">
+        <f>M14*0.000001/($B14/44100)</f>
+        <v>0.12648603515624998</v>
+      </c>
+      <c r="AK14" s="11">
+        <f>S14*0.000001/($B14/44100)</f>
         <v>0.30432875976562501</v>
       </c>
-      <c r="AI14" s="11">
-        <f>V14*0.000001/(B14/44100)</f>
+      <c r="AL14" s="11">
+        <f t="shared" si="1"/>
+        <v>4.597338867187499E-2</v>
+      </c>
+      <c r="AM14" s="11">
+        <f t="shared" si="1"/>
+        <v>5.3057812500000003E-2</v>
+      </c>
+      <c r="AN14" s="11">
+        <f t="shared" si="2"/>
         <v>7.8122460937499999E-2</v>
       </c>
-      <c r="AJ14" s="11">
-        <f>W14*0.000001/(C14/44100)</f>
-        <v>8.0799518151879288E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AO14" s="11">
+        <f t="shared" si="3"/>
+        <v>0.12183486328125</v>
+      </c>
+    </row>
+    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B8</f>
         <v>32</v>
       </c>
-      <c r="T17" s="2">
-        <f>T8/$B8</f>
-        <v>9.2721874999999994</v>
-      </c>
       <c r="U17" s="2">
         <f>U8/$B8</f>
+        <v>9.2721874999999994</v>
+      </c>
+      <c r="V17" s="2">
+        <f>V8/$B8</f>
         <v>10.575625</v>
       </c>
-      <c r="V17" s="2"/>
       <c r="W17" s="2">
         <f>W8/$B8</f>
+        <v>0.8125</v>
+      </c>
+      <c r="X17" s="2">
+        <f>X8/$B8</f>
+        <v>0.78125</v>
+      </c>
+      <c r="Y17" s="2">
+        <f>Y8/$B8</f>
+        <v>1.15625</v>
+      </c>
+      <c r="Z17" s="2">
+        <f>Z8/$B8</f>
         <v>1.9375</v>
       </c>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="10">
-        <f t="shared" ref="Y17:Z17" si="8">Y8/$B8</f>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="10">
+        <f t="shared" ref="AB17:AC17" si="4">AB8/$B8</f>
         <v>20.468125000000001</v>
       </c>
-      <c r="Z17" s="10">
+      <c r="AC17" s="10">
+        <f t="shared" si="4"/>
+        <v>26.46125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" ref="B18:B23" si="5">B9</f>
+        <v>64</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" ref="U18:AC18" si="6">U9/$B9</f>
+        <v>11.12703125</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" ref="V18" si="7">V9/$B9</f>
+        <v>11.324843749999999</v>
+      </c>
+      <c r="W18" s="2">
+        <f>W9/$B9</f>
+        <v>0.71875</v>
+      </c>
+      <c r="X18" s="2">
+        <f>X9/$B9</f>
+        <v>0.859375</v>
+      </c>
+      <c r="Y18" s="2">
+        <f t="shared" ref="Y18:Z18" si="8">Y9/$B9</f>
+        <v>1.234375</v>
+      </c>
+      <c r="Z18" s="2">
         <f t="shared" si="8"/>
-        <v>26.46125</v>
-      </c>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f t="shared" ref="B18:B23" si="9">B9</f>
-        <v>64</v>
-      </c>
-      <c r="T18" s="2">
-        <f t="shared" ref="T18:Z18" si="10">T9/$B9</f>
-        <v>11.12703125</v>
-      </c>
-      <c r="U18" s="2">
-        <f t="shared" ref="U18:W18" si="11">U9/$B9</f>
-        <v>11.324843749999999</v>
-      </c>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2">
+        <v>1.59375</v>
+      </c>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="10">
+        <f t="shared" si="6"/>
+        <v>17.533281250000002</v>
+      </c>
+      <c r="AC18" s="10">
+        <f t="shared" si="6"/>
+        <v>25.982500000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="U19" s="2">
+        <f t="shared" ref="U19:AC19" si="9">U10/$B10</f>
+        <v>13.007578125</v>
+      </c>
+      <c r="V19" s="2">
+        <f t="shared" ref="V19" si="10">V10/$B10</f>
+        <v>13.744375</v>
+      </c>
+      <c r="W19" s="2">
+        <f>W10/$B10</f>
+        <v>0.8359375</v>
+      </c>
+      <c r="X19" s="2">
+        <f>X10/$B10</f>
+        <v>0.921875</v>
+      </c>
+      <c r="Y19" s="2">
+        <f t="shared" ref="Y19:Z19" si="11">Y10/$B10</f>
+        <v>1.3515625</v>
+      </c>
+      <c r="Z19" s="2">
         <f t="shared" si="11"/>
-        <v>1.59375</v>
-      </c>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="10">
-        <f t="shared" si="10"/>
-        <v>17.533281250000002</v>
-      </c>
-      <c r="Z18" s="10">
-        <f t="shared" si="10"/>
-        <v>25.982500000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B19">
+        <v>2.203125</v>
+      </c>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="10">
         <f t="shared" si="9"/>
-        <v>128</v>
-      </c>
-      <c r="T19" s="2">
-        <f t="shared" ref="T19:Z19" si="12">T10/$B10</f>
-        <v>13.007578125</v>
-      </c>
-      <c r="U19" s="2">
-        <f t="shared" ref="U19:W19" si="13">U10/$B10</f>
-        <v>13.744375</v>
-      </c>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2">
-        <f t="shared" si="13"/>
-        <v>2.203125</v>
-      </c>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="10">
+        <v>16.254531249999999</v>
+      </c>
+      <c r="AC19" s="10">
+        <f t="shared" si="9"/>
+        <v>26.314609375</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" ref="U20:AC20" si="12">U11/$B11</f>
+        <v>14.918749999999999</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" ref="V20" si="13">V11/$B11</f>
+        <v>14.673515625</v>
+      </c>
+      <c r="W20" s="2">
+        <f>W11/$B11</f>
+        <v>0.80859375</v>
+      </c>
+      <c r="X20" s="2">
+        <f>X11/$B11</f>
+        <v>0.99609375</v>
+      </c>
+      <c r="Y20" s="2">
+        <f t="shared" ref="Y20:Z20" si="14">Y11/$B11</f>
+        <v>1.4609375</v>
+      </c>
+      <c r="Z20" s="2">
+        <f t="shared" si="14"/>
+        <v>1.86328125</v>
+      </c>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="10">
         <f t="shared" si="12"/>
-        <v>16.254531249999999</v>
-      </c>
-      <c r="Z19" s="10">
+        <v>15.967812500000001</v>
+      </c>
+      <c r="AC20" s="10">
         <f t="shared" si="12"/>
-        <v>26.314609375</v>
-      </c>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f t="shared" si="9"/>
-        <v>256</v>
-      </c>
-      <c r="T20" s="2">
-        <f t="shared" ref="T20:Z20" si="14">T11/$B11</f>
-        <v>14.918749999999999</v>
-      </c>
-      <c r="U20" s="2">
-        <f t="shared" ref="U20:W20" si="15">U11/$B11</f>
-        <v>14.673515625</v>
-      </c>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2">
-        <f t="shared" si="15"/>
-        <v>1.86328125</v>
-      </c>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="10">
-        <f t="shared" si="14"/>
-        <v>15.967812500000001</v>
-      </c>
-      <c r="Z20" s="10">
-        <f t="shared" si="14"/>
         <v>27.311484374999999</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>512</v>
       </c>
-      <c r="T21" s="2">
-        <f t="shared" ref="T21:Z21" si="16">T12/$B12</f>
+      <c r="U21" s="2">
+        <f t="shared" ref="U21:AC21" si="15">U12/$B12</f>
         <v>16.835039062500002</v>
       </c>
-      <c r="U21" s="2">
-        <f t="shared" ref="U21:W21" si="17">U12/$B12</f>
+      <c r="V21" s="2">
+        <f t="shared" ref="V21" si="16">V12/$B12</f>
         <v>17.12515625</v>
       </c>
-      <c r="V21" s="2"/>
       <c r="W21" s="2">
+        <f>W12/$B12</f>
+        <v>0.91796875</v>
+      </c>
+      <c r="X21" s="2">
+        <f>X12/$B12</f>
+        <v>1.07421875</v>
+      </c>
+      <c r="Y21" s="2">
+        <f t="shared" ref="Y21:Z21" si="17">Y12/$B12</f>
+        <v>1.560546875</v>
+      </c>
+      <c r="Z21" s="2">
         <f t="shared" si="17"/>
         <v>2.484375</v>
       </c>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="10">
-        <f t="shared" si="16"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="10">
+        <f t="shared" si="15"/>
         <v>16.20931640625</v>
       </c>
-      <c r="Z21" s="10">
-        <f t="shared" si="16"/>
+      <c r="AC21" s="10">
+        <f t="shared" si="15"/>
         <v>28.66341796875</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>1024</v>
       </c>
-      <c r="T22" s="2">
-        <f t="shared" ref="T22:Z22" si="18">T13/$B13</f>
+      <c r="U22" s="2">
+        <f t="shared" ref="U22:AC22" si="18">U13/$B13</f>
         <v>18.761621093750001</v>
       </c>
-      <c r="U22" s="2">
-        <f t="shared" ref="U22:W22" si="19">U13/$B13</f>
+      <c r="V22" s="2">
+        <f t="shared" ref="V22" si="19">V13/$B13</f>
         <v>18.052275390624999</v>
       </c>
-      <c r="V22" s="2"/>
       <c r="W22" s="2">
-        <f t="shared" si="19"/>
+        <f>W13/$B13</f>
+        <v>0.93359375</v>
+      </c>
+      <c r="X22" s="2">
+        <f>X13/$B13</f>
+        <v>1.1552734375</v>
+      </c>
+      <c r="Y22" s="2">
+        <f t="shared" ref="Y22:Z22" si="20">Y13/$B13</f>
+        <v>1.6845703125</v>
+      </c>
+      <c r="Z22" s="2">
+        <f t="shared" si="20"/>
         <v>2.14453125</v>
       </c>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="10">
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="10">
         <f t="shared" si="18"/>
         <v>16.788164062500002</v>
       </c>
-      <c r="Z22" s="10">
+      <c r="AC22" s="10">
         <f t="shared" si="18"/>
         <v>30.241464843749998</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>2048</v>
       </c>
-      <c r="T23" s="2">
-        <f t="shared" ref="T23:Z23" si="20">T14/$B14</f>
+      <c r="U23" s="2">
+        <f t="shared" ref="U23:AC23" si="21">U14/$B14</f>
         <v>20.681201171874999</v>
       </c>
-      <c r="U23" s="2">
-        <f t="shared" ref="U23:W23" si="21">U14/$B14</f>
+      <c r="V23" s="2">
+        <f t="shared" ref="V23" si="22">V14/$B14</f>
         <v>20.560366210937499</v>
       </c>
-      <c r="V23" s="2"/>
       <c r="W23" s="2">
+        <f>W14/$B14</f>
+        <v>1.04248046875</v>
+      </c>
+      <c r="X23" s="2">
+        <f>X14/$B14</f>
+        <v>1.203125</v>
+      </c>
+      <c r="Y23" s="2">
+        <f t="shared" ref="Y23:Z23" si="23">Y14/$B14</f>
+        <v>1.771484375</v>
+      </c>
+      <c r="Z23" s="2">
+        <f t="shared" si="23"/>
+        <v>2.7626953125</v>
+      </c>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="10">
         <f t="shared" si="21"/>
-        <v>2.7626953125</v>
-      </c>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="10">
-        <f t="shared" si="20"/>
         <v>17.557260742187498</v>
       </c>
-      <c r="Z23" s="10">
-        <f t="shared" si="20"/>
+      <c r="AC23" s="10">
+        <f t="shared" si="21"/>
         <v>31.958188476562501</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="T24" s="2"/>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
-      <c r="Y24" s="10"/>
-      <c r="Z24" s="10"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="10"/>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+    </row>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y26" s="2"/>
+    </row>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y27" s="2"/>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y28" s="2"/>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y29" s="2"/>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y30" s="2"/>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y31" s="2"/>
+    </row>
+    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Benchmark: refactoring Kinetis code
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -1874,11 +1874,11 @@
         <v>Teensy 3.0</v>
       </c>
       <c r="AG2" t="str">
-        <f>U2</f>
+        <f t="shared" ref="AG2:AH6" si="0">U2</f>
         <v>Teensy 3.0</v>
       </c>
       <c r="AH2" t="str">
-        <f>V2</f>
+        <f t="shared" si="0"/>
         <v>Teensy 3.0</v>
       </c>
       <c r="AJ2" t="str">
@@ -1890,19 +1890,19 @@
         <v>NXP K66</v>
       </c>
       <c r="AL2" t="str">
-        <f>W2</f>
+        <f t="shared" ref="AL2:AN6" si="1">W2</f>
         <v>NXP K66</v>
       </c>
       <c r="AM2" t="str">
-        <f>X2</f>
+        <f t="shared" si="1"/>
         <v>NXP K66</v>
       </c>
       <c r="AN2" t="str">
-        <f>Y2</f>
+        <f t="shared" si="1"/>
         <v>NXP K66</v>
       </c>
       <c r="AO2" t="str">
-        <f t="shared" ref="AO2:AO6" si="0">Z2</f>
+        <f t="shared" ref="AO2:AO6" si="2">Z2</f>
         <v>NXP K66</v>
       </c>
     </row>
@@ -1982,11 +1982,11 @@
         <v>96 MHz</v>
       </c>
       <c r="AG3" t="str">
-        <f>U3</f>
+        <f t="shared" si="0"/>
         <v>96 MHz</v>
       </c>
       <c r="AH3" t="str">
-        <f>V3</f>
+        <f t="shared" si="0"/>
         <v>96 MHz</v>
       </c>
       <c r="AJ3" t="str">
@@ -1998,19 +1998,19 @@
         <v>120 MHz</v>
       </c>
       <c r="AL3" t="str">
-        <f>W3</f>
+        <f t="shared" si="1"/>
         <v>180 MHz</v>
       </c>
       <c r="AM3" t="str">
-        <f>X3</f>
+        <f t="shared" si="1"/>
         <v>180 MHz</v>
       </c>
       <c r="AN3" t="str">
-        <f>Y3</f>
+        <f t="shared" si="1"/>
         <v>120 MHz</v>
       </c>
       <c r="AO3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>120 MHz</v>
       </c>
     </row>
@@ -2090,11 +2090,11 @@
         <v>Int32</v>
       </c>
       <c r="AG4" t="str">
-        <f>U4</f>
+        <f t="shared" si="0"/>
         <v>Float</v>
       </c>
       <c r="AH4" t="str">
-        <f>V4</f>
+        <f t="shared" si="0"/>
         <v>All Float</v>
       </c>
       <c r="AJ4" t="str">
@@ -2106,19 +2106,19 @@
         <v>Int32</v>
       </c>
       <c r="AL4" t="str">
-        <f>W4</f>
+        <f t="shared" si="1"/>
         <v>All Float</v>
       </c>
       <c r="AM4" t="str">
-        <f>X4</f>
+        <f t="shared" si="1"/>
         <v>All Float</v>
       </c>
       <c r="AN4" t="str">
-        <f>Y4</f>
+        <f t="shared" si="1"/>
         <v>All Float</v>
       </c>
       <c r="AO4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>All Float</v>
       </c>
     </row>
@@ -2198,11 +2198,11 @@
         <v>KissFFT</v>
       </c>
       <c r="AG5" t="str">
-        <f>U5</f>
+        <f t="shared" si="0"/>
         <v>cfft, radix 2</v>
       </c>
       <c r="AH5" t="str">
-        <f>V5</f>
+        <f t="shared" si="0"/>
         <v>KissFFT</v>
       </c>
       <c r="AJ5" t="str">
@@ -2214,19 +2214,19 @@
         <v>KissFFT</v>
       </c>
       <c r="AL5" t="str">
-        <f>W5</f>
+        <f t="shared" si="1"/>
         <v>cfft, radix 4</v>
       </c>
       <c r="AM5" t="str">
-        <f>X5</f>
+        <f t="shared" si="1"/>
         <v>cfft, radix 2</v>
       </c>
       <c r="AN5" t="str">
-        <f>Y5</f>
+        <f t="shared" si="1"/>
         <v>cfft, radix 2</v>
       </c>
       <c r="AO5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>KissFFT</v>
       </c>
     </row>
@@ -2306,11 +2306,11 @@
         <v>Generic C</v>
       </c>
       <c r="AG6" t="str">
-        <f>U6</f>
+        <f t="shared" si="0"/>
         <v>ARM-Specific</v>
       </c>
       <c r="AH6" t="str">
-        <f>V6</f>
+        <f t="shared" si="0"/>
         <v>Generic C</v>
       </c>
       <c r="AJ6" t="str">
@@ -2322,19 +2322,19 @@
         <v>Generic C</v>
       </c>
       <c r="AL6" t="str">
-        <f>W6</f>
+        <f t="shared" si="1"/>
         <v>ARM-Specific</v>
       </c>
       <c r="AM6" t="str">
-        <f>X6</f>
+        <f t="shared" si="1"/>
         <v>ARM-Specific</v>
       </c>
       <c r="AN6" t="str">
-        <f>Y6</f>
+        <f t="shared" si="1"/>
         <v>ARM-Specific</v>
       </c>
       <c r="AO6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Generic C</v>
       </c>
     </row>
@@ -2505,28 +2505,28 @@
         <v>846.76</v>
       </c>
       <c r="AE8" s="11">
-        <f>K8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AE8:AE14" si="3">K8*0.000001/($B8/44100)</f>
         <v>7.4584124999999987E-2</v>
       </c>
       <c r="AF8" s="11">
-        <f>R8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AF8:AF14" si="4">R8*0.000001/($B8/44100)</f>
         <v>0.56507259374999996</v>
       </c>
       <c r="AG8" s="11">
-        <f>U8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AG8:AH14" si="5">U8*0.000001/($B8/44100)</f>
         <v>0.40890346874999989</v>
       </c>
       <c r="AH8" s="11">
-        <f>V8*0.000001/($B8/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.46638506249999995</v>
       </c>
       <c r="AI8" s="11"/>
       <c r="AJ8" s="11">
-        <f>M8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AJ8:AJ14" si="6">M8*0.000001/($B8/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
       <c r="AK8" s="11">
-        <f>S8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AK8:AK14" si="7">S8*0.000001/($B8/44100)</f>
         <v>0.17502187499999999</v>
       </c>
       <c r="AL8" s="11">
@@ -2612,44 +2612,44 @@
         <v>1662.88</v>
       </c>
       <c r="AE9" s="11">
-        <f>K9*0.000001/($B9/44100)</f>
+        <f t="shared" si="3"/>
         <v>8.4051843749999994E-2</v>
       </c>
       <c r="AF9" s="11">
-        <f>R9*0.000001/($B9/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.58870743749999999</v>
       </c>
       <c r="AG9" s="11">
-        <f>U9*0.000001/($B9/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.49070207812499994</v>
       </c>
       <c r="AH9" s="11">
-        <f>V9*0.000001/($B9/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.49942560937499991</v>
       </c>
       <c r="AI9" s="11"/>
       <c r="AJ9" s="11">
-        <f>M9*0.000001/($B9/44100)</f>
+        <f t="shared" si="6"/>
         <v>7.8553124999999988E-2</v>
       </c>
       <c r="AK9" s="11">
-        <f>S9*0.000001/($B9/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.16399687499999999</v>
       </c>
       <c r="AL9" s="11">
-        <f t="shared" ref="AL9:AM14" si="1">W9*0.000001/($B9/44100)</f>
+        <f t="shared" ref="AL9:AM14" si="8">W9*0.000001/($B9/44100)</f>
         <v>3.1696874999999999E-2</v>
       </c>
       <c r="AM9" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>3.7898437499999993E-2</v>
       </c>
       <c r="AN9" s="11">
-        <f t="shared" ref="AN9:AN14" si="2">Y9*0.000001/($B9/44100)</f>
+        <f t="shared" ref="AN9:AN14" si="9">Y9*0.000001/($B9/44100)</f>
         <v>5.4435937499999996E-2</v>
       </c>
       <c r="AO9" s="11">
-        <f t="shared" ref="AO9:AO14" si="3">Z9*0.000001/($B9/44100)</f>
+        <f t="shared" ref="AO9:AO14" si="10">Z9*0.000001/($B9/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
     </row>
@@ -2719,44 +2719,44 @@
         <v>3368.27</v>
       </c>
       <c r="AE10" s="11">
-        <f>K10*0.000001/($B10/44100)</f>
+        <f t="shared" si="3"/>
         <v>9.4436015624999994E-2</v>
       </c>
       <c r="AF10" s="11">
-        <f>R10*0.000001/($B10/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.68300564062499991</v>
       </c>
       <c r="AG10" s="11">
-        <f>U10*0.000001/($B10/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.57363419531250004</v>
       </c>
       <c r="AH10" s="11">
-        <f>V10*0.000001/($B10/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.60612693749999991</v>
       </c>
       <c r="AI10" s="11"/>
       <c r="AJ10" s="11">
-        <f>M10*0.000001/($B10/44100)</f>
+        <f t="shared" si="6"/>
         <v>8.7510937499999997E-2</v>
       </c>
       <c r="AK10" s="11">
-        <f>S10*0.000001/($B10/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.21774374999999999</v>
       </c>
       <c r="AL10" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>3.6864843750000001E-2</v>
       </c>
       <c r="AM10" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4.0654687499999995E-2</v>
       </c>
       <c r="AN10" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>5.9603906249999998E-2</v>
       </c>
       <c r="AO10" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>9.7157812499999982E-2</v>
       </c>
     </row>
@@ -2826,44 +2826,44 @@
         <v>6991.74</v>
       </c>
       <c r="AE11" s="11">
-        <f>K11*0.000001/($B11/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.10584344531249999</v>
       </c>
       <c r="AF11" s="11">
-        <f>R11*0.000001/($B11/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.72309185156249989</v>
       </c>
       <c r="AG11" s="11">
-        <f>U11*0.000001/($B11/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.65791687499999996</v>
       </c>
       <c r="AH11" s="11">
-        <f>V11*0.000001/($B11/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.64710203906249997</v>
       </c>
       <c r="AI11" s="11"/>
       <c r="AJ11" s="11">
-        <f>M11*0.000001/($B11/44100)</f>
+        <f t="shared" si="6"/>
         <v>9.7502343749999998E-2</v>
       </c>
       <c r="AK11" s="11">
-        <f>S11*0.000001/($B11/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.20654648437500001</v>
       </c>
       <c r="AL11" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>3.5658984375000001E-2</v>
       </c>
       <c r="AM11" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4.3927734374999992E-2</v>
       </c>
       <c r="AN11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>6.4427343749999991E-2</v>
       </c>
       <c r="AO11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>8.2170703124999994E-2</v>
       </c>
     </row>
@@ -2933,44 +2933,44 @@
         <v>14675.67</v>
       </c>
       <c r="AE12" s="11">
-        <f>K12*0.000001/($B12/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.11730427734375</v>
       </c>
       <c r="AF12" s="11">
-        <f>R12*0.000001/($B12/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.82538317968749997</v>
       </c>
       <c r="AG12" s="11">
-        <f>U12*0.000001/($B12/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.74242522265624999</v>
       </c>
       <c r="AH12" s="11">
-        <f>V12*0.000001/($B12/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.75521939062499988</v>
       </c>
       <c r="AI12" s="11"/>
       <c r="AJ12" s="11">
-        <f>M12*0.000001/($B12/44100)</f>
+        <f t="shared" si="6"/>
         <v>0.1070630859375</v>
       </c>
       <c r="AK12" s="11">
-        <f>S12*0.000001/($B12/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.26106855468749995</v>
       </c>
       <c r="AL12" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4.0482421875000001E-2</v>
       </c>
       <c r="AM12" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4.7373046874999991E-2</v>
       </c>
       <c r="AN12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>6.8820117187500002E-2</v>
       </c>
       <c r="AO12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>0.1095609375</v>
       </c>
     </row>
@@ -3049,44 +3049,44 @@
         <v>30967.26</v>
       </c>
       <c r="AE13" s="11">
-        <f>K13*0.000001/($B13/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.12962816015625001</v>
       </c>
       <c r="AF13" s="11">
-        <f>R13*0.000001/($B13/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.86949609960937491</v>
       </c>
       <c r="AG13" s="11">
-        <f>U13*0.000001/($B13/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.82738749023437497</v>
       </c>
       <c r="AH13" s="11">
-        <f>V13*0.000001/($B13/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.79610534472656236</v>
       </c>
       <c r="AI13" s="11"/>
       <c r="AJ13" s="11">
-        <f>M13*0.000001/($B13/44100)</f>
+        <f t="shared" si="6"/>
         <v>5.3531542968749998E-2</v>
       </c>
       <c r="AK13" s="11">
-        <f>S13*0.000001/($B13/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.24982822265624999</v>
       </c>
       <c r="AL13" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4.1171484374999998E-2</v>
       </c>
       <c r="AM13" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>5.0947558593749998E-2</v>
       </c>
       <c r="AN13" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>7.4289550781249991E-2</v>
       </c>
       <c r="AO13" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>9.4573828124999995E-2</v>
       </c>
     </row>
@@ -3153,44 +3153,44 @@
         <v>65450.37</v>
       </c>
       <c r="AE14" s="11">
-        <f>K14*0.000001/($B14/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.14165768408203125</v>
       </c>
       <c r="AF14" s="11">
-        <f>R14*0.000001/($B14/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.97373402929687503</v>
       </c>
       <c r="AG14" s="11">
-        <f>U14*0.000001/($B14/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.91204097167968745</v>
       </c>
       <c r="AH14" s="11">
-        <f>V14*0.000001/($B14/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.90671214990234361</v>
       </c>
       <c r="AI14" s="11"/>
       <c r="AJ14" s="11">
-        <f>M14*0.000001/($B14/44100)</f>
+        <f t="shared" si="6"/>
         <v>0.12648603515624998</v>
       </c>
       <c r="AK14" s="11">
-        <f>S14*0.000001/($B14/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.30432875976562501</v>
       </c>
       <c r="AL14" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4.597338867187499E-2</v>
       </c>
       <c r="AM14" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>5.3057812500000003E-2</v>
       </c>
       <c r="AN14" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>7.8122460937499999E-2</v>
       </c>
       <c r="AO14" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>0.12183486328125</v>
       </c>
     </row>
@@ -3208,270 +3208,270 @@
         <v>32</v>
       </c>
       <c r="U17" s="2">
-        <f>U8/$B8</f>
+        <f t="shared" ref="U17:Z17" si="11">U8/$B8</f>
         <v>9.2721874999999994</v>
       </c>
       <c r="V17" s="2">
-        <f>V8/$B8</f>
+        <f t="shared" si="11"/>
         <v>10.575625</v>
       </c>
       <c r="W17" s="2">
-        <f>W8/$B8</f>
+        <f t="shared" si="11"/>
         <v>0.8125</v>
       </c>
       <c r="X17" s="2">
-        <f>X8/$B8</f>
+        <f t="shared" si="11"/>
         <v>0.78125</v>
       </c>
       <c r="Y17" s="2">
-        <f>Y8/$B8</f>
+        <f t="shared" si="11"/>
         <v>1.15625</v>
       </c>
       <c r="Z17" s="2">
-        <f>Z8/$B8</f>
+        <f t="shared" si="11"/>
         <v>1.9375</v>
       </c>
       <c r="AA17" s="2"/>
       <c r="AB17" s="10">
-        <f t="shared" ref="AB17:AC17" si="4">AB8/$B8</f>
+        <f t="shared" ref="AB17:AC17" si="12">AB8/$B8</f>
         <v>20.468125000000001</v>
       </c>
       <c r="AC17" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>26.46125</v>
       </c>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f t="shared" ref="B18:B23" si="5">B9</f>
+        <f t="shared" ref="B18:B23" si="13">B9</f>
         <v>64</v>
       </c>
       <c r="U18" s="2">
-        <f t="shared" ref="U18:AC18" si="6">U9/$B9</f>
+        <f t="shared" ref="U18:AC18" si="14">U9/$B9</f>
         <v>11.12703125</v>
       </c>
       <c r="V18" s="2">
-        <f t="shared" ref="V18" si="7">V9/$B9</f>
+        <f t="shared" ref="V18" si="15">V9/$B9</f>
         <v>11.324843749999999</v>
       </c>
       <c r="W18" s="2">
-        <f>W9/$B9</f>
+        <f t="shared" ref="W18:X23" si="16">W9/$B9</f>
         <v>0.71875</v>
       </c>
       <c r="X18" s="2">
-        <f>X9/$B9</f>
+        <f t="shared" si="16"/>
         <v>0.859375</v>
       </c>
       <c r="Y18" s="2">
-        <f t="shared" ref="Y18:Z18" si="8">Y9/$B9</f>
+        <f t="shared" ref="Y18:Z18" si="17">Y9/$B9</f>
         <v>1.234375</v>
       </c>
       <c r="Z18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.59375</v>
       </c>
       <c r="AA18" s="2"/>
       <c r="AB18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>17.533281250000002</v>
       </c>
       <c r="AC18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>25.982500000000002</v>
       </c>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>128</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" ref="U19:AC19" si="9">U10/$B10</f>
+        <f t="shared" ref="U19:AC19" si="18">U10/$B10</f>
         <v>13.007578125</v>
       </c>
       <c r="V19" s="2">
-        <f t="shared" ref="V19" si="10">V10/$B10</f>
+        <f t="shared" ref="V19" si="19">V10/$B10</f>
         <v>13.744375</v>
       </c>
       <c r="W19" s="2">
-        <f>W10/$B10</f>
+        <f t="shared" si="16"/>
         <v>0.8359375</v>
       </c>
       <c r="X19" s="2">
-        <f>X10/$B10</f>
+        <f t="shared" si="16"/>
         <v>0.921875</v>
       </c>
       <c r="Y19" s="2">
-        <f t="shared" ref="Y19:Z19" si="11">Y10/$B10</f>
+        <f t="shared" ref="Y19:Z19" si="20">Y10/$B10</f>
         <v>1.3515625</v>
       </c>
       <c r="Z19" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>2.203125</v>
       </c>
       <c r="AA19" s="2"/>
       <c r="AB19" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>16.254531249999999</v>
       </c>
       <c r="AC19" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>26.314609375</v>
       </c>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>256</v>
       </c>
       <c r="U20" s="2">
-        <f t="shared" ref="U20:AC20" si="12">U11/$B11</f>
+        <f t="shared" ref="U20:AC20" si="21">U11/$B11</f>
         <v>14.918749999999999</v>
       </c>
       <c r="V20" s="2">
-        <f t="shared" ref="V20" si="13">V11/$B11</f>
+        <f t="shared" ref="V20" si="22">V11/$B11</f>
         <v>14.673515625</v>
       </c>
       <c r="W20" s="2">
-        <f>W11/$B11</f>
+        <f t="shared" si="16"/>
         <v>0.80859375</v>
       </c>
       <c r="X20" s="2">
-        <f>X11/$B11</f>
+        <f t="shared" si="16"/>
         <v>0.99609375</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" ref="Y20:Z20" si="14">Y11/$B11</f>
+        <f t="shared" ref="Y20:Z20" si="23">Y11/$B11</f>
         <v>1.4609375</v>
       </c>
       <c r="Z20" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>1.86328125</v>
       </c>
       <c r="AA20" s="2"/>
       <c r="AB20" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>15.967812500000001</v>
       </c>
       <c r="AC20" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>27.311484374999999</v>
       </c>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>512</v>
       </c>
       <c r="U21" s="2">
-        <f t="shared" ref="U21:AC21" si="15">U12/$B12</f>
+        <f t="shared" ref="U21:AC21" si="24">U12/$B12</f>
         <v>16.835039062500002</v>
       </c>
       <c r="V21" s="2">
-        <f t="shared" ref="V21" si="16">V12/$B12</f>
+        <f t="shared" ref="V21" si="25">V12/$B12</f>
         <v>17.12515625</v>
       </c>
       <c r="W21" s="2">
-        <f>W12/$B12</f>
+        <f t="shared" si="16"/>
         <v>0.91796875</v>
       </c>
       <c r="X21" s="2">
-        <f>X12/$B12</f>
+        <f t="shared" si="16"/>
         <v>1.07421875</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" ref="Y21:Z21" si="17">Y12/$B12</f>
+        <f t="shared" ref="Y21:Z21" si="26">Y12/$B12</f>
         <v>1.560546875</v>
       </c>
       <c r="Z21" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.484375</v>
       </c>
       <c r="AA21" s="2"/>
       <c r="AB21" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>16.20931640625</v>
       </c>
       <c r="AC21" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>28.66341796875</v>
       </c>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>1024</v>
       </c>
       <c r="U22" s="2">
-        <f t="shared" ref="U22:AC22" si="18">U13/$B13</f>
+        <f t="shared" ref="U22:AC22" si="27">U13/$B13</f>
         <v>18.761621093750001</v>
       </c>
       <c r="V22" s="2">
-        <f t="shared" ref="V22" si="19">V13/$B13</f>
+        <f t="shared" ref="V22" si="28">V13/$B13</f>
         <v>18.052275390624999</v>
       </c>
       <c r="W22" s="2">
-        <f>W13/$B13</f>
+        <f t="shared" si="16"/>
         <v>0.93359375</v>
       </c>
       <c r="X22" s="2">
-        <f>X13/$B13</f>
+        <f t="shared" si="16"/>
         <v>1.1552734375</v>
       </c>
       <c r="Y22" s="2">
-        <f t="shared" ref="Y22:Z22" si="20">Y13/$B13</f>
+        <f t="shared" ref="Y22:Z22" si="29">Y13/$B13</f>
         <v>1.6845703125</v>
       </c>
       <c r="Z22" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>2.14453125</v>
       </c>
       <c r="AA22" s="2"/>
       <c r="AB22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>16.788164062500002</v>
       </c>
       <c r="AC22" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>30.241464843749998</v>
       </c>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>2048</v>
       </c>
       <c r="U23" s="2">
-        <f t="shared" ref="U23:AC23" si="21">U14/$B14</f>
+        <f t="shared" ref="U23:AC23" si="30">U14/$B14</f>
         <v>20.681201171874999</v>
       </c>
       <c r="V23" s="2">
-        <f t="shared" ref="V23" si="22">V14/$B14</f>
+        <f t="shared" ref="V23" si="31">V14/$B14</f>
         <v>20.560366210937499</v>
       </c>
       <c r="W23" s="2">
-        <f>W14/$B14</f>
+        <f t="shared" si="16"/>
         <v>1.04248046875</v>
       </c>
       <c r="X23" s="2">
-        <f>X14/$B14</f>
+        <f t="shared" si="16"/>
         <v>1.203125</v>
       </c>
       <c r="Y23" s="2">
-        <f t="shared" ref="Y23:Z23" si="23">Y14/$B14</f>
+        <f t="shared" ref="Y23:Z23" si="32">Y14/$B14</f>
         <v>1.771484375</v>
       </c>
       <c r="Z23" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>2.7626953125</v>
       </c>
       <c r="AA23" s="2"/>
       <c r="AB23" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>17.557260742187498</v>
       </c>
       <c r="AC23" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>31.958188476562501</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Benchmark: KISS_FFT now working when refactored
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="46">
   <si>
     <t>N</t>
   </si>
@@ -1773,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AO32"/>
+  <dimension ref="B2:AP32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,14 +1791,14 @@
     <col min="18" max="19" width="10.85546875" customWidth="1"/>
     <col min="20" max="20" width="2.5703125" customWidth="1"/>
     <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="11.42578125" customWidth="1"/>
-    <col min="27" max="27" width="3.5703125" customWidth="1"/>
-    <col min="28" max="28" width="11.28515625" style="9" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" style="9" customWidth="1"/>
-    <col min="35" max="35" width="2.140625" customWidth="1"/>
+    <col min="22" max="27" width="11.42578125" customWidth="1"/>
+    <col min="28" max="28" width="3.5703125" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" style="9" customWidth="1"/>
+    <col min="30" max="30" width="10.42578125" style="9" customWidth="1"/>
+    <col min="36" max="36" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -1859,54 +1859,57 @@
       <c r="Z2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="9" t="s">
-        <v>22</v>
+      <c r="AA2" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AD2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF2" t="str">
         <f>K2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AG2" t="str">
         <f>R2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AG2" t="str">
-        <f t="shared" ref="AG2:AH6" si="0">U2</f>
+      <c r="AH2" t="str">
+        <f>U2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AH2" t="str">
-        <f t="shared" si="0"/>
+      <c r="AI2" t="str">
+        <f>V2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AJ2" t="str">
+      <c r="AK2" t="str">
         <f>M2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AK2" t="str">
+      <c r="AL2" t="str">
         <f>S2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AL2" t="str">
-        <f t="shared" ref="AL2:AN6" si="1">W2</f>
+      <c r="AM2" t="str">
+        <f>W2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AM2" t="str">
-        <f t="shared" si="1"/>
+      <c r="AN2" t="str">
+        <f>X2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AN2" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO2" t="str">
+        <f>Z2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AO2" t="str">
-        <f t="shared" ref="AO2:AO6" si="2">Z2</f>
+      <c r="AP2" t="str">
+        <f t="shared" ref="AP2:AP6" si="0">AA2</f>
         <v>NXP K66</v>
       </c>
     </row>
-    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1961,60 +1964,63 @@
       <c r="X3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="Y3" s="12" t="s">
-        <v>43</v>
+      <c r="Y3" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="Z3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AB3" s="9" t="s">
-        <v>10</v>
+      <c r="AA3" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="AC3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AD3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3" t="str">
         <f>K3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AF3" t="str">
+      <c r="AG3" t="str">
         <f>R3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AG3" t="str">
-        <f t="shared" si="0"/>
+      <c r="AH3" t="str">
+        <f>U3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AH3" t="str">
-        <f t="shared" si="0"/>
+      <c r="AI3" t="str">
+        <f>V3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AJ3" t="str">
+      <c r="AK3" t="str">
         <f>M3</f>
         <v>120 MHz</v>
       </c>
-      <c r="AK3" t="str">
+      <c r="AL3" t="str">
         <f>S3</f>
         <v>120 MHz</v>
       </c>
-      <c r="AL3" t="str">
-        <f t="shared" si="1"/>
+      <c r="AM3" t="str">
+        <f>W3</f>
         <v>180 MHz</v>
       </c>
-      <c r="AM3" t="str">
-        <f t="shared" si="1"/>
+      <c r="AN3" t="str">
+        <f>X3</f>
         <v>180 MHz</v>
       </c>
-      <c r="AN3" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO3" t="str">
+        <f>Z3</f>
         <v>120 MHz</v>
       </c>
-      <c r="AO3" t="str">
-        <f t="shared" si="2"/>
+      <c r="AP3" t="str">
+        <f t="shared" si="0"/>
         <v>120 MHz</v>
       </c>
     </row>
-    <row r="4" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>32</v>
       </c>
@@ -2075,54 +2081,57 @@
       <c r="Z4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AB4" s="9" t="s">
+      <c r="AA4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="AC4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" t="str">
+      <c r="AF4" t="str">
         <f>K4</f>
         <v>Int32</v>
       </c>
-      <c r="AF4" t="str">
+      <c r="AG4" t="str">
         <f>R4</f>
         <v>Int32</v>
       </c>
-      <c r="AG4" t="str">
-        <f t="shared" si="0"/>
+      <c r="AH4" t="str">
+        <f>U4</f>
         <v>Float</v>
       </c>
-      <c r="AH4" t="str">
+      <c r="AI4" t="str">
+        <f>V4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AK4" t="str">
+        <f>M4</f>
+        <v>Int32</v>
+      </c>
+      <c r="AL4" t="str">
+        <f>S4</f>
+        <v>Int32</v>
+      </c>
+      <c r="AM4" t="str">
+        <f>W4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AN4" t="str">
+        <f>X4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AO4" t="str">
+        <f>Z4</f>
+        <v>All Float</v>
+      </c>
+      <c r="AP4" t="str">
         <f t="shared" si="0"/>
         <v>All Float</v>
       </c>
-      <c r="AJ4" t="str">
-        <f>M4</f>
-        <v>Int32</v>
-      </c>
-      <c r="AK4" t="str">
-        <f>S4</f>
-        <v>Int32</v>
-      </c>
-      <c r="AL4" t="str">
-        <f t="shared" si="1"/>
-        <v>All Float</v>
-      </c>
-      <c r="AM4" t="str">
-        <f t="shared" si="1"/>
-        <v>All Float</v>
-      </c>
-      <c r="AN4" t="str">
-        <f t="shared" si="1"/>
-        <v>All Float</v>
-      </c>
-      <c r="AO4" t="str">
-        <f t="shared" si="2"/>
-        <v>All Float</v>
-      </c>
-    </row>
-    <row r="5" spans="2:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>26</v>
       </c>
@@ -2178,59 +2187,62 @@
         <v>26</v>
       </c>
       <c r="Y5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="AA5" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="AC5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AE5" t="str">
+      <c r="AD5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF5" t="str">
         <f>K5</f>
         <v>cfft, radix 2</v>
       </c>
-      <c r="AF5" t="str">
+      <c r="AG5" t="str">
         <f>R5</f>
         <v>KissFFT</v>
       </c>
-      <c r="AG5" t="str">
-        <f t="shared" si="0"/>
+      <c r="AH5" t="str">
+        <f>U5</f>
         <v>cfft, radix 2</v>
       </c>
-      <c r="AH5" t="str">
+      <c r="AI5" t="str">
+        <f>V5</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="AK5" t="str">
+        <f>M5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AL5" t="str">
+        <f>S5</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="AM5" t="str">
+        <f>W5</f>
+        <v>cfft, radix 4</v>
+      </c>
+      <c r="AN5" t="str">
+        <f>X5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AO5" t="str">
+        <f>Z5</f>
+        <v>cfft, radix 2</v>
+      </c>
+      <c r="AP5" t="str">
         <f t="shared" si="0"/>
         <v>KissFFT</v>
       </c>
-      <c r="AJ5" t="str">
-        <f>M5</f>
-        <v>cfft, radix 2</v>
-      </c>
-      <c r="AK5" t="str">
-        <f>S5</f>
-        <v>KissFFT</v>
-      </c>
-      <c r="AL5" t="str">
-        <f t="shared" si="1"/>
-        <v>cfft, radix 4</v>
-      </c>
-      <c r="AM5" t="str">
-        <f t="shared" si="1"/>
-        <v>cfft, radix 2</v>
-      </c>
-      <c r="AN5" t="str">
-        <f t="shared" si="1"/>
-        <v>cfft, radix 2</v>
-      </c>
-      <c r="AO5" t="str">
-        <f t="shared" si="2"/>
-        <v>KissFFT</v>
-      </c>
-    </row>
-    <row r="6" spans="2:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>27</v>
       </c>
@@ -2286,59 +2298,62 @@
         <v>27</v>
       </c>
       <c r="Y6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Z6" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AA6" s="12" t="s">
         <v>25</v>
       </c>
       <c r="AC6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AE6" t="str">
+      <c r="AD6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF6" t="str">
         <f>K6</f>
         <v>ARM-Specific</v>
       </c>
-      <c r="AF6" t="str">
+      <c r="AG6" t="str">
         <f>R6</f>
         <v>Generic C</v>
       </c>
-      <c r="AG6" t="str">
-        <f t="shared" si="0"/>
+      <c r="AH6" t="str">
+        <f>U6</f>
         <v>ARM-Specific</v>
       </c>
-      <c r="AH6" t="str">
+      <c r="AI6" t="str">
+        <f>V6</f>
+        <v>Generic C</v>
+      </c>
+      <c r="AK6" t="str">
+        <f>M6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AL6" t="str">
+        <f>S6</f>
+        <v>Generic C</v>
+      </c>
+      <c r="AM6" t="str">
+        <f>W6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AN6" t="str">
+        <f>X6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AO6" t="str">
+        <f>Z6</f>
+        <v>ARM-Specific</v>
+      </c>
+      <c r="AP6" t="str">
         <f t="shared" si="0"/>
         <v>Generic C</v>
       </c>
-      <c r="AJ6" t="str">
-        <f>M6</f>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AK6" t="str">
-        <f>S6</f>
-        <v>Generic C</v>
-      </c>
-      <c r="AL6" t="str">
-        <f t="shared" si="1"/>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AM6" t="str">
-        <f t="shared" si="1"/>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AN6" t="str">
-        <f t="shared" si="1"/>
-        <v>ARM-Specific</v>
-      </c>
-      <c r="AO6" t="str">
-        <f t="shared" si="2"/>
-        <v>Generic C</v>
-      </c>
-    </row>
-    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -2402,14 +2417,14 @@
       <c r="Z7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AB7" s="9" t="s">
+      <c r="AA7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="AC7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AE7" t="s">
-        <v>42</v>
+      <c r="AD7" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="AF7" t="s">
         <v>42</v>
@@ -2420,7 +2435,7 @@
       <c r="AH7" t="s">
         <v>42</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AI7" t="s">
         <v>42</v>
       </c>
       <c r="AK7" t="s">
@@ -2438,8 +2453,11 @@
       <c r="AO7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AP7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>32</v>
       </c>
@@ -2493,60 +2511,63 @@
         <v>25</v>
       </c>
       <c r="Y8" s="12">
+        <v>48</v>
+      </c>
+      <c r="Z8" s="12">
         <v>37</v>
       </c>
-      <c r="Z8" s="12">
+      <c r="AA8" s="12">
         <v>62</v>
       </c>
-      <c r="AB8" s="9">
+      <c r="AC8" s="9">
         <v>654.98</v>
       </c>
-      <c r="AC8" s="9">
+      <c r="AD8" s="9">
         <v>846.76</v>
       </c>
-      <c r="AE8" s="11">
-        <f t="shared" ref="AE8:AE14" si="3">K8*0.000001/($B8/44100)</f>
+      <c r="AF8" s="11">
+        <f>K8*0.000001/($B8/44100)</f>
         <v>7.4584124999999987E-2</v>
       </c>
-      <c r="AF8" s="11">
-        <f t="shared" ref="AF8:AF14" si="4">R8*0.000001/($B8/44100)</f>
+      <c r="AG8" s="11">
+        <f>R8*0.000001/($B8/44100)</f>
         <v>0.56507259374999996</v>
       </c>
-      <c r="AG8" s="11">
-        <f t="shared" ref="AG8:AH14" si="5">U8*0.000001/($B8/44100)</f>
+      <c r="AH8" s="11">
+        <f>U8*0.000001/($B8/44100)</f>
         <v>0.40890346874999989</v>
       </c>
-      <c r="AH8" s="11">
-        <f t="shared" si="5"/>
+      <c r="AI8" s="11">
+        <f>V8*0.000001/($B8/44100)</f>
         <v>0.46638506249999995</v>
       </c>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11">
-        <f t="shared" ref="AJ8:AJ14" si="6">M8*0.000001/($B8/44100)</f>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11">
+        <f>M8*0.000001/($B8/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
-      <c r="AK8" s="11">
-        <f t="shared" ref="AK8:AK14" si="7">S8*0.000001/($B8/44100)</f>
+      <c r="AL8" s="11">
+        <f>S8*0.000001/($B8/44100)</f>
         <v>0.17502187499999999</v>
       </c>
-      <c r="AL8" s="11">
+      <c r="AM8" s="11">
         <f>W8*0.000001/($B8/44100)</f>
         <v>3.5831249999999995E-2</v>
       </c>
-      <c r="AM8" s="11">
+      <c r="AN8" s="11">
         <f>X8*0.000001/($B8/44100)</f>
         <v>3.4453124999999994E-2</v>
       </c>
-      <c r="AN8" s="11">
-        <f>Y8*0.000001/($B8/44100)</f>
-        <v>5.0990624999999998E-2</v>
-      </c>
       <c r="AO8" s="11">
         <f>Z8*0.000001/($B8/44100)</f>
+        <v>5.0990624999999998E-2</v>
+      </c>
+      <c r="AP8" s="11">
+        <f>AA8*0.000001/($B8/44100)</f>
         <v>8.5443749999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>64</v>
       </c>
@@ -2600,60 +2621,63 @@
         <v>55</v>
       </c>
       <c r="Y9" s="12">
+        <v>80</v>
+      </c>
+      <c r="Z9" s="12">
         <v>79</v>
       </c>
-      <c r="Z9" s="12">
+      <c r="AA9" s="12">
         <v>102</v>
       </c>
-      <c r="AB9" s="9">
+      <c r="AC9" s="9">
         <v>1122.1300000000001</v>
       </c>
-      <c r="AC9" s="9">
+      <c r="AD9" s="9">
         <v>1662.88</v>
       </c>
-      <c r="AE9" s="11">
-        <f t="shared" si="3"/>
+      <c r="AF9" s="11">
+        <f>K9*0.000001/($B9/44100)</f>
         <v>8.4051843749999994E-2</v>
       </c>
-      <c r="AF9" s="11">
-        <f t="shared" si="4"/>
+      <c r="AG9" s="11">
+        <f>R9*0.000001/($B9/44100)</f>
         <v>0.58870743749999999</v>
       </c>
-      <c r="AG9" s="11">
-        <f t="shared" si="5"/>
+      <c r="AH9" s="11">
+        <f>U9*0.000001/($B9/44100)</f>
         <v>0.49070207812499994</v>
       </c>
-      <c r="AH9" s="11">
-        <f t="shared" si="5"/>
+      <c r="AI9" s="11">
+        <f>V9*0.000001/($B9/44100)</f>
         <v>0.49942560937499991</v>
       </c>
-      <c r="AI9" s="11"/>
-      <c r="AJ9" s="11">
-        <f t="shared" si="6"/>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="11">
+        <f>M9*0.000001/($B9/44100)</f>
         <v>7.8553124999999988E-2</v>
       </c>
-      <c r="AK9" s="11">
-        <f t="shared" si="7"/>
+      <c r="AL9" s="11">
+        <f>S9*0.000001/($B9/44100)</f>
         <v>0.16399687499999999</v>
       </c>
-      <c r="AL9" s="11">
-        <f t="shared" ref="AL9:AM14" si="8">W9*0.000001/($B9/44100)</f>
+      <c r="AM9" s="11">
+        <f>W9*0.000001/($B9/44100)</f>
         <v>3.1696874999999999E-2</v>
       </c>
-      <c r="AM9" s="11">
-        <f t="shared" si="8"/>
+      <c r="AN9" s="11">
+        <f>X9*0.000001/($B9/44100)</f>
         <v>3.7898437499999993E-2</v>
       </c>
-      <c r="AN9" s="11">
-        <f t="shared" ref="AN9:AN14" si="9">Y9*0.000001/($B9/44100)</f>
+      <c r="AO9" s="11">
+        <f>Z9*0.000001/($B9/44100)</f>
         <v>5.4435937499999996E-2</v>
       </c>
-      <c r="AO9" s="11">
-        <f t="shared" ref="AO9:AO14" si="10">Z9*0.000001/($B9/44100)</f>
+      <c r="AP9" s="11">
+        <f t="shared" ref="AP9:AP14" si="1">AA9*0.000001/($B9/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>128</v>
       </c>
@@ -2707,60 +2731,63 @@
         <v>118</v>
       </c>
       <c r="Y10" s="12">
+        <v>220</v>
+      </c>
+      <c r="Z10" s="12">
         <v>173</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="AA10" s="12">
         <v>282</v>
       </c>
-      <c r="AB10" s="9">
+      <c r="AC10" s="9">
         <v>2080.58</v>
       </c>
-      <c r="AC10" s="9">
+      <c r="AD10" s="9">
         <v>3368.27</v>
       </c>
-      <c r="AE10" s="11">
-        <f t="shared" si="3"/>
+      <c r="AF10" s="11">
+        <f>K10*0.000001/($B10/44100)</f>
         <v>9.4436015624999994E-2</v>
       </c>
-      <c r="AF10" s="11">
-        <f t="shared" si="4"/>
+      <c r="AG10" s="11">
+        <f>R10*0.000001/($B10/44100)</f>
         <v>0.68300564062499991</v>
       </c>
-      <c r="AG10" s="11">
-        <f t="shared" si="5"/>
+      <c r="AH10" s="11">
+        <f>U10*0.000001/($B10/44100)</f>
         <v>0.57363419531250004</v>
       </c>
-      <c r="AH10" s="11">
-        <f t="shared" si="5"/>
+      <c r="AI10" s="11">
+        <f>V10*0.000001/($B10/44100)</f>
         <v>0.60612693749999991</v>
       </c>
-      <c r="AI10" s="11"/>
-      <c r="AJ10" s="11">
-        <f t="shared" si="6"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11">
+        <f>M10*0.000001/($B10/44100)</f>
         <v>8.7510937499999997E-2</v>
       </c>
-      <c r="AK10" s="11">
-        <f t="shared" si="7"/>
+      <c r="AL10" s="11">
+        <f>S10*0.000001/($B10/44100)</f>
         <v>0.21774374999999999</v>
       </c>
-      <c r="AL10" s="11">
-        <f t="shared" si="8"/>
+      <c r="AM10" s="11">
+        <f>W10*0.000001/($B10/44100)</f>
         <v>3.6864843750000001E-2</v>
       </c>
-      <c r="AM10" s="11">
-        <f t="shared" si="8"/>
+      <c r="AN10" s="11">
+        <f>X10*0.000001/($B10/44100)</f>
         <v>4.0654687499999995E-2</v>
       </c>
-      <c r="AN10" s="11">
-        <f t="shared" si="9"/>
+      <c r="AO10" s="11">
+        <f>Z10*0.000001/($B10/44100)</f>
         <v>5.9603906249999998E-2</v>
       </c>
-      <c r="AO10" s="11">
-        <f t="shared" si="10"/>
+      <c r="AP10" s="11">
+        <f t="shared" si="1"/>
         <v>9.7157812499999982E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>256</v>
       </c>
@@ -2814,60 +2841,63 @@
         <v>255</v>
       </c>
       <c r="Y11" s="12">
+        <v>375</v>
+      </c>
+      <c r="Z11" s="12">
         <v>374</v>
       </c>
-      <c r="Z11" s="12">
+      <c r="AA11" s="12">
         <v>477</v>
       </c>
-      <c r="AB11" s="9">
+      <c r="AC11" s="9">
         <v>4087.76</v>
       </c>
-      <c r="AC11" s="9">
+      <c r="AD11" s="9">
         <v>6991.74</v>
       </c>
-      <c r="AE11" s="11">
-        <f t="shared" si="3"/>
+      <c r="AF11" s="11">
+        <f>K11*0.000001/($B11/44100)</f>
         <v>0.10584344531249999</v>
       </c>
-      <c r="AF11" s="11">
-        <f t="shared" si="4"/>
+      <c r="AG11" s="11">
+        <f>R11*0.000001/($B11/44100)</f>
         <v>0.72309185156249989</v>
       </c>
-      <c r="AG11" s="11">
-        <f t="shared" si="5"/>
+      <c r="AH11" s="11">
+        <f>U11*0.000001/($B11/44100)</f>
         <v>0.65791687499999996</v>
       </c>
-      <c r="AH11" s="11">
-        <f t="shared" si="5"/>
+      <c r="AI11" s="11">
+        <f>V11*0.000001/($B11/44100)</f>
         <v>0.64710203906249997</v>
       </c>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="11">
-        <f t="shared" si="6"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11">
+        <f>M11*0.000001/($B11/44100)</f>
         <v>9.7502343749999998E-2</v>
       </c>
-      <c r="AK11" s="11">
-        <f t="shared" si="7"/>
+      <c r="AL11" s="11">
+        <f>S11*0.000001/($B11/44100)</f>
         <v>0.20654648437500001</v>
       </c>
-      <c r="AL11" s="11">
-        <f t="shared" si="8"/>
+      <c r="AM11" s="11">
+        <f>W11*0.000001/($B11/44100)</f>
         <v>3.5658984375000001E-2</v>
       </c>
-      <c r="AM11" s="11">
-        <f t="shared" si="8"/>
+      <c r="AN11" s="11">
+        <f>X11*0.000001/($B11/44100)</f>
         <v>4.3927734374999992E-2</v>
       </c>
-      <c r="AN11" s="11">
-        <f t="shared" si="9"/>
+      <c r="AO11" s="11">
+        <f>Z11*0.000001/($B11/44100)</f>
         <v>6.4427343749999991E-2</v>
       </c>
-      <c r="AO11" s="11">
-        <f t="shared" si="10"/>
+      <c r="AP11" s="11">
+        <f t="shared" si="1"/>
         <v>8.2170703124999994E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>512</v>
       </c>
@@ -2921,60 +2951,63 @@
         <v>550</v>
       </c>
       <c r="Y12" s="12">
+        <v>990</v>
+      </c>
+      <c r="Z12" s="12">
         <v>799</v>
       </c>
-      <c r="Z12" s="12">
+      <c r="AA12" s="12">
         <v>1272</v>
       </c>
-      <c r="AB12" s="9">
+      <c r="AC12" s="9">
         <v>8299.17</v>
       </c>
-      <c r="AC12" s="9">
+      <c r="AD12" s="9">
         <v>14675.67</v>
       </c>
-      <c r="AE12" s="11">
-        <f t="shared" si="3"/>
+      <c r="AF12" s="11">
+        <f>K12*0.000001/($B12/44100)</f>
         <v>0.11730427734375</v>
       </c>
-      <c r="AF12" s="11">
-        <f t="shared" si="4"/>
+      <c r="AG12" s="11">
+        <f>R12*0.000001/($B12/44100)</f>
         <v>0.82538317968749997</v>
       </c>
-      <c r="AG12" s="11">
-        <f t="shared" si="5"/>
+      <c r="AH12" s="11">
+        <f>U12*0.000001/($B12/44100)</f>
         <v>0.74242522265624999</v>
       </c>
-      <c r="AH12" s="11">
-        <f t="shared" si="5"/>
+      <c r="AI12" s="11">
+        <f>V12*0.000001/($B12/44100)</f>
         <v>0.75521939062499988</v>
       </c>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="11">
-        <f t="shared" si="6"/>
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="11">
+        <f>M12*0.000001/($B12/44100)</f>
         <v>0.1070630859375</v>
       </c>
-      <c r="AK12" s="11">
-        <f t="shared" si="7"/>
+      <c r="AL12" s="11">
+        <f>S12*0.000001/($B12/44100)</f>
         <v>0.26106855468749995</v>
       </c>
-      <c r="AL12" s="11">
-        <f t="shared" si="8"/>
+      <c r="AM12" s="11">
+        <f>W12*0.000001/($B12/44100)</f>
         <v>4.0482421875000001E-2</v>
       </c>
-      <c r="AM12" s="11">
-        <f t="shared" si="8"/>
+      <c r="AN12" s="11">
+        <f>X12*0.000001/($B12/44100)</f>
         <v>4.7373046874999991E-2</v>
       </c>
-      <c r="AN12" s="11">
-        <f t="shared" si="9"/>
+      <c r="AO12" s="11">
+        <f>Z12*0.000001/($B12/44100)</f>
         <v>6.8820117187500002E-2</v>
       </c>
-      <c r="AO12" s="11">
-        <f t="shared" si="10"/>
+      <c r="AP12" s="11">
+        <f t="shared" si="1"/>
         <v>0.1095609375</v>
       </c>
     </row>
-    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1024</v>
       </c>
@@ -3037,60 +3070,63 @@
         <v>1183</v>
       </c>
       <c r="Y13" s="12">
+        <v>1728</v>
+      </c>
+      <c r="Z13" s="12">
         <v>1725</v>
       </c>
-      <c r="Z13" s="12">
+      <c r="AA13" s="12">
         <v>2196</v>
       </c>
-      <c r="AB13" s="9">
+      <c r="AC13" s="9">
         <v>17191.080000000002</v>
       </c>
-      <c r="AC13" s="9">
+      <c r="AD13" s="9">
         <v>30967.26</v>
       </c>
-      <c r="AE13" s="11">
-        <f t="shared" si="3"/>
+      <c r="AF13" s="11">
+        <f>K13*0.000001/($B13/44100)</f>
         <v>0.12962816015625001</v>
       </c>
-      <c r="AF13" s="11">
-        <f t="shared" si="4"/>
+      <c r="AG13" s="11">
+        <f>R13*0.000001/($B13/44100)</f>
         <v>0.86949609960937491</v>
       </c>
-      <c r="AG13" s="11">
-        <f t="shared" si="5"/>
+      <c r="AH13" s="11">
+        <f>U13*0.000001/($B13/44100)</f>
         <v>0.82738749023437497</v>
       </c>
-      <c r="AH13" s="11">
-        <f t="shared" si="5"/>
+      <c r="AI13" s="11">
+        <f>V13*0.000001/($B13/44100)</f>
         <v>0.79610534472656236</v>
       </c>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11">
-        <f t="shared" si="6"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11">
+        <f>M13*0.000001/($B13/44100)</f>
         <v>5.3531542968749998E-2</v>
       </c>
-      <c r="AK13" s="11">
-        <f t="shared" si="7"/>
+      <c r="AL13" s="11">
+        <f>S13*0.000001/($B13/44100)</f>
         <v>0.24982822265624999</v>
       </c>
-      <c r="AL13" s="11">
-        <f t="shared" si="8"/>
+      <c r="AM13" s="11">
+        <f>W13*0.000001/($B13/44100)</f>
         <v>4.1171484374999998E-2</v>
       </c>
-      <c r="AM13" s="11">
-        <f t="shared" si="8"/>
+      <c r="AN13" s="11">
+        <f>X13*0.000001/($B13/44100)</f>
         <v>5.0947558593749998E-2</v>
       </c>
-      <c r="AN13" s="11">
-        <f t="shared" si="9"/>
+      <c r="AO13" s="11">
+        <f>Z13*0.000001/($B13/44100)</f>
         <v>7.4289550781249991E-2</v>
       </c>
-      <c r="AO13" s="11">
-        <f t="shared" si="10"/>
+      <c r="AP13" s="11">
+        <f t="shared" si="1"/>
         <v>9.4573828124999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2048</v>
       </c>
@@ -3141,60 +3177,63 @@
         <v>2464</v>
       </c>
       <c r="Y14" s="12">
+        <v>4412</v>
+      </c>
+      <c r="Z14" s="12">
         <v>3628</v>
       </c>
-      <c r="Z14" s="12">
+      <c r="AA14" s="12">
         <v>5658</v>
       </c>
-      <c r="AB14" s="9">
+      <c r="AC14" s="9">
         <v>35957.269999999997</v>
       </c>
-      <c r="AC14" s="9">
+      <c r="AD14" s="9">
         <v>65450.37</v>
       </c>
-      <c r="AE14" s="11">
-        <f t="shared" si="3"/>
+      <c r="AF14" s="11">
+        <f>K14*0.000001/($B14/44100)</f>
         <v>0.14165768408203125</v>
       </c>
-      <c r="AF14" s="11">
-        <f t="shared" si="4"/>
+      <c r="AG14" s="11">
+        <f>R14*0.000001/($B14/44100)</f>
         <v>0.97373402929687503</v>
       </c>
-      <c r="AG14" s="11">
-        <f t="shared" si="5"/>
+      <c r="AH14" s="11">
+        <f>U14*0.000001/($B14/44100)</f>
         <v>0.91204097167968745</v>
       </c>
-      <c r="AH14" s="11">
-        <f t="shared" si="5"/>
+      <c r="AI14" s="11">
+        <f>V14*0.000001/($B14/44100)</f>
         <v>0.90671214990234361</v>
       </c>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11">
-        <f t="shared" si="6"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11">
+        <f>M14*0.000001/($B14/44100)</f>
         <v>0.12648603515624998</v>
       </c>
-      <c r="AK14" s="11">
-        <f t="shared" si="7"/>
+      <c r="AL14" s="11">
+        <f>S14*0.000001/($B14/44100)</f>
         <v>0.30432875976562501</v>
       </c>
-      <c r="AL14" s="11">
-        <f t="shared" si="8"/>
+      <c r="AM14" s="11">
+        <f>W14*0.000001/($B14/44100)</f>
         <v>4.597338867187499E-2</v>
       </c>
-      <c r="AM14" s="11">
-        <f t="shared" si="8"/>
+      <c r="AN14" s="11">
+        <f>X14*0.000001/($B14/44100)</f>
         <v>5.3057812500000003E-2</v>
       </c>
-      <c r="AN14" s="11">
-        <f t="shared" si="9"/>
+      <c r="AO14" s="11">
+        <f>Z14*0.000001/($B14/44100)</f>
         <v>7.8122460937499999E-2</v>
       </c>
-      <c r="AO14" s="11">
-        <f t="shared" si="10"/>
+      <c r="AP14" s="11">
+        <f t="shared" si="1"/>
         <v>0.12183486328125</v>
       </c>
     </row>
-    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -3202,314 +3241,343 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B8</f>
         <v>32</v>
       </c>
       <c r="U17" s="2">
-        <f t="shared" ref="U17:Z17" si="11">U8/$B8</f>
+        <f t="shared" ref="U17:AA17" si="2">U8/$B8</f>
         <v>9.2721874999999994</v>
       </c>
       <c r="V17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>10.575625</v>
       </c>
       <c r="W17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>0.8125</v>
       </c>
       <c r="X17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>0.78125</v>
       </c>
-      <c r="Y17" s="2">
-        <f t="shared" si="11"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2">
+        <f t="shared" si="2"/>
         <v>1.15625</v>
       </c>
-      <c r="Z17" s="2">
-        <f t="shared" si="11"/>
+      <c r="AA17" s="2">
+        <f t="shared" si="2"/>
         <v>1.9375</v>
       </c>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="10">
-        <f t="shared" ref="AB17:AC17" si="12">AB8/$B8</f>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="10">
+        <f t="shared" ref="AC17:AD17" si="3">AC8/$B8</f>
         <v>20.468125000000001</v>
       </c>
-      <c r="AC17" s="10">
+      <c r="AD17" s="10">
+        <f t="shared" si="3"/>
+        <v>26.46125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" ref="B18:B23" si="4">B9</f>
+        <v>64</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" ref="U18:AD18" si="5">U9/$B9</f>
+        <v>11.12703125</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" ref="V18" si="6">V9/$B9</f>
+        <v>11.324843749999999</v>
+      </c>
+      <c r="W18" s="2">
+        <f t="shared" ref="W18:Y23" si="7">W9/$B9</f>
+        <v>0.71875</v>
+      </c>
+      <c r="X18" s="2">
+        <f t="shared" si="7"/>
+        <v>0.859375</v>
+      </c>
+      <c r="Y18" s="2">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+      <c r="Z18" s="2">
+        <f t="shared" ref="Z18:AA18" si="8">Z9/$B9</f>
+        <v>1.234375</v>
+      </c>
+      <c r="AA18" s="2">
+        <f t="shared" si="8"/>
+        <v>1.59375</v>
+      </c>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="10">
+        <f t="shared" si="5"/>
+        <v>17.533281250000002</v>
+      </c>
+      <c r="AD18" s="10">
+        <f t="shared" si="5"/>
+        <v>25.982500000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="U19" s="2">
+        <f t="shared" ref="U19:AD19" si="9">U10/$B10</f>
+        <v>13.007578125</v>
+      </c>
+      <c r="V19" s="2">
+        <f t="shared" ref="V19" si="10">V10/$B10</f>
+        <v>13.744375</v>
+      </c>
+      <c r="W19" s="2">
+        <f t="shared" si="7"/>
+        <v>0.8359375</v>
+      </c>
+      <c r="X19" s="2">
+        <f t="shared" si="7"/>
+        <v>0.921875</v>
+      </c>
+      <c r="Y19" s="2">
+        <f t="shared" ref="Y19" si="11">Y10/$B10</f>
+        <v>1.71875</v>
+      </c>
+      <c r="Z19" s="2">
+        <f t="shared" ref="Z19:AA19" si="12">Z10/$B10</f>
+        <v>1.3515625</v>
+      </c>
+      <c r="AA19" s="2">
         <f t="shared" si="12"/>
-        <v>26.46125</v>
-      </c>
-    </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f t="shared" ref="B18:B23" si="13">B9</f>
-        <v>64</v>
-      </c>
-      <c r="U18" s="2">
-        <f t="shared" ref="U18:AC18" si="14">U9/$B9</f>
-        <v>11.12703125</v>
-      </c>
-      <c r="V18" s="2">
-        <f t="shared" ref="V18" si="15">V9/$B9</f>
-        <v>11.324843749999999</v>
-      </c>
-      <c r="W18" s="2">
-        <f t="shared" ref="W18:X23" si="16">W9/$B9</f>
-        <v>0.71875</v>
-      </c>
-      <c r="X18" s="2">
+        <v>2.203125</v>
+      </c>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="10">
+        <f t="shared" si="9"/>
+        <v>16.254531249999999</v>
+      </c>
+      <c r="AD19" s="10">
+        <f t="shared" si="9"/>
+        <v>26.314609375</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="4"/>
+        <v>256</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" ref="U20:AD20" si="13">U11/$B11</f>
+        <v>14.918749999999999</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" ref="V20" si="14">V11/$B11</f>
+        <v>14.673515625</v>
+      </c>
+      <c r="W20" s="2">
+        <f t="shared" si="7"/>
+        <v>0.80859375</v>
+      </c>
+      <c r="X20" s="2">
+        <f t="shared" si="7"/>
+        <v>0.99609375</v>
+      </c>
+      <c r="Y20" s="2">
+        <f t="shared" ref="Y20" si="15">Y11/$B11</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="Z20" s="2">
+        <f t="shared" ref="Z20:AA20" si="16">Z11/$B11</f>
+        <v>1.4609375</v>
+      </c>
+      <c r="AA20" s="2">
         <f t="shared" si="16"/>
-        <v>0.859375</v>
-      </c>
-      <c r="Y18" s="2">
-        <f t="shared" ref="Y18:Z18" si="17">Y9/$B9</f>
-        <v>1.234375</v>
-      </c>
-      <c r="Z18" s="2">
+        <v>1.86328125</v>
+      </c>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="10">
+        <f t="shared" si="13"/>
+        <v>15.967812500000001</v>
+      </c>
+      <c r="AD20" s="10">
+        <f t="shared" si="13"/>
+        <v>27.311484374999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="U21" s="2">
+        <f t="shared" ref="U21:AD21" si="17">U12/$B12</f>
+        <v>16.835039062500002</v>
+      </c>
+      <c r="V21" s="2">
+        <f t="shared" ref="V21" si="18">V12/$B12</f>
+        <v>17.12515625</v>
+      </c>
+      <c r="W21" s="2">
+        <f t="shared" si="7"/>
+        <v>0.91796875</v>
+      </c>
+      <c r="X21" s="2">
+        <f t="shared" si="7"/>
+        <v>1.07421875</v>
+      </c>
+      <c r="Y21" s="2">
+        <f t="shared" ref="Y21" si="19">Y12/$B12</f>
+        <v>1.93359375</v>
+      </c>
+      <c r="Z21" s="2">
+        <f t="shared" ref="Z21:AA21" si="20">Z12/$B12</f>
+        <v>1.560546875</v>
+      </c>
+      <c r="AA21" s="2">
+        <f t="shared" si="20"/>
+        <v>2.484375</v>
+      </c>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="10">
         <f t="shared" si="17"/>
-        <v>1.59375</v>
-      </c>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="10">
-        <f t="shared" si="14"/>
-        <v>17.533281250000002</v>
-      </c>
-      <c r="AC18" s="10">
-        <f t="shared" si="14"/>
-        <v>25.982500000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f t="shared" si="13"/>
-        <v>128</v>
-      </c>
-      <c r="U19" s="2">
-        <f t="shared" ref="U19:AC19" si="18">U10/$B10</f>
-        <v>13.007578125</v>
-      </c>
-      <c r="V19" s="2">
-        <f t="shared" ref="V19" si="19">V10/$B10</f>
-        <v>13.744375</v>
-      </c>
-      <c r="W19" s="2">
-        <f t="shared" si="16"/>
-        <v>0.8359375</v>
-      </c>
-      <c r="X19" s="2">
-        <f t="shared" si="16"/>
-        <v>0.921875</v>
-      </c>
-      <c r="Y19" s="2">
-        <f t="shared" ref="Y19:Z19" si="20">Y10/$B10</f>
-        <v>1.3515625</v>
-      </c>
-      <c r="Z19" s="2">
-        <f t="shared" si="20"/>
-        <v>2.203125</v>
-      </c>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="10">
-        <f t="shared" si="18"/>
-        <v>16.254531249999999</v>
-      </c>
-      <c r="AC19" s="10">
-        <f t="shared" si="18"/>
-        <v>26.314609375</v>
-      </c>
-    </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f t="shared" si="13"/>
-        <v>256</v>
-      </c>
-      <c r="U20" s="2">
-        <f t="shared" ref="U20:AC20" si="21">U11/$B11</f>
-        <v>14.918749999999999</v>
-      </c>
-      <c r="V20" s="2">
-        <f t="shared" ref="V20" si="22">V11/$B11</f>
-        <v>14.673515625</v>
-      </c>
-      <c r="W20" s="2">
-        <f t="shared" si="16"/>
-        <v>0.80859375</v>
-      </c>
-      <c r="X20" s="2">
-        <f t="shared" si="16"/>
-        <v>0.99609375</v>
-      </c>
-      <c r="Y20" s="2">
-        <f t="shared" ref="Y20:Z20" si="23">Y11/$B11</f>
-        <v>1.4609375</v>
-      </c>
-      <c r="Z20" s="2">
-        <f t="shared" si="23"/>
-        <v>1.86328125</v>
-      </c>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="10">
+        <v>16.20931640625</v>
+      </c>
+      <c r="AD21" s="10">
+        <f t="shared" si="17"/>
+        <v>28.66341796875</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f t="shared" si="4"/>
+        <v>1024</v>
+      </c>
+      <c r="U22" s="2">
+        <f t="shared" ref="U22:AD22" si="21">U13/$B13</f>
+        <v>18.761621093750001</v>
+      </c>
+      <c r="V22" s="2">
+        <f t="shared" ref="V22" si="22">V13/$B13</f>
+        <v>18.052275390624999</v>
+      </c>
+      <c r="W22" s="2">
+        <f t="shared" si="7"/>
+        <v>0.93359375</v>
+      </c>
+      <c r="X22" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1552734375</v>
+      </c>
+      <c r="Y22" s="2">
+        <f t="shared" ref="Y22" si="23">Y13/$B13</f>
+        <v>1.6875</v>
+      </c>
+      <c r="Z22" s="2">
+        <f t="shared" ref="Z22:AA22" si="24">Z13/$B13</f>
+        <v>1.6845703125</v>
+      </c>
+      <c r="AA22" s="2">
+        <f t="shared" si="24"/>
+        <v>2.14453125</v>
+      </c>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="10">
         <f t="shared" si="21"/>
-        <v>15.967812500000001</v>
-      </c>
-      <c r="AC20" s="10">
+        <v>16.788164062500002</v>
+      </c>
+      <c r="AD22" s="10">
         <f t="shared" si="21"/>
-        <v>27.311484374999999</v>
-      </c>
-    </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f t="shared" si="13"/>
-        <v>512</v>
-      </c>
-      <c r="U21" s="2">
-        <f t="shared" ref="U21:AC21" si="24">U12/$B12</f>
-        <v>16.835039062500002</v>
-      </c>
-      <c r="V21" s="2">
-        <f t="shared" ref="V21" si="25">V12/$B12</f>
-        <v>17.12515625</v>
-      </c>
-      <c r="W21" s="2">
-        <f t="shared" si="16"/>
-        <v>0.91796875</v>
-      </c>
-      <c r="X21" s="2">
-        <f t="shared" si="16"/>
-        <v>1.07421875</v>
-      </c>
-      <c r="Y21" s="2">
-        <f t="shared" ref="Y21:Z21" si="26">Y12/$B12</f>
-        <v>1.560546875</v>
-      </c>
-      <c r="Z21" s="2">
-        <f t="shared" si="26"/>
-        <v>2.484375</v>
-      </c>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="10">
-        <f t="shared" si="24"/>
-        <v>16.20931640625</v>
-      </c>
-      <c r="AC21" s="10">
-        <f t="shared" si="24"/>
-        <v>28.66341796875</v>
-      </c>
-    </row>
-    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <f t="shared" si="13"/>
-        <v>1024</v>
-      </c>
-      <c r="U22" s="2">
-        <f t="shared" ref="U22:AC22" si="27">U13/$B13</f>
-        <v>18.761621093750001</v>
-      </c>
-      <c r="V22" s="2">
-        <f t="shared" ref="V22" si="28">V13/$B13</f>
-        <v>18.052275390624999</v>
-      </c>
-      <c r="W22" s="2">
-        <f t="shared" si="16"/>
-        <v>0.93359375</v>
-      </c>
-      <c r="X22" s="2">
-        <f t="shared" si="16"/>
-        <v>1.1552734375</v>
-      </c>
-      <c r="Y22" s="2">
-        <f t="shared" ref="Y22:Z22" si="29">Y13/$B13</f>
-        <v>1.6845703125</v>
-      </c>
-      <c r="Z22" s="2">
-        <f t="shared" si="29"/>
-        <v>2.14453125</v>
-      </c>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="10">
-        <f t="shared" si="27"/>
-        <v>16.788164062500002</v>
-      </c>
-      <c r="AC22" s="10">
-        <f t="shared" si="27"/>
         <v>30.241464843749998</v>
       </c>
     </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="U23" s="2">
-        <f t="shared" ref="U23:AC23" si="30">U14/$B14</f>
+        <f t="shared" ref="U23:AD23" si="25">U14/$B14</f>
         <v>20.681201171874999</v>
       </c>
       <c r="V23" s="2">
-        <f t="shared" ref="V23" si="31">V14/$B14</f>
+        <f t="shared" ref="V23" si="26">V14/$B14</f>
         <v>20.560366210937499</v>
       </c>
       <c r="W23" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>1.04248046875</v>
       </c>
       <c r="X23" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>1.203125</v>
       </c>
       <c r="Y23" s="2">
-        <f t="shared" ref="Y23:Z23" si="32">Y14/$B14</f>
+        <f t="shared" ref="Y23" si="27">Y14/$B14</f>
+        <v>2.154296875</v>
+      </c>
+      <c r="Z23" s="2">
+        <f t="shared" ref="Z23:AA23" si="28">Z14/$B14</f>
         <v>1.771484375</v>
       </c>
-      <c r="Z23" s="2">
-        <f t="shared" si="32"/>
+      <c r="AA23" s="2">
+        <f t="shared" si="28"/>
         <v>2.7626953125</v>
       </c>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="10">
-        <f t="shared" si="30"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="10">
+        <f t="shared" si="25"/>
         <v>17.557260742187498</v>
       </c>
-      <c r="AC23" s="10">
-        <f t="shared" si="30"/>
+      <c r="AD23" s="10">
+        <f t="shared" si="25"/>
         <v>31.958188476562501</v>
       </c>
     </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
+      <c r="Y24" s="2" t="e">
+        <f t="shared" ref="Y24" si="29">Y15/$B15</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
-      <c r="AB24" s="10"/>
+      <c r="AB24" s="2"/>
       <c r="AC24" s="10"/>
-    </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y25" s="2"/>
+      <c r="AD24" s="10"/>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Z25" s="2"/>
-    </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y26" s="2"/>
-    </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y27" s="2"/>
-    </row>
-    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y28" s="2"/>
-    </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y29" s="2"/>
-    </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y30" s="2"/>
-    </row>
-    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y31" s="2"/>
-    </row>
-    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Y32" s="2"/>
+      <c r="AA25" s="2"/>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Z26" s="2"/>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Z28" s="2"/>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Z29" s="2"/>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Z30" s="2"/>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Z31" s="2"/>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="Z32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Benchmark: refactor again.  better FIR.
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -1776,7 +1776,7 @@
   <dimension ref="B2:AP32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,11 +1877,11 @@
         <v>Teensy 3.0</v>
       </c>
       <c r="AH2" t="str">
-        <f>U2</f>
+        <f t="shared" ref="AH2:AI6" si="0">U2</f>
         <v>Teensy 3.0</v>
       </c>
       <c r="AI2" t="str">
-        <f>V2</f>
+        <f t="shared" si="0"/>
         <v>Teensy 3.0</v>
       </c>
       <c r="AK2" t="str">
@@ -1893,11 +1893,11 @@
         <v>NXP K66</v>
       </c>
       <c r="AM2" t="str">
-        <f>W2</f>
+        <f t="shared" ref="AM2:AN6" si="1">W2</f>
         <v>NXP K66</v>
       </c>
       <c r="AN2" t="str">
-        <f>X2</f>
+        <f t="shared" si="1"/>
         <v>NXP K66</v>
       </c>
       <c r="AO2" t="str">
@@ -1905,7 +1905,7 @@
         <v>NXP K66</v>
       </c>
       <c r="AP2" t="str">
-        <f t="shared" ref="AP2:AP6" si="0">AA2</f>
+        <f t="shared" ref="AP2:AP6" si="2">AA2</f>
         <v>NXP K66</v>
       </c>
     </row>
@@ -1988,11 +1988,11 @@
         <v>96 MHz</v>
       </c>
       <c r="AH3" t="str">
-        <f>U3</f>
+        <f t="shared" si="0"/>
         <v>96 MHz</v>
       </c>
       <c r="AI3" t="str">
-        <f>V3</f>
+        <f t="shared" si="0"/>
         <v>96 MHz</v>
       </c>
       <c r="AK3" t="str">
@@ -2004,11 +2004,11 @@
         <v>120 MHz</v>
       </c>
       <c r="AM3" t="str">
-        <f>W3</f>
+        <f t="shared" si="1"/>
         <v>180 MHz</v>
       </c>
       <c r="AN3" t="str">
-        <f>X3</f>
+        <f t="shared" si="1"/>
         <v>180 MHz</v>
       </c>
       <c r="AO3" t="str">
@@ -2016,7 +2016,7 @@
         <v>120 MHz</v>
       </c>
       <c r="AP3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>120 MHz</v>
       </c>
     </row>
@@ -2099,11 +2099,11 @@
         <v>Int32</v>
       </c>
       <c r="AH4" t="str">
-        <f>U4</f>
+        <f t="shared" si="0"/>
         <v>Float</v>
       </c>
       <c r="AI4" t="str">
-        <f>V4</f>
+        <f t="shared" si="0"/>
         <v>All Float</v>
       </c>
       <c r="AK4" t="str">
@@ -2115,11 +2115,11 @@
         <v>Int32</v>
       </c>
       <c r="AM4" t="str">
-        <f>W4</f>
+        <f t="shared" si="1"/>
         <v>All Float</v>
       </c>
       <c r="AN4" t="str">
-        <f>X4</f>
+        <f t="shared" si="1"/>
         <v>All Float</v>
       </c>
       <c r="AO4" t="str">
@@ -2127,7 +2127,7 @@
         <v>All Float</v>
       </c>
       <c r="AP4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>All Float</v>
       </c>
     </row>
@@ -2210,11 +2210,11 @@
         <v>KissFFT</v>
       </c>
       <c r="AH5" t="str">
-        <f>U5</f>
+        <f t="shared" si="0"/>
         <v>cfft, radix 2</v>
       </c>
       <c r="AI5" t="str">
-        <f>V5</f>
+        <f t="shared" si="0"/>
         <v>KissFFT</v>
       </c>
       <c r="AK5" t="str">
@@ -2226,11 +2226,11 @@
         <v>KissFFT</v>
       </c>
       <c r="AM5" t="str">
-        <f>W5</f>
+        <f t="shared" si="1"/>
         <v>cfft, radix 4</v>
       </c>
       <c r="AN5" t="str">
-        <f>X5</f>
+        <f t="shared" si="1"/>
         <v>cfft, radix 2</v>
       </c>
       <c r="AO5" t="str">
@@ -2238,7 +2238,7 @@
         <v>cfft, radix 2</v>
       </c>
       <c r="AP5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>KissFFT</v>
       </c>
     </row>
@@ -2321,11 +2321,11 @@
         <v>Generic C</v>
       </c>
       <c r="AH6" t="str">
-        <f>U6</f>
+        <f t="shared" si="0"/>
         <v>ARM-Specific</v>
       </c>
       <c r="AI6" t="str">
-        <f>V6</f>
+        <f t="shared" si="0"/>
         <v>Generic C</v>
       </c>
       <c r="AK6" t="str">
@@ -2337,11 +2337,11 @@
         <v>Generic C</v>
       </c>
       <c r="AM6" t="str">
-        <f>W6</f>
+        <f t="shared" si="1"/>
         <v>ARM-Specific</v>
       </c>
       <c r="AN6" t="str">
-        <f>X6</f>
+        <f t="shared" si="1"/>
         <v>ARM-Specific</v>
       </c>
       <c r="AO6" t="str">
@@ -2349,7 +2349,7 @@
         <v>ARM-Specific</v>
       </c>
       <c r="AP6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Generic C</v>
       </c>
     </row>
@@ -2511,7 +2511,7 @@
         <v>25</v>
       </c>
       <c r="Y8" s="12">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Z8" s="12">
         <v>37</v>
@@ -2526,36 +2526,36 @@
         <v>846.76</v>
       </c>
       <c r="AF8" s="11">
-        <f>K8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AF8:AF14" si="3">K8*0.000001/($B8/44100)</f>
         <v>7.4584124999999987E-2</v>
       </c>
       <c r="AG8" s="11">
-        <f>R8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AG8:AG14" si="4">R8*0.000001/($B8/44100)</f>
         <v>0.56507259374999996</v>
       </c>
       <c r="AH8" s="11">
-        <f>U8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AH8:AI14" si="5">U8*0.000001/($B8/44100)</f>
         <v>0.40890346874999989</v>
       </c>
       <c r="AI8" s="11">
-        <f>V8*0.000001/($B8/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.46638506249999995</v>
       </c>
       <c r="AJ8" s="11"/>
       <c r="AK8" s="11">
-        <f>M8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AK8:AK14" si="6">M8*0.000001/($B8/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
       <c r="AL8" s="11">
-        <f>S8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AL8:AL14" si="7">S8*0.000001/($B8/44100)</f>
         <v>0.17502187499999999</v>
       </c>
       <c r="AM8" s="11">
-        <f>W8*0.000001/($B8/44100)</f>
+        <f t="shared" ref="AM8:AN14" si="8">W8*0.000001/($B8/44100)</f>
         <v>3.5831249999999995E-2</v>
       </c>
       <c r="AN8" s="11">
-        <f>X8*0.000001/($B8/44100)</f>
+        <f t="shared" si="8"/>
         <v>3.4453124999999994E-2</v>
       </c>
       <c r="AO8" s="11">
@@ -2621,7 +2621,7 @@
         <v>55</v>
       </c>
       <c r="Y9" s="12">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Z9" s="12">
         <v>79</v>
@@ -2636,44 +2636,44 @@
         <v>1662.88</v>
       </c>
       <c r="AF9" s="11">
-        <f>K9*0.000001/($B9/44100)</f>
+        <f t="shared" si="3"/>
         <v>8.4051843749999994E-2</v>
       </c>
       <c r="AG9" s="11">
-        <f>R9*0.000001/($B9/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.58870743749999999</v>
       </c>
       <c r="AH9" s="11">
-        <f>U9*0.000001/($B9/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.49070207812499994</v>
       </c>
       <c r="AI9" s="11">
-        <f>V9*0.000001/($B9/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.49942560937499991</v>
       </c>
       <c r="AJ9" s="11"/>
       <c r="AK9" s="11">
-        <f>M9*0.000001/($B9/44100)</f>
+        <f t="shared" si="6"/>
         <v>7.8553124999999988E-2</v>
       </c>
       <c r="AL9" s="11">
-        <f>S9*0.000001/($B9/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.16399687499999999</v>
       </c>
       <c r="AM9" s="11">
-        <f>W9*0.000001/($B9/44100)</f>
+        <f t="shared" si="8"/>
         <v>3.1696874999999999E-2</v>
       </c>
       <c r="AN9" s="11">
-        <f>X9*0.000001/($B9/44100)</f>
+        <f t="shared" si="8"/>
         <v>3.7898437499999993E-2</v>
       </c>
       <c r="AO9" s="11">
-        <f>Z9*0.000001/($B9/44100)</f>
+        <f t="shared" ref="AO9:AO14" si="9">Z9*0.000001/($B9/44100)</f>
         <v>5.4435937499999996E-2</v>
       </c>
       <c r="AP9" s="11">
-        <f t="shared" ref="AP9:AP14" si="1">AA9*0.000001/($B9/44100)</f>
+        <f t="shared" ref="AP9:AP14" si="10">AA9*0.000001/($B9/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
         <v>118</v>
       </c>
       <c r="Y10" s="12">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="Z10" s="12">
         <v>173</v>
@@ -2746,44 +2746,44 @@
         <v>3368.27</v>
       </c>
       <c r="AF10" s="11">
-        <f>K10*0.000001/($B10/44100)</f>
+        <f t="shared" si="3"/>
         <v>9.4436015624999994E-2</v>
       </c>
       <c r="AG10" s="11">
-        <f>R10*0.000001/($B10/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.68300564062499991</v>
       </c>
       <c r="AH10" s="11">
-        <f>U10*0.000001/($B10/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.57363419531250004</v>
       </c>
       <c r="AI10" s="11">
-        <f>V10*0.000001/($B10/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.60612693749999991</v>
       </c>
       <c r="AJ10" s="11"/>
       <c r="AK10" s="11">
-        <f>M10*0.000001/($B10/44100)</f>
+        <f t="shared" si="6"/>
         <v>8.7510937499999997E-2</v>
       </c>
       <c r="AL10" s="11">
-        <f>S10*0.000001/($B10/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.21774374999999999</v>
       </c>
       <c r="AM10" s="11">
-        <f>W10*0.000001/($B10/44100)</f>
+        <f t="shared" si="8"/>
         <v>3.6864843750000001E-2</v>
       </c>
       <c r="AN10" s="11">
-        <f>X10*0.000001/($B10/44100)</f>
+        <f t="shared" si="8"/>
         <v>4.0654687499999995E-2</v>
       </c>
       <c r="AO10" s="11">
-        <f>Z10*0.000001/($B10/44100)</f>
+        <f t="shared" si="9"/>
         <v>5.9603906249999998E-2</v>
       </c>
       <c r="AP10" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>9.7157812499999982E-2</v>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
         <v>255</v>
       </c>
       <c r="Y11" s="12">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="Z11" s="12">
         <v>374</v>
@@ -2856,44 +2856,44 @@
         <v>6991.74</v>
       </c>
       <c r="AF11" s="11">
-        <f>K11*0.000001/($B11/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.10584344531249999</v>
       </c>
       <c r="AG11" s="11">
-        <f>R11*0.000001/($B11/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.72309185156249989</v>
       </c>
       <c r="AH11" s="11">
-        <f>U11*0.000001/($B11/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.65791687499999996</v>
       </c>
       <c r="AI11" s="11">
-        <f>V11*0.000001/($B11/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.64710203906249997</v>
       </c>
       <c r="AJ11" s="11"/>
       <c r="AK11" s="11">
-        <f>M11*0.000001/($B11/44100)</f>
+        <f t="shared" si="6"/>
         <v>9.7502343749999998E-2</v>
       </c>
       <c r="AL11" s="11">
-        <f>S11*0.000001/($B11/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.20654648437500001</v>
       </c>
       <c r="AM11" s="11">
-        <f>W11*0.000001/($B11/44100)</f>
+        <f t="shared" si="8"/>
         <v>3.5658984375000001E-2</v>
       </c>
       <c r="AN11" s="11">
-        <f>X11*0.000001/($B11/44100)</f>
+        <f t="shared" si="8"/>
         <v>4.3927734374999992E-2</v>
       </c>
       <c r="AO11" s="11">
-        <f>Z11*0.000001/($B11/44100)</f>
+        <f t="shared" si="9"/>
         <v>6.4427343749999991E-2</v>
       </c>
       <c r="AP11" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>8.2170703124999994E-2</v>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
         <v>550</v>
       </c>
       <c r="Y12" s="12">
-        <v>990</v>
+        <v>946</v>
       </c>
       <c r="Z12" s="12">
         <v>799</v>
@@ -2966,44 +2966,44 @@
         <v>14675.67</v>
       </c>
       <c r="AF12" s="11">
-        <f>K12*0.000001/($B12/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.11730427734375</v>
       </c>
       <c r="AG12" s="11">
-        <f>R12*0.000001/($B12/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.82538317968749997</v>
       </c>
       <c r="AH12" s="11">
-        <f>U12*0.000001/($B12/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.74242522265624999</v>
       </c>
       <c r="AI12" s="11">
-        <f>V12*0.000001/($B12/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.75521939062499988</v>
       </c>
       <c r="AJ12" s="11"/>
       <c r="AK12" s="11">
-        <f>M12*0.000001/($B12/44100)</f>
+        <f t="shared" si="6"/>
         <v>0.1070630859375</v>
       </c>
       <c r="AL12" s="11">
-        <f>S12*0.000001/($B12/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.26106855468749995</v>
       </c>
       <c r="AM12" s="11">
-        <f>W12*0.000001/($B12/44100)</f>
+        <f t="shared" si="8"/>
         <v>4.0482421875000001E-2</v>
       </c>
       <c r="AN12" s="11">
-        <f>X12*0.000001/($B12/44100)</f>
+        <f t="shared" si="8"/>
         <v>4.7373046874999991E-2</v>
       </c>
       <c r="AO12" s="11">
-        <f>Z12*0.000001/($B12/44100)</f>
+        <f t="shared" si="9"/>
         <v>6.8820117187500002E-2</v>
       </c>
       <c r="AP12" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0.1095609375</v>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
         <v>1183</v>
       </c>
       <c r="Y13" s="12">
-        <v>1728</v>
+        <v>1644</v>
       </c>
       <c r="Z13" s="12">
         <v>1725</v>
@@ -3085,44 +3085,44 @@
         <v>30967.26</v>
       </c>
       <c r="AF13" s="11">
-        <f>K13*0.000001/($B13/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.12962816015625001</v>
       </c>
       <c r="AG13" s="11">
-        <f>R13*0.000001/($B13/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.86949609960937491</v>
       </c>
       <c r="AH13" s="11">
-        <f>U13*0.000001/($B13/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.82738749023437497</v>
       </c>
       <c r="AI13" s="11">
-        <f>V13*0.000001/($B13/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.79610534472656236</v>
       </c>
       <c r="AJ13" s="11"/>
       <c r="AK13" s="11">
-        <f>M13*0.000001/($B13/44100)</f>
+        <f t="shared" si="6"/>
         <v>5.3531542968749998E-2</v>
       </c>
       <c r="AL13" s="11">
-        <f>S13*0.000001/($B13/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.24982822265624999</v>
       </c>
       <c r="AM13" s="11">
-        <f>W13*0.000001/($B13/44100)</f>
+        <f t="shared" si="8"/>
         <v>4.1171484374999998E-2</v>
       </c>
       <c r="AN13" s="11">
-        <f>X13*0.000001/($B13/44100)</f>
+        <f t="shared" si="8"/>
         <v>5.0947558593749998E-2</v>
       </c>
       <c r="AO13" s="11">
-        <f>Z13*0.000001/($B13/44100)</f>
+        <f t="shared" si="9"/>
         <v>7.4289550781249991E-2</v>
       </c>
       <c r="AP13" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>9.4573828124999995E-2</v>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
         <v>2464</v>
       </c>
       <c r="Y14" s="12">
-        <v>4412</v>
+        <v>4198</v>
       </c>
       <c r="Z14" s="12">
         <v>3628</v>
@@ -3192,44 +3192,44 @@
         <v>65450.37</v>
       </c>
       <c r="AF14" s="11">
-        <f>K14*0.000001/($B14/44100)</f>
+        <f t="shared" si="3"/>
         <v>0.14165768408203125</v>
       </c>
       <c r="AG14" s="11">
-        <f>R14*0.000001/($B14/44100)</f>
+        <f t="shared" si="4"/>
         <v>0.97373402929687503</v>
       </c>
       <c r="AH14" s="11">
-        <f>U14*0.000001/($B14/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.91204097167968745</v>
       </c>
       <c r="AI14" s="11">
-        <f>V14*0.000001/($B14/44100)</f>
+        <f t="shared" si="5"/>
         <v>0.90671214990234361</v>
       </c>
       <c r="AJ14" s="11"/>
       <c r="AK14" s="11">
-        <f>M14*0.000001/($B14/44100)</f>
+        <f t="shared" si="6"/>
         <v>0.12648603515624998</v>
       </c>
       <c r="AL14" s="11">
-        <f>S14*0.000001/($B14/44100)</f>
+        <f t="shared" si="7"/>
         <v>0.30432875976562501</v>
       </c>
       <c r="AM14" s="11">
-        <f>W14*0.000001/($B14/44100)</f>
+        <f t="shared" si="8"/>
         <v>4.597338867187499E-2</v>
       </c>
       <c r="AN14" s="11">
-        <f>X14*0.000001/($B14/44100)</f>
+        <f t="shared" si="8"/>
         <v>5.3057812500000003E-2</v>
       </c>
       <c r="AO14" s="11">
-        <f>Z14*0.000001/($B14/44100)</f>
+        <f t="shared" si="9"/>
         <v>7.8122460937499999E-2</v>
       </c>
       <c r="AP14" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0.12183486328125</v>
       </c>
     </row>
@@ -3247,295 +3247,295 @@
         <v>32</v>
       </c>
       <c r="U17" s="2">
-        <f t="shared" ref="U17:AA17" si="2">U8/$B8</f>
+        <f t="shared" ref="U17:AA17" si="11">U8/$B8</f>
         <v>9.2721874999999994</v>
       </c>
       <c r="V17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>10.575625</v>
       </c>
       <c r="W17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.8125</v>
       </c>
       <c r="X17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.78125</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>1.15625</v>
       </c>
       <c r="AA17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>1.9375</v>
       </c>
       <c r="AB17" s="2"/>
       <c r="AC17" s="10">
-        <f t="shared" ref="AC17:AD17" si="3">AC8/$B8</f>
+        <f t="shared" ref="AC17:AD17" si="12">AC8/$B8</f>
         <v>20.468125000000001</v>
       </c>
       <c r="AD17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>26.46125</v>
       </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f t="shared" ref="B18:B23" si="4">B9</f>
+        <f t="shared" ref="B18:B23" si="13">B9</f>
         <v>64</v>
       </c>
       <c r="U18" s="2">
-        <f t="shared" ref="U18:AD18" si="5">U9/$B9</f>
+        <f t="shared" ref="U18:AD18" si="14">U9/$B9</f>
         <v>11.12703125</v>
       </c>
       <c r="V18" s="2">
-        <f t="shared" ref="V18" si="6">V9/$B9</f>
+        <f t="shared" ref="V18" si="15">V9/$B9</f>
         <v>11.324843749999999</v>
       </c>
       <c r="W18" s="2">
-        <f t="shared" ref="W18:Y23" si="7">W9/$B9</f>
+        <f t="shared" ref="W18:Y23" si="16">W9/$B9</f>
         <v>0.71875</v>
       </c>
       <c r="X18" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.859375</v>
       </c>
       <c r="Y18" s="2">
-        <f t="shared" si="7"/>
-        <v>1.25</v>
+        <f t="shared" si="16"/>
+        <v>1.203125</v>
       </c>
       <c r="Z18" s="2">
-        <f t="shared" ref="Z18:AA18" si="8">Z9/$B9</f>
+        <f t="shared" ref="Z18:AA18" si="17">Z9/$B9</f>
         <v>1.234375</v>
       </c>
       <c r="AA18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.59375</v>
       </c>
       <c r="AB18" s="2"/>
       <c r="AC18" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>17.533281250000002</v>
       </c>
       <c r="AD18" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>25.982500000000002</v>
       </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>128</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" ref="U19:AD19" si="9">U10/$B10</f>
+        <f t="shared" ref="U19:AD19" si="18">U10/$B10</f>
         <v>13.007578125</v>
       </c>
       <c r="V19" s="2">
-        <f t="shared" ref="V19" si="10">V10/$B10</f>
+        <f t="shared" ref="V19" si="19">V10/$B10</f>
         <v>13.744375</v>
       </c>
       <c r="W19" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.8359375</v>
       </c>
       <c r="X19" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.921875</v>
       </c>
       <c r="Y19" s="2">
-        <f t="shared" ref="Y19" si="11">Y10/$B10</f>
-        <v>1.71875</v>
+        <f t="shared" ref="Y19" si="20">Y10/$B10</f>
+        <v>1.640625</v>
       </c>
       <c r="Z19" s="2">
-        <f t="shared" ref="Z19:AA19" si="12">Z10/$B10</f>
+        <f t="shared" ref="Z19:AA19" si="21">Z10/$B10</f>
         <v>1.3515625</v>
       </c>
       <c r="AA19" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>2.203125</v>
       </c>
       <c r="AB19" s="2"/>
       <c r="AC19" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>16.254531249999999</v>
       </c>
       <c r="AD19" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>26.314609375</v>
       </c>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>256</v>
       </c>
       <c r="U20" s="2">
-        <f t="shared" ref="U20:AD20" si="13">U11/$B11</f>
+        <f t="shared" ref="U20:AD20" si="22">U11/$B11</f>
         <v>14.918749999999999</v>
       </c>
       <c r="V20" s="2">
-        <f t="shared" ref="V20" si="14">V11/$B11</f>
+        <f t="shared" ref="V20" si="23">V11/$B11</f>
         <v>14.673515625</v>
       </c>
       <c r="W20" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.80859375</v>
       </c>
       <c r="X20" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.99609375</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" ref="Y20" si="15">Y11/$B11</f>
-        <v>1.46484375</v>
+        <f t="shared" ref="Y20" si="24">Y11/$B11</f>
+        <v>1.40625</v>
       </c>
       <c r="Z20" s="2">
-        <f t="shared" ref="Z20:AA20" si="16">Z11/$B11</f>
+        <f t="shared" ref="Z20:AA20" si="25">Z11/$B11</f>
         <v>1.4609375</v>
       </c>
       <c r="AA20" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>1.86328125</v>
       </c>
       <c r="AB20" s="2"/>
       <c r="AC20" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>15.967812500000001</v>
       </c>
       <c r="AD20" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>27.311484374999999</v>
       </c>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>512</v>
       </c>
       <c r="U21" s="2">
-        <f t="shared" ref="U21:AD21" si="17">U12/$B12</f>
+        <f t="shared" ref="U21:AD21" si="26">U12/$B12</f>
         <v>16.835039062500002</v>
       </c>
       <c r="V21" s="2">
-        <f t="shared" ref="V21" si="18">V12/$B12</f>
+        <f t="shared" ref="V21" si="27">V12/$B12</f>
         <v>17.12515625</v>
       </c>
       <c r="W21" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.91796875</v>
       </c>
       <c r="X21" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.07421875</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" ref="Y21" si="19">Y12/$B12</f>
-        <v>1.93359375</v>
+        <f t="shared" ref="Y21" si="28">Y12/$B12</f>
+        <v>1.84765625</v>
       </c>
       <c r="Z21" s="2">
-        <f t="shared" ref="Z21:AA21" si="20">Z12/$B12</f>
+        <f t="shared" ref="Z21:AA21" si="29">Z12/$B12</f>
         <v>1.560546875</v>
       </c>
       <c r="AA21" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>2.484375</v>
       </c>
       <c r="AB21" s="2"/>
       <c r="AC21" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>16.20931640625</v>
       </c>
       <c r="AD21" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>28.66341796875</v>
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1024</v>
       </c>
       <c r="U22" s="2">
-        <f t="shared" ref="U22:AD22" si="21">U13/$B13</f>
+        <f t="shared" ref="U22:AD22" si="30">U13/$B13</f>
         <v>18.761621093750001</v>
       </c>
       <c r="V22" s="2">
-        <f t="shared" ref="V22" si="22">V13/$B13</f>
+        <f t="shared" ref="V22" si="31">V13/$B13</f>
         <v>18.052275390624999</v>
       </c>
       <c r="W22" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.93359375</v>
       </c>
       <c r="X22" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.1552734375</v>
       </c>
       <c r="Y22" s="2">
-        <f t="shared" ref="Y22" si="23">Y13/$B13</f>
-        <v>1.6875</v>
+        <f t="shared" ref="Y22" si="32">Y13/$B13</f>
+        <v>1.60546875</v>
       </c>
       <c r="Z22" s="2">
-        <f t="shared" ref="Z22:AA22" si="24">Z13/$B13</f>
+        <f t="shared" ref="Z22:AA22" si="33">Z13/$B13</f>
         <v>1.6845703125</v>
       </c>
       <c r="AA22" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="33"/>
         <v>2.14453125</v>
       </c>
       <c r="AB22" s="2"/>
       <c r="AC22" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>16.788164062500002</v>
       </c>
       <c r="AD22" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>30.241464843749998</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>2048</v>
       </c>
       <c r="U23" s="2">
-        <f t="shared" ref="U23:AD23" si="25">U14/$B14</f>
+        <f t="shared" ref="U23:AD23" si="34">U14/$B14</f>
         <v>20.681201171874999</v>
       </c>
       <c r="V23" s="2">
-        <f t="shared" ref="V23" si="26">V14/$B14</f>
+        <f t="shared" ref="V23" si="35">V14/$B14</f>
         <v>20.560366210937499</v>
       </c>
       <c r="W23" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.04248046875</v>
       </c>
       <c r="X23" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>1.203125</v>
       </c>
       <c r="Y23" s="2">
-        <f t="shared" ref="Y23" si="27">Y14/$B14</f>
-        <v>2.154296875</v>
+        <f t="shared" ref="Y23" si="36">Y14/$B14</f>
+        <v>2.0498046875</v>
       </c>
       <c r="Z23" s="2">
-        <f t="shared" ref="Z23:AA23" si="28">Z14/$B14</f>
+        <f t="shared" ref="Z23:AA23" si="37">Z14/$B14</f>
         <v>1.771484375</v>
       </c>
       <c r="AA23" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="37"/>
         <v>2.7626953125</v>
       </c>
       <c r="AB23" s="2"/>
       <c r="AC23" s="10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>17.557260742187498</v>
       </c>
       <c r="AD23" s="10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>31.958188476562501</v>
       </c>
     </row>
@@ -3545,7 +3545,7 @@
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2" t="e">
-        <f t="shared" ref="Y24" si="29">Y15/$B15</f>
+        <f t="shared" ref="Y24" si="38">Y15/$B15</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Z24" s="2"/>

</xml_diff>

<commit_message>
Benchmark: refactor for Arduino
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="49">
   <si>
     <t>N</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>cfft, radix 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino Uno </t>
+  </si>
+  <si>
+    <t>16 MHz</t>
+  </si>
+  <si>
+    <t>Int 16</t>
   </si>
 </sst>
 </file>
@@ -1773,88 +1782,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AP32"/>
+  <dimension ref="B2:AS32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="2.42578125" customWidth="1"/>
-    <col min="6" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="11" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="2" customWidth="1"/>
-    <col min="18" max="19" width="10.85546875" customWidth="1"/>
-    <col min="20" max="20" width="2.5703125" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="11.42578125" customWidth="1"/>
-    <col min="28" max="28" width="3.5703125" customWidth="1"/>
-    <col min="29" max="29" width="11.28515625" style="9" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" style="9" customWidth="1"/>
-    <col min="36" max="36" width="2.140625" customWidth="1"/>
+    <col min="4" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="19" width="2" customWidth="1"/>
+    <col min="20" max="21" width="10.85546875" customWidth="1"/>
+    <col min="22" max="22" width="2.5703125" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="11.42578125" customWidth="1"/>
+    <col min="31" max="31" width="3.5703125" customWidth="1"/>
+    <col min="32" max="32" width="11.28515625" style="9" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" style="9" customWidth="1"/>
+    <col min="39" max="39" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="U2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="W2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="Y2" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="Z2" s="12" t="s">
         <v>41</v>
@@ -1862,220 +1873,238 @@
       <c r="AA2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AB2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AG2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" t="str">
-        <f>K2</f>
+      <c r="AI2" t="str">
+        <f>M2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AG2" t="str">
-        <f>R2</f>
+      <c r="AJ2" t="str">
+        <f>T2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AH2" t="str">
-        <f t="shared" ref="AH2:AI6" si="0">U2</f>
+      <c r="AK2" t="str">
+        <f t="shared" ref="AK2:AL6" si="0">X2</f>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AI2" t="str">
+      <c r="AL2" t="str">
         <f t="shared" si="0"/>
         <v>Teensy 3.0</v>
       </c>
-      <c r="AK2" t="str">
-        <f>M2</f>
+      <c r="AN2" t="str">
+        <f>O2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AL2" t="str">
-        <f>S2</f>
+      <c r="AO2" t="str">
+        <f>U2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AM2" t="str">
-        <f t="shared" ref="AM2:AN6" si="1">W2</f>
+      <c r="AP2" t="str">
+        <f t="shared" ref="AP2:AQ6" si="1">Z2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AN2" t="str">
+      <c r="AQ2" t="str">
         <f t="shared" si="1"/>
         <v>NXP K66</v>
       </c>
-      <c r="AO2" t="str">
-        <f>Z2</f>
+      <c r="AR2" t="str">
+        <f>AC2</f>
         <v>NXP K66</v>
       </c>
-      <c r="AP2" t="str">
-        <f t="shared" ref="AP2:AP6" si="2">AA2</f>
+      <c r="AS2" t="str">
+        <f t="shared" ref="AS2:AS6" si="2">AD2</f>
         <v>NXP K66</v>
       </c>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>10</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>36</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="T3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="U3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="W3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="Y3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="14" t="s">
+      <c r="Z3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="AA3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="AB3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="AC3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AD3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AF3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AD3" s="9" t="s">
+      <c r="AG3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AF3" t="str">
-        <f>K3</f>
+      <c r="AI3" t="str">
+        <f>M3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AG3" t="str">
-        <f>R3</f>
+      <c r="AJ3" t="str">
+        <f>T3</f>
         <v>96 MHz</v>
       </c>
-      <c r="AH3" t="str">
+      <c r="AK3" t="str">
         <f t="shared" si="0"/>
         <v>96 MHz</v>
       </c>
-      <c r="AI3" t="str">
+      <c r="AL3" t="str">
         <f t="shared" si="0"/>
         <v>96 MHz</v>
       </c>
-      <c r="AK3" t="str">
-        <f>M3</f>
+      <c r="AN3" t="str">
+        <f>O3</f>
         <v>120 MHz</v>
       </c>
-      <c r="AL3" t="str">
-        <f>S3</f>
+      <c r="AO3" t="str">
+        <f>U3</f>
         <v>120 MHz</v>
       </c>
-      <c r="AM3" t="str">
+      <c r="AP3" t="str">
         <f t="shared" si="1"/>
         <v>180 MHz</v>
       </c>
-      <c r="AN3" t="str">
+      <c r="AQ3" t="str">
         <f t="shared" si="1"/>
         <v>180 MHz</v>
       </c>
-      <c r="AO3" t="str">
-        <f>Z3</f>
+      <c r="AR3" t="str">
+        <f>AC3</f>
         <v>120 MHz</v>
       </c>
-      <c r="AP3" t="str">
+      <c r="AS3" t="str">
         <f t="shared" si="2"/>
         <v>120 MHz</v>
       </c>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="N4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="N4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" t="s">
-        <v>40</v>
       </c>
       <c r="P4" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="Q4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="U4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="W4" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="W4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="X4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y4" s="12" t="s">
+      <c r="X4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="13" t="s">
         <v>29</v>
       </c>
       <c r="Z4" s="12" t="s">
@@ -2084,276 +2113,303 @@
       <c r="AA4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AC4" s="9" t="s">
+      <c r="AB4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" s="9" t="s">
+      <c r="AC4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AF4" t="str">
-        <f>K4</f>
+      <c r="AI4" t="str">
+        <f>M4</f>
         <v>Int32</v>
       </c>
-      <c r="AG4" t="str">
-        <f>R4</f>
+      <c r="AJ4" t="str">
+        <f>T4</f>
         <v>Int32</v>
       </c>
-      <c r="AH4" t="str">
+      <c r="AK4" t="str">
         <f t="shared" si="0"/>
         <v>Float</v>
       </c>
-      <c r="AI4" t="str">
+      <c r="AL4" t="str">
         <f t="shared" si="0"/>
         <v>All Float</v>
       </c>
-      <c r="AK4" t="str">
-        <f>M4</f>
+      <c r="AN4" t="str">
+        <f>O4</f>
         <v>Int32</v>
       </c>
-      <c r="AL4" t="str">
-        <f>S4</f>
+      <c r="AO4" t="str">
+        <f>U4</f>
         <v>Int32</v>
       </c>
-      <c r="AM4" t="str">
+      <c r="AP4" t="str">
         <f t="shared" si="1"/>
         <v>All Float</v>
       </c>
-      <c r="AN4" t="str">
+      <c r="AQ4" t="str">
         <f t="shared" si="1"/>
         <v>All Float</v>
       </c>
-      <c r="AO4" t="str">
-        <f>Z4</f>
+      <c r="AR4" t="str">
+        <f>AC4</f>
         <v>All Float</v>
       </c>
-      <c r="AP4" t="str">
+      <c r="AS4" t="str">
         <f t="shared" si="2"/>
         <v>All Float</v>
       </c>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
       </c>
       <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="N5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="O5" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="N5" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" t="s">
-        <v>39</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="Q5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="U5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="W5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="Y5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="W5" s="14" t="s">
+      <c r="Z5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="AA5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="Y5" s="12" t="s">
+      <c r="AB5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="AC5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="12" t="s">
+      <c r="AD5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AF5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AG5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AF5" t="str">
-        <f>K5</f>
+      <c r="AI5" t="str">
+        <f>M5</f>
         <v>cfft, radix 2</v>
       </c>
-      <c r="AG5" t="str">
-        <f>R5</f>
+      <c r="AJ5" t="str">
+        <f>T5</f>
         <v>KissFFT</v>
       </c>
-      <c r="AH5" t="str">
+      <c r="AK5" t="str">
         <f t="shared" si="0"/>
         <v>cfft, radix 2</v>
       </c>
-      <c r="AI5" t="str">
+      <c r="AL5" t="str">
         <f t="shared" si="0"/>
         <v>KissFFT</v>
       </c>
-      <c r="AK5" t="str">
-        <f>M5</f>
+      <c r="AN5" t="str">
+        <f>O5</f>
         <v>cfft, radix 2</v>
       </c>
-      <c r="AL5" t="str">
-        <f>S5</f>
+      <c r="AO5" t="str">
+        <f>U5</f>
         <v>KissFFT</v>
       </c>
-      <c r="AM5" t="str">
+      <c r="AP5" t="str">
         <f t="shared" si="1"/>
         <v>cfft, radix 4</v>
       </c>
-      <c r="AN5" t="str">
+      <c r="AQ5" t="str">
         <f t="shared" si="1"/>
         <v>cfft, radix 2</v>
       </c>
-      <c r="AO5" t="str">
-        <f>Z5</f>
+      <c r="AR5" t="str">
+        <f>AC5</f>
         <v>cfft, radix 2</v>
       </c>
-      <c r="AP5" t="str">
+      <c r="AS5" t="str">
         <f t="shared" si="2"/>
         <v>KissFFT</v>
       </c>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="N6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="O6" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="N6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" t="s">
-        <v>25</v>
       </c>
       <c r="P6" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="Q6" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="R6" t="s">
         <v>25</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="T6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="W6" t="s">
+        <v>25</v>
+      </c>
+      <c r="X6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="V6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="X6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y6" s="12" t="s">
+      <c r="Y6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="Z6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="AA6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AC6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AD6" s="9" t="s">
+      <c r="AF6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AF6" t="str">
-        <f>K6</f>
+      <c r="AG6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI6" t="str">
+        <f>M6</f>
         <v>ARM-Specific</v>
       </c>
-      <c r="AG6" t="str">
-        <f>R6</f>
+      <c r="AJ6" t="str">
+        <f>T6</f>
         <v>Generic C</v>
       </c>
-      <c r="AH6" t="str">
+      <c r="AK6" t="str">
         <f t="shared" si="0"/>
         <v>ARM-Specific</v>
       </c>
-      <c r="AI6" t="str">
+      <c r="AL6" t="str">
         <f t="shared" si="0"/>
         <v>Generic C</v>
       </c>
-      <c r="AK6" t="str">
-        <f>M6</f>
+      <c r="AN6" t="str">
+        <f>O6</f>
         <v>ARM-Specific</v>
       </c>
-      <c r="AL6" t="str">
-        <f>S6</f>
+      <c r="AO6" t="str">
+        <f>U6</f>
         <v>Generic C</v>
       </c>
-      <c r="AM6" t="str">
+      <c r="AP6" t="str">
         <f t="shared" si="1"/>
         <v>ARM-Specific</v>
       </c>
-      <c r="AN6" t="str">
+      <c r="AQ6" t="str">
         <f t="shared" si="1"/>
         <v>ARM-Specific</v>
       </c>
-      <c r="AO6" t="str">
-        <f>Z6</f>
+      <c r="AR6" t="str">
+        <f>AC6</f>
         <v>ARM-Specific</v>
       </c>
-      <c r="AP6" t="str">
+      <c r="AS6" t="str">
         <f t="shared" si="2"/>
         <v>Generic C</v>
       </c>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2419,7 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>4</v>
       </c>
       <c r="G7" t="s">
@@ -2375,43 +2431,43 @@
       <c r="I7" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="P7" t="s">
         <v>4</v>
       </c>
-      <c r="R7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="U7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="V7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="W7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="X7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y7" s="12" t="s">
+      <c r="Q7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="13" t="s">
         <v>4</v>
       </c>
       <c r="Z7" s="12" t="s">
@@ -2420,33 +2476,33 @@
       <c r="AA7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AC7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>42</v>
+      <c r="AB7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG7" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="AI7" t="s">
         <v>42</v>
       </c>
+      <c r="AJ7" t="s">
+        <v>42</v>
+      </c>
       <c r="AK7" t="s">
         <v>42</v>
       </c>
       <c r="AL7" t="s">
         <v>42</v>
       </c>
-      <c r="AM7" t="s">
-        <v>42</v>
-      </c>
       <c r="AN7" t="s">
         <v>42</v>
       </c>
@@ -2456,1128 +2512,1149 @@
       <c r="AP7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="AQ7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>32</v>
       </c>
       <c r="C8">
+        <v>4980.8</v>
+      </c>
+      <c r="D8">
         <f>'ARM-Specific Functions'!E10</f>
         <v>31.61</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>702.67</v>
       </c>
-      <c r="F8">
+      <c r="G8">
+        <v>12559.2</v>
+      </c>
+      <c r="H8">
         <f>'ARM-Specific Functions'!H10</f>
         <v>54.12</v>
       </c>
-      <c r="K8" s="13">
+      <c r="M8" s="13">
         <f>'ARM-Specific Functions'!H10</f>
         <v>54.12</v>
       </c>
-      <c r="L8" s="12">
+      <c r="N8" s="12">
         <v>35</v>
       </c>
-      <c r="M8" s="12">
+      <c r="O8" s="12">
         <v>51</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>74.41</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>144.16</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>262.33999999999997</v>
       </c>
-      <c r="R8" s="13">
+      <c r="T8" s="13">
         <v>410.03</v>
       </c>
-      <c r="S8" s="12">
+      <c r="U8" s="12">
         <v>127</v>
       </c>
-      <c r="U8" s="13">
+      <c r="W8">
+        <v>6378</v>
+      </c>
+      <c r="X8" s="13">
         <f>'ARM-Specific Functions'!K10</f>
         <v>296.70999999999998</v>
       </c>
-      <c r="V8" s="13">
+      <c r="Y8" s="13">
         <v>338.42</v>
       </c>
-      <c r="W8" s="12">
+      <c r="Z8" s="12">
         <v>26</v>
       </c>
-      <c r="X8" s="12">
+      <c r="AA8" s="12">
         <v>25</v>
       </c>
-      <c r="Y8" s="12">
+      <c r="AB8" s="12">
         <v>46</v>
       </c>
-      <c r="Z8" s="12">
+      <c r="AC8" s="12">
         <v>37</v>
       </c>
-      <c r="AA8" s="12">
+      <c r="AD8" s="12">
         <v>62</v>
       </c>
-      <c r="AC8" s="9">
+      <c r="AF8" s="9">
         <v>654.98</v>
       </c>
-      <c r="AD8" s="9">
+      <c r="AG8" s="9">
         <v>846.76</v>
       </c>
-      <c r="AF8" s="11">
-        <f t="shared" ref="AF8:AF14" si="3">K8*0.000001/($B8/44100)</f>
+      <c r="AI8" s="11">
+        <f t="shared" ref="AI8:AI14" si="3">M8*0.000001/($B8/44100)</f>
         <v>7.4584124999999987E-2</v>
       </c>
-      <c r="AG8" s="11">
-        <f t="shared" ref="AG8:AG14" si="4">R8*0.000001/($B8/44100)</f>
+      <c r="AJ8" s="11">
+        <f t="shared" ref="AJ8:AJ14" si="4">T8*0.000001/($B8/44100)</f>
         <v>0.56507259374999996</v>
       </c>
-      <c r="AH8" s="11">
-        <f t="shared" ref="AH8:AI14" si="5">U8*0.000001/($B8/44100)</f>
+      <c r="AK8" s="11">
+        <f t="shared" ref="AK8:AL14" si="5">X8*0.000001/($B8/44100)</f>
         <v>0.40890346874999989</v>
       </c>
-      <c r="AI8" s="11">
+      <c r="AL8" s="11">
         <f t="shared" si="5"/>
         <v>0.46638506249999995</v>
       </c>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="11">
-        <f t="shared" ref="AK8:AK14" si="6">M8*0.000001/($B8/44100)</f>
+      <c r="AM8" s="11"/>
+      <c r="AN8" s="11">
+        <f t="shared" ref="AN8:AN14" si="6">O8*0.000001/($B8/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
-      <c r="AL8" s="11">
-        <f t="shared" ref="AL8:AL14" si="7">S8*0.000001/($B8/44100)</f>
+      <c r="AO8" s="11">
+        <f t="shared" ref="AO8:AO14" si="7">U8*0.000001/($B8/44100)</f>
         <v>0.17502187499999999</v>
       </c>
-      <c r="AM8" s="11">
-        <f t="shared" ref="AM8:AN14" si="8">W8*0.000001/($B8/44100)</f>
+      <c r="AP8" s="11">
+        <f t="shared" ref="AP8:AQ14" si="8">Z8*0.000001/($B8/44100)</f>
         <v>3.5831249999999995E-2</v>
       </c>
-      <c r="AN8" s="11">
+      <c r="AQ8" s="11">
         <f t="shared" si="8"/>
         <v>3.4453124999999994E-2</v>
       </c>
-      <c r="AO8" s="11">
-        <f>Z8*0.000001/($B8/44100)</f>
+      <c r="AR8" s="11">
+        <f>AC8*0.000001/($B8/44100)</f>
         <v>5.0990624999999998E-2</v>
       </c>
-      <c r="AP8" s="11">
-        <f>AA8*0.000001/($B8/44100)</f>
+      <c r="AS8" s="11">
+        <f>AD8*0.000001/($B8/44100)</f>
         <v>8.5443749999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>64</v>
       </c>
       <c r="C9">
+        <v>10102.4</v>
+      </c>
+      <c r="D9">
         <f>'ARM-Specific Functions'!E11</f>
         <v>67.150000000000006</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1495.29</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <f>'ARM-Specific Functions'!H11</f>
         <v>121.98</v>
       </c>
-      <c r="K9" s="13">
+      <c r="M9" s="13">
         <f>'ARM-Specific Functions'!H11</f>
         <v>121.98</v>
       </c>
-      <c r="L9" s="12">
+      <c r="N9" s="12">
         <v>77</v>
       </c>
-      <c r="M9" s="12">
+      <c r="O9" s="12">
         <v>114</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>162.52000000000001</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>323.75</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>592.08000000000004</v>
       </c>
-      <c r="R9" s="13">
+      <c r="T9" s="13">
         <v>854.36</v>
       </c>
-      <c r="S9" s="12">
+      <c r="U9" s="12">
         <v>238</v>
       </c>
-      <c r="U9" s="13">
+      <c r="X9" s="13">
         <f>'ARM-Specific Functions'!K11</f>
         <v>712.13</v>
       </c>
-      <c r="V9" s="13">
+      <c r="Y9" s="13">
         <v>724.79</v>
       </c>
-      <c r="W9" s="12">
+      <c r="Z9" s="12">
         <v>46</v>
       </c>
-      <c r="X9" s="12">
+      <c r="AA9" s="12">
         <v>55</v>
       </c>
-      <c r="Y9" s="12">
+      <c r="AB9" s="12">
         <v>77</v>
       </c>
-      <c r="Z9" s="12">
+      <c r="AC9" s="12">
         <v>79</v>
       </c>
-      <c r="AA9" s="12">
+      <c r="AD9" s="12">
         <v>102</v>
       </c>
-      <c r="AC9" s="9">
+      <c r="AF9" s="9">
         <v>1122.1300000000001</v>
       </c>
-      <c r="AD9" s="9">
+      <c r="AG9" s="9">
         <v>1662.88</v>
       </c>
-      <c r="AF9" s="11">
+      <c r="AI9" s="11">
         <f t="shared" si="3"/>
         <v>8.4051843749999994E-2</v>
       </c>
-      <c r="AG9" s="11">
+      <c r="AJ9" s="11">
         <f t="shared" si="4"/>
         <v>0.58870743749999999</v>
       </c>
-      <c r="AH9" s="11">
+      <c r="AK9" s="11">
         <f t="shared" si="5"/>
         <v>0.49070207812499994</v>
       </c>
-      <c r="AI9" s="11">
+      <c r="AL9" s="11">
         <f t="shared" si="5"/>
         <v>0.49942560937499991</v>
       </c>
-      <c r="AJ9" s="11"/>
-      <c r="AK9" s="11">
+      <c r="AM9" s="11"/>
+      <c r="AN9" s="11">
         <f t="shared" si="6"/>
         <v>7.8553124999999988E-2</v>
       </c>
-      <c r="AL9" s="11">
+      <c r="AO9" s="11">
         <f t="shared" si="7"/>
         <v>0.16399687499999999</v>
       </c>
-      <c r="AM9" s="11">
+      <c r="AP9" s="11">
         <f t="shared" si="8"/>
         <v>3.1696874999999999E-2</v>
       </c>
-      <c r="AN9" s="11">
+      <c r="AQ9" s="11">
         <f t="shared" si="8"/>
         <v>3.7898437499999993E-2</v>
       </c>
-      <c r="AO9" s="11">
-        <f t="shared" ref="AO9:AO14" si="9">Z9*0.000001/($B9/44100)</f>
+      <c r="AR9" s="11">
+        <f t="shared" ref="AR9:AR14" si="9">AC9*0.000001/($B9/44100)</f>
         <v>5.4435937499999996E-2</v>
       </c>
-      <c r="AP9" s="11">
-        <f t="shared" ref="AP9:AP14" si="10">AA9*0.000001/($B9/44100)</f>
+      <c r="AS9" s="11">
+        <f t="shared" ref="AS9:AS14" si="10">AD9*0.000001/($B9/44100)</f>
         <v>7.0284374999999996E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>128</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <f>'ARM-Specific Functions'!E12</f>
         <v>144.36000000000001</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>3835.47</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <f>'ARM-Specific Functions'!H12</f>
         <v>274.10000000000002</v>
       </c>
-      <c r="K10" s="13">
+      <c r="M10" s="13">
         <f>'ARM-Specific Functions'!H12</f>
         <v>274.10000000000002</v>
       </c>
-      <c r="L10" s="12">
+      <c r="N10" s="12">
         <v>173</v>
       </c>
-      <c r="M10" s="12">
+      <c r="O10" s="12">
         <v>254</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>355.3</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>721.27</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>1318.83</v>
       </c>
-      <c r="R10" s="13">
+      <c r="T10" s="13">
         <v>1982.42</v>
       </c>
-      <c r="S10" s="12">
+      <c r="U10" s="12">
         <v>632</v>
       </c>
-      <c r="U10" s="13">
+      <c r="X10" s="13">
         <f>'ARM-Specific Functions'!K12</f>
         <v>1664.97</v>
       </c>
-      <c r="V10" s="13">
+      <c r="Y10" s="13">
         <v>1759.28</v>
       </c>
-      <c r="W10" s="12">
+      <c r="Z10" s="12">
         <v>107</v>
       </c>
-      <c r="X10" s="12">
+      <c r="AA10" s="12">
         <v>118</v>
       </c>
-      <c r="Y10" s="12">
+      <c r="AB10" s="12">
         <v>210</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="AC10" s="12">
         <v>173</v>
       </c>
-      <c r="AA10" s="12">
+      <c r="AD10" s="12">
         <v>282</v>
       </c>
-      <c r="AC10" s="9">
+      <c r="AF10" s="9">
         <v>2080.58</v>
       </c>
-      <c r="AD10" s="9">
+      <c r="AG10" s="9">
         <v>3368.27</v>
       </c>
-      <c r="AF10" s="11">
+      <c r="AI10" s="11">
         <f t="shared" si="3"/>
         <v>9.4436015624999994E-2</v>
       </c>
-      <c r="AG10" s="11">
+      <c r="AJ10" s="11">
         <f t="shared" si="4"/>
         <v>0.68300564062499991</v>
       </c>
-      <c r="AH10" s="11">
+      <c r="AK10" s="11">
         <f t="shared" si="5"/>
         <v>0.57363419531250004</v>
       </c>
-      <c r="AI10" s="11">
+      <c r="AL10" s="11">
         <f t="shared" si="5"/>
         <v>0.60612693749999991</v>
       </c>
-      <c r="AJ10" s="11"/>
-      <c r="AK10" s="11">
+      <c r="AM10" s="11"/>
+      <c r="AN10" s="11">
         <f t="shared" si="6"/>
         <v>8.7510937499999997E-2</v>
       </c>
-      <c r="AL10" s="11">
+      <c r="AO10" s="11">
         <f t="shared" si="7"/>
         <v>0.21774374999999999</v>
       </c>
-      <c r="AM10" s="11">
+      <c r="AP10" s="11">
         <f t="shared" si="8"/>
         <v>3.6864843750000001E-2</v>
       </c>
-      <c r="AN10" s="11">
+      <c r="AQ10" s="11">
         <f t="shared" si="8"/>
         <v>4.0654687499999995E-2</v>
       </c>
-      <c r="AO10" s="11">
+      <c r="AR10" s="11">
         <f t="shared" si="9"/>
         <v>5.9603906249999998E-2</v>
       </c>
-      <c r="AP10" s="11">
+      <c r="AS10" s="11">
         <f t="shared" si="10"/>
         <v>9.7157812499999982E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>256</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <f>'ARM-Specific Functions'!E13</f>
         <v>313.25</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>8025.18</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <f>'ARM-Specific Functions'!H13</f>
         <v>614.41999999999996</v>
       </c>
-      <c r="K11" s="13">
+      <c r="M11" s="13">
         <f>'ARM-Specific Functions'!H13</f>
         <v>614.41999999999996</v>
       </c>
-      <c r="L11" s="12">
+      <c r="N11" s="12">
         <v>382</v>
       </c>
-      <c r="M11" s="12">
+      <c r="O11" s="12">
         <v>566</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>776.61</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>1595.22</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>2917.8</v>
       </c>
-      <c r="R11" s="13">
+      <c r="T11" s="13">
         <v>4197.54</v>
       </c>
-      <c r="S11" s="12">
+      <c r="U11" s="12">
         <v>1199</v>
       </c>
-      <c r="U11" s="13">
+      <c r="X11" s="13">
         <f>'ARM-Specific Functions'!K13</f>
         <v>3819.2</v>
       </c>
-      <c r="V11" s="13">
+      <c r="Y11" s="13">
         <v>3756.42</v>
       </c>
-      <c r="W11" s="12">
+      <c r="Z11" s="12">
         <v>207</v>
       </c>
-      <c r="X11" s="12">
+      <c r="AA11" s="12">
         <v>255</v>
       </c>
-      <c r="Y11" s="12">
+      <c r="AB11" s="12">
         <v>360</v>
       </c>
-      <c r="Z11" s="12">
+      <c r="AC11" s="12">
         <v>374</v>
       </c>
-      <c r="AA11" s="12">
+      <c r="AD11" s="12">
         <v>477</v>
       </c>
-      <c r="AC11" s="9">
+      <c r="AF11" s="9">
         <v>4087.76</v>
       </c>
-      <c r="AD11" s="9">
+      <c r="AG11" s="9">
         <v>6991.74</v>
       </c>
-      <c r="AF11" s="11">
+      <c r="AI11" s="11">
         <f t="shared" si="3"/>
         <v>0.10584344531249999</v>
       </c>
-      <c r="AG11" s="11">
+      <c r="AJ11" s="11">
         <f t="shared" si="4"/>
         <v>0.72309185156249989</v>
       </c>
-      <c r="AH11" s="11">
+      <c r="AK11" s="11">
         <f t="shared" si="5"/>
         <v>0.65791687499999996</v>
       </c>
-      <c r="AI11" s="11">
+      <c r="AL11" s="11">
         <f t="shared" si="5"/>
         <v>0.64710203906249997</v>
       </c>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="11">
+      <c r="AM11" s="11"/>
+      <c r="AN11" s="11">
         <f t="shared" si="6"/>
         <v>9.7502343749999998E-2</v>
       </c>
-      <c r="AL11" s="11">
+      <c r="AO11" s="11">
         <f t="shared" si="7"/>
         <v>0.20654648437500001</v>
       </c>
-      <c r="AM11" s="11">
+      <c r="AP11" s="11">
         <f t="shared" si="8"/>
         <v>3.5658984375000001E-2</v>
       </c>
-      <c r="AN11" s="11">
+      <c r="AQ11" s="11">
         <f t="shared" si="8"/>
         <v>4.3927734374999992E-2</v>
       </c>
-      <c r="AO11" s="11">
+      <c r="AR11" s="11">
         <f t="shared" si="9"/>
         <v>6.4427343749999991E-2</v>
       </c>
-      <c r="AP11" s="11">
+      <c r="AS11" s="11">
         <f t="shared" si="10"/>
         <v>8.2170703124999994E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>512</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <f>'ARM-Specific Functions'!E14</f>
         <v>667.18</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>19443.13</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <f>'ARM-Specific Functions'!H14</f>
         <v>1361.9</v>
       </c>
-      <c r="K12" s="13">
+      <c r="M12" s="13">
         <f>'ARM-Specific Functions'!H14</f>
         <v>1361.9</v>
       </c>
-      <c r="L12" s="12">
+      <c r="N12" s="12">
         <v>835</v>
       </c>
-      <c r="M12" s="12">
+      <c r="O12" s="12">
         <v>1243</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>1688.09</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>3498.65</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>6393.07</v>
       </c>
-      <c r="R12" s="13">
+      <c r="T12" s="13">
         <v>9582.68</v>
       </c>
-      <c r="S12" s="12">
+      <c r="U12" s="12">
         <v>3031</v>
       </c>
-      <c r="U12" s="13">
+      <c r="X12" s="13">
         <f>'ARM-Specific Functions'!K14</f>
         <v>8619.5400000000009</v>
       </c>
-      <c r="V12" s="13">
+      <c r="Y12" s="13">
         <v>8768.08</v>
       </c>
-      <c r="W12" s="12">
+      <c r="Z12" s="12">
         <v>470</v>
       </c>
-      <c r="X12" s="12">
+      <c r="AA12" s="12">
         <v>550</v>
       </c>
-      <c r="Y12" s="12">
+      <c r="AB12" s="12">
         <v>946</v>
       </c>
-      <c r="Z12" s="12">
+      <c r="AC12" s="12">
         <v>799</v>
       </c>
-      <c r="AA12" s="12">
+      <c r="AD12" s="12">
         <v>1272</v>
       </c>
-      <c r="AC12" s="9">
+      <c r="AF12" s="9">
         <v>8299.17</v>
       </c>
-      <c r="AD12" s="9">
+      <c r="AG12" s="9">
         <v>14675.67</v>
       </c>
-      <c r="AF12" s="11">
+      <c r="AI12" s="11">
         <f t="shared" si="3"/>
         <v>0.11730427734375</v>
       </c>
-      <c r="AG12" s="11">
+      <c r="AJ12" s="11">
         <f t="shared" si="4"/>
         <v>0.82538317968749997</v>
       </c>
-      <c r="AH12" s="11">
+      <c r="AK12" s="11">
         <f t="shared" si="5"/>
         <v>0.74242522265624999</v>
       </c>
-      <c r="AI12" s="11">
+      <c r="AL12" s="11">
         <f t="shared" si="5"/>
         <v>0.75521939062499988</v>
       </c>
-      <c r="AJ12" s="11"/>
-      <c r="AK12" s="11">
+      <c r="AM12" s="11"/>
+      <c r="AN12" s="11">
         <f t="shared" si="6"/>
         <v>0.1070630859375</v>
       </c>
-      <c r="AL12" s="11">
+      <c r="AO12" s="11">
         <f t="shared" si="7"/>
         <v>0.26106855468749995</v>
       </c>
-      <c r="AM12" s="11">
+      <c r="AP12" s="11">
         <f t="shared" si="8"/>
         <v>4.0482421875000001E-2</v>
       </c>
-      <c r="AN12" s="11">
+      <c r="AQ12" s="11">
         <f t="shared" si="8"/>
         <v>4.7373046874999991E-2</v>
       </c>
-      <c r="AO12" s="11">
+      <c r="AR12" s="11">
         <f t="shared" si="9"/>
         <v>6.8820117187500002E-2</v>
       </c>
-      <c r="AP12" s="11">
+      <c r="AS12" s="11">
         <f t="shared" si="10"/>
         <v>0.1095609375</v>
       </c>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1024</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <f>'ARM-Specific Functions'!E15</f>
         <v>1442.6</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>40529.33</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <f>'ARM-Specific Functions'!H15</f>
         <v>3009.96</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>3621.3</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>6826.63</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>13542.68</v>
       </c>
-      <c r="K13" s="13">
+      <c r="M13" s="13">
         <f>'ARM-Specific Functions'!H15</f>
         <v>3009.96</v>
       </c>
-      <c r="L13" s="12">
+      <c r="N13" s="12">
         <v>1827</v>
       </c>
-      <c r="M13" s="12">
+      <c r="O13" s="12">
         <v>1243</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>3654.13</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>7621.21</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>13917.22</v>
       </c>
-      <c r="R13" s="13">
+      <c r="T13" s="13">
         <v>20189.66</v>
       </c>
-      <c r="S13" s="12">
+      <c r="U13" s="12">
         <v>5801</v>
       </c>
-      <c r="U13" s="13">
+      <c r="X13" s="13">
         <f>'ARM-Specific Functions'!K15</f>
         <v>19211.900000000001</v>
       </c>
-      <c r="V13" s="13">
+      <c r="Y13" s="13">
         <v>18485.53</v>
       </c>
-      <c r="W13" s="12">
+      <c r="Z13" s="12">
         <v>956</v>
       </c>
-      <c r="X13" s="12">
+      <c r="AA13" s="12">
         <v>1183</v>
       </c>
-      <c r="Y13" s="12">
+      <c r="AB13" s="12">
         <v>1644</v>
       </c>
-      <c r="Z13" s="12">
+      <c r="AC13" s="12">
         <v>1725</v>
       </c>
-      <c r="AA13" s="12">
+      <c r="AD13" s="12">
         <v>2196</v>
       </c>
-      <c r="AC13" s="9">
+      <c r="AF13" s="9">
         <v>17191.080000000002</v>
       </c>
-      <c r="AD13" s="9">
+      <c r="AG13" s="9">
         <v>30967.26</v>
       </c>
-      <c r="AF13" s="11">
+      <c r="AI13" s="11">
         <f t="shared" si="3"/>
         <v>0.12962816015625001</v>
       </c>
-      <c r="AG13" s="11">
+      <c r="AJ13" s="11">
         <f t="shared" si="4"/>
         <v>0.86949609960937491</v>
       </c>
-      <c r="AH13" s="11">
+      <c r="AK13" s="11">
         <f t="shared" si="5"/>
         <v>0.82738749023437497</v>
       </c>
-      <c r="AI13" s="11">
+      <c r="AL13" s="11">
         <f t="shared" si="5"/>
         <v>0.79610534472656236</v>
       </c>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11">
+      <c r="AM13" s="11"/>
+      <c r="AN13" s="11">
         <f t="shared" si="6"/>
         <v>5.3531542968749998E-2</v>
       </c>
-      <c r="AL13" s="11">
+      <c r="AO13" s="11">
         <f t="shared" si="7"/>
         <v>0.24982822265624999</v>
       </c>
-      <c r="AM13" s="11">
+      <c r="AP13" s="11">
         <f t="shared" si="8"/>
         <v>4.1171484374999998E-2</v>
       </c>
-      <c r="AN13" s="11">
+      <c r="AQ13" s="11">
         <f t="shared" si="8"/>
         <v>5.0947558593749998E-2</v>
       </c>
-      <c r="AO13" s="11">
+      <c r="AR13" s="11">
         <f t="shared" si="9"/>
         <v>7.4289550781249991E-2</v>
       </c>
-      <c r="AP13" s="11">
+      <c r="AS13" s="11">
         <f t="shared" si="10"/>
         <v>9.4573828124999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2048</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <f>'ARM-Specific Functions'!E16</f>
         <v>3088.11</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <f>'ARM-Specific Functions'!H16</f>
         <v>6578.57</v>
       </c>
-      <c r="K14" s="13">
+      <c r="M14" s="13">
         <f>'ARM-Specific Functions'!H16</f>
         <v>6578.57</v>
       </c>
-      <c r="L14" s="12">
+      <c r="N14" s="12">
         <v>3927</v>
       </c>
-      <c r="M14" s="12">
+      <c r="O14" s="12">
         <v>5874</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>7866.48</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>16942.04</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>30090.02</v>
       </c>
-      <c r="R14" s="13">
+      <c r="T14" s="13">
         <v>45220.12</v>
       </c>
-      <c r="S14" s="12">
+      <c r="U14" s="12">
         <v>14133</v>
       </c>
-      <c r="U14" s="13">
+      <c r="X14" s="13">
         <f>'ARM-Specific Functions'!K16</f>
         <v>42355.1</v>
       </c>
-      <c r="V14" s="13">
+      <c r="Y14" s="13">
         <v>42107.63</v>
       </c>
-      <c r="W14" s="12">
+      <c r="Z14" s="12">
         <v>2135</v>
       </c>
-      <c r="X14" s="12">
+      <c r="AA14" s="12">
         <v>2464</v>
       </c>
-      <c r="Y14" s="12">
+      <c r="AB14" s="12">
         <v>4198</v>
       </c>
-      <c r="Z14" s="12">
+      <c r="AC14" s="12">
         <v>3628</v>
       </c>
-      <c r="AA14" s="12">
+      <c r="AD14" s="12">
         <v>5658</v>
       </c>
-      <c r="AC14" s="9">
+      <c r="AF14" s="9">
         <v>35957.269999999997</v>
       </c>
-      <c r="AD14" s="9">
+      <c r="AG14" s="9">
         <v>65450.37</v>
       </c>
-      <c r="AF14" s="11">
+      <c r="AI14" s="11">
         <f t="shared" si="3"/>
         <v>0.14165768408203125</v>
       </c>
-      <c r="AG14" s="11">
+      <c r="AJ14" s="11">
         <f t="shared" si="4"/>
         <v>0.97373402929687503</v>
       </c>
-      <c r="AH14" s="11">
+      <c r="AK14" s="11">
         <f t="shared" si="5"/>
         <v>0.91204097167968745</v>
       </c>
-      <c r="AI14" s="11">
+      <c r="AL14" s="11">
         <f t="shared" si="5"/>
         <v>0.90671214990234361</v>
       </c>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11">
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="11">
         <f t="shared" si="6"/>
         <v>0.12648603515624998</v>
       </c>
-      <c r="AL14" s="11">
+      <c r="AO14" s="11">
         <f t="shared" si="7"/>
         <v>0.30432875976562501</v>
       </c>
-      <c r="AM14" s="11">
+      <c r="AP14" s="11">
         <f t="shared" si="8"/>
         <v>4.597338867187499E-2</v>
       </c>
-      <c r="AN14" s="11">
+      <c r="AQ14" s="11">
         <f t="shared" si="8"/>
         <v>5.3057812500000003E-2</v>
       </c>
-      <c r="AO14" s="11">
+      <c r="AR14" s="11">
         <f t="shared" si="9"/>
         <v>7.8122460937499999E-2</v>
       </c>
-      <c r="AP14" s="11">
+      <c r="AS14" s="11">
         <f t="shared" si="10"/>
         <v>0.12183486328125</v>
       </c>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="U16" t="s">
+      <c r="X16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B8</f>
         <v>32</v>
       </c>
-      <c r="U17" s="2">
-        <f t="shared" ref="U17:AA17" si="11">U8/$B8</f>
+      <c r="X17" s="2">
+        <f t="shared" ref="X17:AD17" si="11">X8/$B8</f>
         <v>9.2721874999999994</v>
       </c>
-      <c r="V17" s="2">
+      <c r="Y17" s="2">
         <f t="shared" si="11"/>
         <v>10.575625</v>
       </c>
-      <c r="W17" s="2">
+      <c r="Z17" s="2">
         <f t="shared" si="11"/>
         <v>0.8125</v>
       </c>
-      <c r="X17" s="2">
+      <c r="AA17" s="2">
         <f t="shared" si="11"/>
         <v>0.78125</v>
       </c>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2">
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2">
         <f t="shared" si="11"/>
         <v>1.15625</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AD17" s="2">
         <f t="shared" si="11"/>
         <v>1.9375</v>
       </c>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="10">
-        <f t="shared" ref="AC17:AD17" si="12">AC8/$B8</f>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="10">
+        <f t="shared" ref="AF17:AG17" si="12">AF8/$B8</f>
         <v>20.468125000000001</v>
       </c>
-      <c r="AD17" s="10">
+      <c r="AG17" s="10">
         <f t="shared" si="12"/>
         <v>26.46125</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" ref="B18:B23" si="13">B9</f>
         <v>64</v>
       </c>
-      <c r="U18" s="2">
-        <f t="shared" ref="U18:AD18" si="14">U9/$B9</f>
+      <c r="X18" s="2">
+        <f t="shared" ref="X18:AG18" si="14">X9/$B9</f>
         <v>11.12703125</v>
       </c>
-      <c r="V18" s="2">
-        <f t="shared" ref="V18" si="15">V9/$B9</f>
+      <c r="Y18" s="2">
+        <f t="shared" ref="Y18" si="15">Y9/$B9</f>
         <v>11.324843749999999</v>
       </c>
-      <c r="W18" s="2">
-        <f t="shared" ref="W18:Y23" si="16">W9/$B9</f>
+      <c r="Z18" s="2">
+        <f t="shared" ref="Z18:AB23" si="16">Z9/$B9</f>
         <v>0.71875</v>
       </c>
-      <c r="X18" s="2">
+      <c r="AA18" s="2">
         <f t="shared" si="16"/>
         <v>0.859375</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="AB18" s="2">
         <f t="shared" si="16"/>
         <v>1.203125</v>
       </c>
-      <c r="Z18" s="2">
-        <f t="shared" ref="Z18:AA18" si="17">Z9/$B9</f>
+      <c r="AC18" s="2">
+        <f t="shared" ref="AC18:AD18" si="17">AC9/$B9</f>
         <v>1.234375</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AD18" s="2">
         <f t="shared" si="17"/>
         <v>1.59375</v>
       </c>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="10">
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="10">
         <f t="shared" si="14"/>
         <v>17.533281250000002</v>
       </c>
-      <c r="AD18" s="10">
+      <c r="AG18" s="10">
         <f t="shared" si="14"/>
         <v>25.982500000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="13"/>
         <v>128</v>
       </c>
-      <c r="U19" s="2">
-        <f t="shared" ref="U19:AD19" si="18">U10/$B10</f>
+      <c r="X19" s="2">
+        <f t="shared" ref="X19:AG19" si="18">X10/$B10</f>
         <v>13.007578125</v>
       </c>
-      <c r="V19" s="2">
-        <f t="shared" ref="V19" si="19">V10/$B10</f>
+      <c r="Y19" s="2">
+        <f t="shared" ref="Y19" si="19">Y10/$B10</f>
         <v>13.744375</v>
       </c>
-      <c r="W19" s="2">
+      <c r="Z19" s="2">
         <f t="shared" si="16"/>
         <v>0.8359375</v>
       </c>
-      <c r="X19" s="2">
+      <c r="AA19" s="2">
         <f t="shared" si="16"/>
         <v>0.921875</v>
       </c>
-      <c r="Y19" s="2">
-        <f t="shared" ref="Y19" si="20">Y10/$B10</f>
+      <c r="AB19" s="2">
+        <f t="shared" ref="AB19" si="20">AB10/$B10</f>
         <v>1.640625</v>
       </c>
-      <c r="Z19" s="2">
-        <f t="shared" ref="Z19:AA19" si="21">Z10/$B10</f>
+      <c r="AC19" s="2">
+        <f t="shared" ref="AC19:AD19" si="21">AC10/$B10</f>
         <v>1.3515625</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AD19" s="2">
         <f t="shared" si="21"/>
         <v>2.203125</v>
       </c>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="10">
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="10">
         <f t="shared" si="18"/>
         <v>16.254531249999999</v>
       </c>
-      <c r="AD19" s="10">
+      <c r="AG19" s="10">
         <f t="shared" si="18"/>
         <v>26.314609375</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="13"/>
         <v>256</v>
       </c>
-      <c r="U20" s="2">
-        <f t="shared" ref="U20:AD20" si="22">U11/$B11</f>
+      <c r="X20" s="2">
+        <f t="shared" ref="X20:AG20" si="22">X11/$B11</f>
         <v>14.918749999999999</v>
       </c>
-      <c r="V20" s="2">
-        <f t="shared" ref="V20" si="23">V11/$B11</f>
+      <c r="Y20" s="2">
+        <f t="shared" ref="Y20" si="23">Y11/$B11</f>
         <v>14.673515625</v>
       </c>
-      <c r="W20" s="2">
+      <c r="Z20" s="2">
         <f t="shared" si="16"/>
         <v>0.80859375</v>
       </c>
-      <c r="X20" s="2">
+      <c r="AA20" s="2">
         <f t="shared" si="16"/>
         <v>0.99609375</v>
       </c>
-      <c r="Y20" s="2">
-        <f t="shared" ref="Y20" si="24">Y11/$B11</f>
+      <c r="AB20" s="2">
+        <f t="shared" ref="AB20" si="24">AB11/$B11</f>
         <v>1.40625</v>
       </c>
-      <c r="Z20" s="2">
-        <f t="shared" ref="Z20:AA20" si="25">Z11/$B11</f>
+      <c r="AC20" s="2">
+        <f t="shared" ref="AC20:AD20" si="25">AC11/$B11</f>
         <v>1.4609375</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AD20" s="2">
         <f t="shared" si="25"/>
         <v>1.86328125</v>
       </c>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="10">
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="10">
         <f t="shared" si="22"/>
         <v>15.967812500000001</v>
       </c>
-      <c r="AD20" s="10">
+      <c r="AG20" s="10">
         <f t="shared" si="22"/>
         <v>27.311484374999999</v>
       </c>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="13"/>
         <v>512</v>
       </c>
-      <c r="U21" s="2">
-        <f t="shared" ref="U21:AD21" si="26">U12/$B12</f>
+      <c r="X21" s="2">
+        <f t="shared" ref="X21:AG21" si="26">X12/$B12</f>
         <v>16.835039062500002</v>
       </c>
-      <c r="V21" s="2">
-        <f t="shared" ref="V21" si="27">V12/$B12</f>
+      <c r="Y21" s="2">
+        <f t="shared" ref="Y21" si="27">Y12/$B12</f>
         <v>17.12515625</v>
       </c>
-      <c r="W21" s="2">
+      <c r="Z21" s="2">
         <f t="shared" si="16"/>
         <v>0.91796875</v>
       </c>
-      <c r="X21" s="2">
+      <c r="AA21" s="2">
         <f t="shared" si="16"/>
         <v>1.07421875</v>
       </c>
-      <c r="Y21" s="2">
-        <f t="shared" ref="Y21" si="28">Y12/$B12</f>
+      <c r="AB21" s="2">
+        <f t="shared" ref="AB21" si="28">AB12/$B12</f>
         <v>1.84765625</v>
       </c>
-      <c r="Z21" s="2">
-        <f t="shared" ref="Z21:AA21" si="29">Z12/$B12</f>
+      <c r="AC21" s="2">
+        <f t="shared" ref="AC21:AD21" si="29">AC12/$B12</f>
         <v>1.560546875</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="AD21" s="2">
         <f t="shared" si="29"/>
         <v>2.484375</v>
       </c>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="10">
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="10">
         <f t="shared" si="26"/>
         <v>16.20931640625</v>
       </c>
-      <c r="AD21" s="10">
+      <c r="AG21" s="10">
         <f t="shared" si="26"/>
         <v>28.66341796875</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="13"/>
         <v>1024</v>
       </c>
-      <c r="U22" s="2">
-        <f t="shared" ref="U22:AD22" si="30">U13/$B13</f>
+      <c r="X22" s="2">
+        <f t="shared" ref="X22:AG22" si="30">X13/$B13</f>
         <v>18.761621093750001</v>
       </c>
-      <c r="V22" s="2">
-        <f t="shared" ref="V22" si="31">V13/$B13</f>
+      <c r="Y22" s="2">
+        <f t="shared" ref="Y22" si="31">Y13/$B13</f>
         <v>18.052275390624999</v>
       </c>
-      <c r="W22" s="2">
+      <c r="Z22" s="2">
         <f t="shared" si="16"/>
         <v>0.93359375</v>
       </c>
-      <c r="X22" s="2">
+      <c r="AA22" s="2">
         <f t="shared" si="16"/>
         <v>1.1552734375</v>
       </c>
-      <c r="Y22" s="2">
-        <f t="shared" ref="Y22" si="32">Y13/$B13</f>
+      <c r="AB22" s="2">
+        <f t="shared" ref="AB22" si="32">AB13/$B13</f>
         <v>1.60546875</v>
       </c>
-      <c r="Z22" s="2">
-        <f t="shared" ref="Z22:AA22" si="33">Z13/$B13</f>
+      <c r="AC22" s="2">
+        <f t="shared" ref="AC22:AD22" si="33">AC13/$B13</f>
         <v>1.6845703125</v>
       </c>
-      <c r="AA22" s="2">
+      <c r="AD22" s="2">
         <f t="shared" si="33"/>
         <v>2.14453125</v>
       </c>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="10">
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="10">
         <f t="shared" si="30"/>
         <v>16.788164062500002</v>
       </c>
-      <c r="AD22" s="10">
+      <c r="AG22" s="10">
         <f t="shared" si="30"/>
         <v>30.241464843749998</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="13"/>
         <v>2048</v>
       </c>
-      <c r="U23" s="2">
-        <f t="shared" ref="U23:AD23" si="34">U14/$B14</f>
+      <c r="X23" s="2">
+        <f t="shared" ref="X23:AG23" si="34">X14/$B14</f>
         <v>20.681201171874999</v>
       </c>
-      <c r="V23" s="2">
-        <f t="shared" ref="V23" si="35">V14/$B14</f>
+      <c r="Y23" s="2">
+        <f t="shared" ref="Y23" si="35">Y14/$B14</f>
         <v>20.560366210937499</v>
       </c>
-      <c r="W23" s="2">
+      <c r="Z23" s="2">
         <f t="shared" si="16"/>
         <v>1.04248046875</v>
       </c>
-      <c r="X23" s="2">
+      <c r="AA23" s="2">
         <f t="shared" si="16"/>
         <v>1.203125</v>
       </c>
-      <c r="Y23" s="2">
-        <f t="shared" ref="Y23" si="36">Y14/$B14</f>
+      <c r="AB23" s="2">
+        <f t="shared" ref="AB23" si="36">AB14/$B14</f>
         <v>2.0498046875</v>
       </c>
-      <c r="Z23" s="2">
-        <f t="shared" ref="Z23:AA23" si="37">Z14/$B14</f>
+      <c r="AC23" s="2">
+        <f t="shared" ref="AC23:AD23" si="37">AC14/$B14</f>
         <v>1.771484375</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="AD23" s="2">
         <f t="shared" si="37"/>
         <v>2.7626953125</v>
       </c>
-      <c r="AB23" s="2"/>
-      <c r="AC23" s="10">
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="10">
         <f t="shared" si="34"/>
         <v>17.557260742187498</v>
       </c>
-      <c r="AD23" s="10">
+      <c r="AG23" s="10">
         <f t="shared" si="34"/>
         <v>31.958188476562501</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="X24" s="2"/>
-      <c r="Y24" s="2" t="e">
-        <f t="shared" ref="Y24" si="38">Y15/$B15</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="10"/>
-      <c r="AD24" s="10"/>
-    </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z25" s="2"/>
-      <c r="AA25" s="2"/>
-    </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z26" s="2"/>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z27" s="2"/>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z28" s="2"/>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z29" s="2"/>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z30" s="2"/>
-    </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z31" s="2"/>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Z32" s="2"/>
+      <c r="AB24" s="2" t="e">
+        <f t="shared" ref="AB24" si="38">AB15/$B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="10"/>
+      <c r="AG24" s="10"/>
+    </row>
+    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+    </row>
+    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC26" s="2"/>
+    </row>
+    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC27" s="2"/>
+    </row>
+    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC28" s="2"/>
+    </row>
+    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC29" s="2"/>
+    </row>
+    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC30" s="2"/>
+    </row>
+    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC31" s="2"/>
+    </row>
+    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AC32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Benchmark: still formatting results
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FFT Speed Results.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ARM-Specific Functions" sheetId="1" r:id="rId1"/>
     <sheet name="Compare (2)" sheetId="9" r:id="rId2"/>
     <sheet name="Compare" sheetId="6" r:id="rId3"/>
-    <sheet name="Arduino Uno" sheetId="4" r:id="rId4"/>
-    <sheet name="Arduino M0 Pro" sheetId="8" r:id="rId5"/>
-    <sheet name="Teensy 3.2" sheetId="3" r:id="rId6"/>
-    <sheet name="NXP K66" sheetId="5" r:id="rId7"/>
-    <sheet name="Old" sheetId="2" r:id="rId8"/>
-    <sheet name="AllData" sheetId="7" r:id="rId9"/>
+    <sheet name="AllData" sheetId="7" r:id="rId4"/>
+    <sheet name="Arduino Uno" sheetId="4" r:id="rId5"/>
+    <sheet name="Arduino M0 Pro" sheetId="8" r:id="rId6"/>
+    <sheet name="Teensy 3.2" sheetId="3" r:id="rId7"/>
+    <sheet name="NXP K66" sheetId="5" r:id="rId8"/>
+    <sheet name="Old" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="65">
   <si>
     <t>N</t>
   </si>
@@ -212,6 +212,12 @@
   <si>
     <t>FFT per sec</t>
   </si>
+  <si>
+    <t>CMSIS Radix 4</t>
+  </si>
+  <si>
+    <t>NXP FRDM-K66</t>
+  </si>
 </sst>
 </file>
 
@@ -222,7 +228,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +261,12 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -305,7 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -323,6 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,11 +686,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86646784"/>
-        <c:axId val="86648704"/>
+        <c:axId val="144131584"/>
+        <c:axId val="149833216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86646784"/>
+        <c:axId val="144131584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,7 +719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86648704"/>
+        <c:crossAx val="149833216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -714,7 +727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86648704"/>
+        <c:axId val="149833216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -746,7 +759,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86646784"/>
+        <c:crossAx val="144131584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1105,11 +1118,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86692608"/>
-        <c:axId val="86694528"/>
+        <c:axId val="42398464"/>
+        <c:axId val="42400384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86692608"/>
+        <c:axId val="42398464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1151,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86694528"/>
+        <c:crossAx val="42400384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1146,7 +1159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86694528"/>
+        <c:axId val="42400384"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1178,7 +1191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86692608"/>
+        <c:crossAx val="42398464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1514,11 +1527,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43682432"/>
-        <c:axId val="45893504"/>
+        <c:axId val="42485632"/>
+        <c:axId val="42487808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43682432"/>
+        <c:axId val="42485632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,7 +1560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45893504"/>
+        <c:crossAx val="42487808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1555,7 +1568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45893504"/>
+        <c:axId val="42487808"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1588,7 +1601,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43682432"/>
+        <c:crossAx val="42485632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1924,11 +1937,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142019968"/>
-        <c:axId val="142984320"/>
+        <c:axId val="42502784"/>
+        <c:axId val="42504960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142019968"/>
+        <c:axId val="42502784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,7 +1970,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142984320"/>
+        <c:crossAx val="42504960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1965,7 +1978,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142984320"/>
+        <c:axId val="42504960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1998,7 +2011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142019968"/>
+        <c:crossAx val="42502784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3653,7 +3666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
@@ -4525,7 +4538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
@@ -5212,6 +5225,1589 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:F98"/>
+  <sheetViews>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5" s="17">
+        <v>4980.8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6" s="17">
+        <v>10102.4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="F7" s="17">
+        <v>12559.2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>32</v>
+      </c>
+      <c r="F8" s="17">
+        <v>6378</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" s="17">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10" s="17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>32</v>
+      </c>
+      <c r="F11" s="17">
+        <v>103.4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>64</v>
+      </c>
+      <c r="F12" s="17">
+        <v>204.4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>128</v>
+      </c>
+      <c r="F13" s="17">
+        <v>520.4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>256</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1030.4000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15">
+        <v>512</v>
+      </c>
+      <c r="F15" s="17">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16">
+        <v>1024</v>
+      </c>
+      <c r="F16" s="17">
+        <v>4975</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17" s="17">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18" s="17">
+        <v>68.400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>32</v>
+      </c>
+      <c r="F19" s="17">
+        <v>192.8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <v>64</v>
+      </c>
+      <c r="F20" s="17">
+        <v>383.6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <v>128</v>
+      </c>
+      <c r="F21" s="17">
+        <v>993.2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22">
+        <v>256</v>
+      </c>
+      <c r="F22" s="17">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23">
+        <v>512</v>
+      </c>
+      <c r="F23" s="17">
+        <v>4858</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24">
+        <v>1024</v>
+      </c>
+      <c r="F24" s="17">
+        <v>9679</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" s="17">
+        <v>73.8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26" s="17">
+        <v>177.6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>32</v>
+      </c>
+      <c r="F27" s="17">
+        <v>496.4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28">
+        <v>64</v>
+      </c>
+      <c r="F28" s="17">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29">
+        <v>128</v>
+      </c>
+      <c r="F29" s="17">
+        <v>2849.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30">
+        <v>256</v>
+      </c>
+      <c r="F30" s="17">
+        <v>6295.8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>512</v>
+      </c>
+      <c r="F31" s="17">
+        <v>14922</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32">
+        <v>1024</v>
+      </c>
+      <c r="F32" s="17">
+        <v>32259.4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33" s="17">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34">
+        <v>16</v>
+      </c>
+      <c r="F34" s="17">
+        <v>14.12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35">
+        <v>32</v>
+      </c>
+      <c r="F35" s="17">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36">
+        <v>64</v>
+      </c>
+      <c r="F36" s="17">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37">
+        <v>128</v>
+      </c>
+      <c r="F37" s="17">
+        <v>139.74</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38">
+        <v>256</v>
+      </c>
+      <c r="F38" s="17">
+        <v>272.54000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39">
+        <v>512</v>
+      </c>
+      <c r="F39" s="17">
+        <v>635.05999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40">
+        <v>1024</v>
+      </c>
+      <c r="F40" s="17">
+        <v>1254.4000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <v>8</v>
+      </c>
+      <c r="F41" s="17">
+        <v>12.38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42">
+        <v>16</v>
+      </c>
+      <c r="F42" s="17">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43">
+        <v>32</v>
+      </c>
+      <c r="F43" s="17">
+        <v>60.7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44">
+        <v>64</v>
+      </c>
+      <c r="F44" s="17">
+        <v>116.58</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45">
+        <v>128</v>
+      </c>
+      <c r="F45" s="17">
+        <v>303.7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46">
+        <v>256</v>
+      </c>
+      <c r="F46" s="17">
+        <v>597.08000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47">
+        <v>512</v>
+      </c>
+      <c r="F47" s="17">
+        <v>1476.16</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48">
+        <v>1024</v>
+      </c>
+      <c r="F48" s="17">
+        <v>2920.28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49" s="17">
+        <v>49.44</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50">
+        <v>16</v>
+      </c>
+      <c r="F50" s="17">
+        <v>88.9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51">
+        <v>32</v>
+      </c>
+      <c r="F51" s="17">
+        <v>282.3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52">
+        <v>64</v>
+      </c>
+      <c r="F52" s="17">
+        <v>552.04</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53">
+        <v>128</v>
+      </c>
+      <c r="F53" s="17">
+        <v>1520.76</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54">
+        <v>256</v>
+      </c>
+      <c r="F54" s="17">
+        <v>3022.52</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55">
+        <v>512</v>
+      </c>
+      <c r="F55" s="17">
+        <v>7711.3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56">
+        <v>1024</v>
+      </c>
+      <c r="F56" s="17">
+        <v>15382.98</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" t="s">
+        <v>31</v>
+      </c>
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57" s="17">
+        <v>62.2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58">
+        <v>16</v>
+      </c>
+      <c r="F58" s="17">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59">
+        <v>32</v>
+      </c>
+      <c r="F59" s="17">
+        <v>319.8</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" t="s">
+        <v>31</v>
+      </c>
+      <c r="E60">
+        <v>64</v>
+      </c>
+      <c r="F60" s="17">
+        <v>627.20000000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" t="s">
+        <v>31</v>
+      </c>
+      <c r="E61">
+        <v>128</v>
+      </c>
+      <c r="F61" s="17">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E62">
+        <v>256</v>
+      </c>
+      <c r="F62" s="17">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" t="s">
+        <v>60</v>
+      </c>
+      <c r="D63" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63">
+        <v>512</v>
+      </c>
+      <c r="F63" s="17">
+        <v>7403</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" t="s">
+        <v>31</v>
+      </c>
+      <c r="E64">
+        <v>1024</v>
+      </c>
+      <c r="F64" s="17">
+        <v>14605.4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" t="s">
+        <v>32</v>
+      </c>
+      <c r="E65">
+        <v>8</v>
+      </c>
+      <c r="F65" s="17">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" t="s">
+        <v>60</v>
+      </c>
+      <c r="D66" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66">
+        <v>16</v>
+      </c>
+      <c r="F66" s="17">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
+      </c>
+      <c r="D67" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67">
+        <v>32</v>
+      </c>
+      <c r="F67" s="17">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+      <c r="D68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68">
+        <v>64</v>
+      </c>
+      <c r="F68" s="17">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" t="s">
+        <v>60</v>
+      </c>
+      <c r="D69" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69">
+        <v>128</v>
+      </c>
+      <c r="F69" s="17">
+        <v>4241</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70">
+        <v>256</v>
+      </c>
+      <c r="F70" s="17">
+        <v>8763</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" t="s">
+        <v>60</v>
+      </c>
+      <c r="D71" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71">
+        <v>512</v>
+      </c>
+      <c r="F71" s="17">
+        <v>21103</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" t="s">
+        <v>32</v>
+      </c>
+      <c r="E72">
+        <v>1024</v>
+      </c>
+      <c r="F72" s="17">
+        <v>43329</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" t="s">
+        <v>60</v>
+      </c>
+      <c r="D73" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73">
+        <v>8</v>
+      </c>
+      <c r="F73" s="17">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" t="s">
+        <v>60</v>
+      </c>
+      <c r="D74" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74">
+        <v>16</v>
+      </c>
+      <c r="F74" s="17">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>36</v>
+      </c>
+      <c r="C75" t="s">
+        <v>60</v>
+      </c>
+      <c r="D75" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75">
+        <v>32</v>
+      </c>
+      <c r="F75" s="17">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" t="s">
+        <v>60</v>
+      </c>
+      <c r="D76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76">
+        <v>64</v>
+      </c>
+      <c r="F76" s="17">
+        <v>5035</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77">
+        <v>128</v>
+      </c>
+      <c r="F77" s="17">
+        <v>12312</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78">
+        <v>256</v>
+      </c>
+      <c r="F78" s="17">
+        <v>27349</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79">
+        <v>512</v>
+      </c>
+      <c r="F79" s="17">
+        <v>63732</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>36</v>
+      </c>
+      <c r="C80" t="s">
+        <v>60</v>
+      </c>
+      <c r="D80" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80">
+        <v>1024</v>
+      </c>
+      <c r="F80" s="17">
+        <v>138469</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81" t="s">
+        <v>31</v>
+      </c>
+      <c r="E81">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" t="s">
+        <v>60</v>
+      </c>
+      <c r="D82" t="s">
+        <v>31</v>
+      </c>
+      <c r="E82">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83" t="s">
+        <v>31</v>
+      </c>
+      <c r="E83">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" t="s">
+        <v>60</v>
+      </c>
+      <c r="D84" t="s">
+        <v>31</v>
+      </c>
+      <c r="E84">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" t="s">
+        <v>60</v>
+      </c>
+      <c r="D85" t="s">
+        <v>31</v>
+      </c>
+      <c r="E85">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" t="s">
+        <v>60</v>
+      </c>
+      <c r="D86" t="s">
+        <v>31</v>
+      </c>
+      <c r="E86">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>64</v>
+      </c>
+      <c r="C87" t="s">
+        <v>60</v>
+      </c>
+      <c r="D87" t="s">
+        <v>32</v>
+      </c>
+      <c r="E87">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" t="s">
+        <v>60</v>
+      </c>
+      <c r="D88" t="s">
+        <v>32</v>
+      </c>
+      <c r="E88">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89" t="s">
+        <v>60</v>
+      </c>
+      <c r="D89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E89">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>64</v>
+      </c>
+      <c r="C90" t="s">
+        <v>60</v>
+      </c>
+      <c r="D90" t="s">
+        <v>32</v>
+      </c>
+      <c r="E90">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>64</v>
+      </c>
+      <c r="C91" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" t="s">
+        <v>32</v>
+      </c>
+      <c r="E91">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>64</v>
+      </c>
+      <c r="C92" t="s">
+        <v>60</v>
+      </c>
+      <c r="D92" t="s">
+        <v>32</v>
+      </c>
+      <c r="E92">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>64</v>
+      </c>
+      <c r="C93" t="s">
+        <v>60</v>
+      </c>
+      <c r="D93" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>64</v>
+      </c>
+      <c r="C94" t="s">
+        <v>60</v>
+      </c>
+      <c r="D94" t="s">
+        <v>22</v>
+      </c>
+      <c r="E94">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>64</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" t="s">
+        <v>60</v>
+      </c>
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>64</v>
+      </c>
+      <c r="C97" t="s">
+        <v>60</v>
+      </c>
+      <c r="D97" t="s">
+        <v>22</v>
+      </c>
+      <c r="E97">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>64</v>
+      </c>
+      <c r="C98" t="s">
+        <v>60</v>
+      </c>
+      <c r="D98" t="s">
+        <v>22</v>
+      </c>
+      <c r="E98">
+        <v>1024</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5445,12 +7041,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K10" sqref="K10:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5692,12 +7288,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="M10" sqref="M10:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6083,12 +7679,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G12:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6347,7 +7943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AS32"/>
   <sheetViews>
@@ -8228,122 +9824,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <v>32</v>
-      </c>
-      <c r="F5">
-        <v>4980.8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6">
-        <v>64</v>
-      </c>
-      <c r="F6">
-        <v>10102.4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7">
-        <v>32</v>
-      </c>
-      <c r="F7">
-        <v>12559.2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>32</v>
-      </c>
-      <c r="F8">
-        <v>6378</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>